<commit_message>
change size of canola stubble cat A to 1% to increase its quality. Redo grain_propn functin in stubble sim to make it easier to understand (same result)
</commit_message>
<xml_diff>
--- a/stubble sim.xlsx
+++ b/stubble sim.xlsx
@@ -774,10 +774,10 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1">
-        <v>0.7632431705833963</v>
+        <v>0.7632407081291448</v>
       </c>
       <c r="B1">
-        <v>0.01461359346040558</v>
+        <v>0.01461892953374144</v>
       </c>
       <c r="C1">
         <v>0</v>
@@ -788,58 +788,58 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2">
-        <v>0.1776586271990664</v>
+        <v>0.1776590689724449</v>
       </c>
       <c r="B2">
-        <v>0.7281681340483785</v>
+        <v>0.728158415035312</v>
       </c>
       <c r="C2">
-        <v>0.6955126932651354</v>
+        <v>0.6955074434115286</v>
       </c>
       <c r="D2">
-        <v>0.184988845145639</v>
+        <v>0.1849920720800949</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3">
-        <v>0</v>
+        <v>8.112697552874444E-18</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>3.317029860677889E-17</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>3.141128805256694E-17</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>8.00434827190673E-18</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4">
-        <v>0</v>
+        <v>5.729642221079343E-17</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>2.342726833367584E-16</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>2.218674835237584E-16</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>5.655993401404293E-17</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5">
-        <v>0.05909820221753723</v>
+        <v>0.05910022289841008</v>
       </c>
       <c r="B5">
-        <v>0.2572182724912158</v>
+        <v>0.2572226554309462</v>
       </c>
       <c r="C5">
-        <v>0.3044873067348645</v>
+        <v>0.3044925565884709</v>
       </c>
       <c r="D5">
-        <v>0.8150111548543609</v>
+        <v>0.815007927919905</v>
       </c>
     </row>
   </sheetData>
@@ -1023,10 +1023,10 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1">
-        <v>0.4271062341794111</v>
+        <v>0.7168348031366673</v>
       </c>
       <c r="B1">
-        <v>0</v>
+        <v>0.02978849117830595</v>
       </c>
       <c r="C1">
         <v>0</v>
@@ -1037,13 +1037,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2">
-        <v>0.5695200870426755</v>
+        <v>0.2823222605127404</v>
       </c>
       <c r="B2">
-        <v>0.9744378431396262</v>
+        <v>0.9665379169450865</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>0.3888902535642045</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1051,44 +1051,44 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3">
-        <v>7.869531232707829E-13</v>
+        <v>1.090492102067622E-06</v>
       </c>
       <c r="B3">
-        <v>5.955550572052952E-12</v>
+        <v>4.752492256304215E-06</v>
       </c>
       <c r="C3">
-        <v>1.771096990464771E-10</v>
+        <v>0.0007935567444627874</v>
       </c>
       <c r="D3">
-        <v>1.028671089127642E-11</v>
+        <v>0.001410268770281795</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4">
-        <v>0.00250788657463974</v>
+        <v>0.0001456984526927458</v>
       </c>
       <c r="B4">
-        <v>0.01899745592075483</v>
+        <v>0.0006349474845136278</v>
       </c>
       <c r="C4">
-        <v>0.6983594029114579</v>
+        <v>0.1037261208925042</v>
       </c>
       <c r="D4">
-        <v>0.1099537198267961</v>
+        <v>0.0983035723041345</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5">
-        <v>0.0008657922024865962</v>
+        <v>0.000696147405797672</v>
       </c>
       <c r="B5">
-        <v>0.006564700933663254</v>
+        <v>0.003033891899837479</v>
       </c>
       <c r="C5">
-        <v>0.3016405969114322</v>
+        <v>0.5065900687988284</v>
       </c>
       <c r="D5">
-        <v>0.8900462801629173</v>
+        <v>0.9002861589255836</v>
       </c>
     </row>
   </sheetData>
@@ -1106,10 +1106,10 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1">
-        <v>0.4271062341794111</v>
+        <v>0.7168348031366673</v>
       </c>
       <c r="B1">
-        <v>0</v>
+        <v>0.02978849117830595</v>
       </c>
       <c r="C1">
         <v>0</v>
@@ -1120,13 +1120,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2">
-        <v>0.5695200870426755</v>
+        <v>0.2823222605127404</v>
       </c>
       <c r="B2">
-        <v>0.9744378431396262</v>
+        <v>0.9665379169450865</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>0.3888902535642045</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1134,44 +1134,44 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3">
-        <v>7.869531232707829E-13</v>
+        <v>1.090492102067622E-06</v>
       </c>
       <c r="B3">
-        <v>5.955550572052952E-12</v>
+        <v>4.752492256304215E-06</v>
       </c>
       <c r="C3">
-        <v>1.771096990464771E-10</v>
+        <v>0.0007935567444627874</v>
       </c>
       <c r="D3">
-        <v>1.028671089127642E-11</v>
+        <v>0.001410268770281795</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4">
-        <v>0.00250788657463974</v>
+        <v>0.0001456984526927458</v>
       </c>
       <c r="B4">
-        <v>0.01899745592075483</v>
+        <v>0.0006349474845136278</v>
       </c>
       <c r="C4">
-        <v>0.6983594029114579</v>
+        <v>0.1037261208925042</v>
       </c>
       <c r="D4">
-        <v>0.1099537198267961</v>
+        <v>0.0983035723041345</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5">
-        <v>0.0008657922024865962</v>
+        <v>0.000696147405797672</v>
       </c>
       <c r="B5">
-        <v>0.006564700933663254</v>
+        <v>0.003033891899837479</v>
       </c>
       <c r="C5">
-        <v>0.3016405969114322</v>
+        <v>0.5065900687988284</v>
       </c>
       <c r="D5">
-        <v>0.8900462801629173</v>
+        <v>0.9002861589255836</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Make yield in stubble sim total grain (eg include spilt grain). And improve comment for harvest data.
</commit_message>
<xml_diff>
--- a/stubble sim.xlsx
+++ b/stubble sim.xlsx
@@ -348,532 +348,532 @@
   <sheetData>
     <row r="1" spans="1:17">
       <c r="A1">
-        <v>0.04096645837226049</v>
+        <v>0.03850847086992486</v>
       </c>
       <c r="B1">
-        <v>0.04096645837226049</v>
+        <v>0.03850847086992486</v>
       </c>
       <c r="C1">
-        <v>0.0442931700571384</v>
+        <v>0.04163557985371009</v>
       </c>
       <c r="D1">
-        <v>0.0442931700571384</v>
+        <v>0.04163557985371009</v>
       </c>
       <c r="E1">
-        <v>0.03784020239147139</v>
+        <v>0.0355697902479831</v>
       </c>
       <c r="F1">
-        <v>0.03784020239147139</v>
+        <v>0.0355697902479831</v>
       </c>
       <c r="G1">
         <v>0.03779284293916666</v>
       </c>
       <c r="H1">
-        <v>0.02361228629227815</v>
+        <v>0.022194926099272</v>
       </c>
       <c r="I1">
-        <v>0.03197531223700031</v>
+        <v>0.0310160528698903</v>
       </c>
       <c r="J1">
-        <v>0.03197531223700031</v>
+        <v>0.0310160528698903</v>
       </c>
       <c r="K1">
-        <v>0.03197531223700031</v>
+        <v>0.0310160528698903</v>
       </c>
       <c r="L1">
-        <v>0.03197531223700031</v>
+        <v>0.0310160528698903</v>
       </c>
       <c r="M1">
-        <v>0.04236509862414617</v>
+        <v>0.03812858876173155</v>
       </c>
       <c r="N1">
-        <v>0.04236509862414617</v>
+        <v>0.03812858876173155</v>
       </c>
       <c r="O1">
-        <v>0.04236509862414617</v>
+        <v>0.03812858876173155</v>
       </c>
       <c r="P1">
-        <v>0.04236509862414617</v>
+        <v>0.03812858876173155</v>
       </c>
       <c r="Q1">
-        <v>0.04236509862414617</v>
+        <v>0.03812858876173155</v>
       </c>
     </row>
     <row r="2" spans="1:17">
       <c r="A2">
-        <v>0.007282397191859693</v>
+        <v>0.006845453360348112</v>
       </c>
       <c r="B2">
-        <v>0.007282397191859693</v>
+        <v>0.006845453360348112</v>
       </c>
       <c r="C2">
-        <v>0.00787376966570005</v>
+        <v>0.007401343485758047</v>
       </c>
       <c r="D2">
-        <v>0.00787376966570005</v>
+        <v>0.007401343485758047</v>
       </c>
       <c r="E2">
-        <v>0.00672665870041741</v>
+        <v>0.006323059178392365</v>
       </c>
       <c r="F2">
-        <v>0.00672665870041741</v>
+        <v>0.006323059178392365</v>
       </c>
       <c r="G2">
         <v>0.006718239853483219</v>
       </c>
       <c r="H2">
-        <v>0.004197435029060463</v>
+        <v>0.003945478177052217</v>
       </c>
       <c r="I2">
-        <v>0.007894511271558234</v>
+        <v>0.007657675933411485</v>
       </c>
       <c r="J2">
-        <v>0.007894511271558234</v>
+        <v>0.007657675933411485</v>
       </c>
       <c r="K2">
-        <v>0.007894511271558234</v>
+        <v>0.007657675933411485</v>
       </c>
       <c r="L2">
-        <v>0.007894511271558234</v>
+        <v>0.007657675933411485</v>
       </c>
       <c r="M2">
-        <v>0.01045968671486455</v>
+        <v>0.009413718043378096</v>
       </c>
       <c r="N2">
-        <v>0.01045968671486455</v>
+        <v>0.009413718043378096</v>
       </c>
       <c r="O2">
-        <v>0.01045968671486455</v>
+        <v>0.009413718043378096</v>
       </c>
       <c r="P2">
-        <v>0.01045968671486455</v>
+        <v>0.009413718043378096</v>
       </c>
       <c r="Q2">
-        <v>0.01045968671486455</v>
+        <v>0.009413718043378096</v>
       </c>
     </row>
     <row r="3" spans="1:17">
       <c r="A3">
-        <v>0.00719956352314239</v>
+        <v>0.006767589711753846</v>
       </c>
       <c r="B3">
-        <v>0.00719956352314239</v>
+        <v>0.006767589711753846</v>
       </c>
       <c r="C3">
-        <v>0.007784209427379899</v>
+        <v>0.007317156861737104</v>
       </c>
       <c r="D3">
-        <v>0.007784209427379899</v>
+        <v>0.007317156861737104</v>
       </c>
       <c r="E3">
-        <v>0.006650146282365346</v>
+        <v>0.006251137505423425</v>
       </c>
       <c r="F3">
-        <v>0.006650146282365346</v>
+        <v>0.006251137505423425</v>
       </c>
       <c r="G3">
         <v>0.006641823195653999</v>
       </c>
       <c r="H3">
-        <v>0.004149691280195976</v>
+        <v>0.00390060031284912</v>
       </c>
       <c r="I3">
-        <v>0.009235426068180919</v>
+        <v>0.008958363286135491</v>
       </c>
       <c r="J3">
-        <v>0.009235426068180919</v>
+        <v>0.008958363286135491</v>
       </c>
       <c r="K3">
-        <v>0.009235426068180919</v>
+        <v>0.008958363286135491</v>
       </c>
       <c r="L3">
-        <v>0.009235426068180919</v>
+        <v>0.008958363286135491</v>
       </c>
       <c r="M3">
-        <v>0.01223630697691039</v>
+        <v>0.01101267627921935</v>
       </c>
       <c r="N3">
-        <v>0.01223630697691039</v>
+        <v>0.01101267627921935</v>
       </c>
       <c r="O3">
-        <v>0.01223630697691039</v>
+        <v>0.01101267627921935</v>
       </c>
       <c r="P3">
-        <v>0.01223630697691039</v>
+        <v>0.01101267627921935</v>
       </c>
       <c r="Q3">
-        <v>0.01223630697691039</v>
+        <v>0.01101267627921935</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="A4">
-        <v>0.007033896185707779</v>
+        <v>0.006611862414565312</v>
       </c>
       <c r="B4">
-        <v>0.007033896185707779</v>
+        <v>0.006611862414565312</v>
       </c>
       <c r="C4">
-        <v>0.007605088950739593</v>
+        <v>0.007148783613695218</v>
       </c>
       <c r="D4">
-        <v>0.007605088950739593</v>
+        <v>0.007148783613695218</v>
       </c>
       <c r="E4">
-        <v>0.006497121446261215</v>
+        <v>0.006107294159485542</v>
       </c>
       <c r="F4">
-        <v>0.006497121446261215</v>
+        <v>0.006107294159485542</v>
       </c>
       <c r="G4">
         <v>0.006488989879995556</v>
       </c>
       <c r="H4">
-        <v>0.004054203782466998</v>
+        <v>0.003810844584442924</v>
       </c>
       <c r="I4">
-        <v>0.006018134199081025</v>
+        <v>0.005837590173108594</v>
       </c>
       <c r="J4">
-        <v>0.006018134199081025</v>
+        <v>0.005837590173108594</v>
       </c>
       <c r="K4">
-        <v>0.006018134199081025</v>
+        <v>0.005837590173108594</v>
       </c>
       <c r="L4">
-        <v>0.006018134199081025</v>
+        <v>0.005837590173108594</v>
       </c>
       <c r="M4">
-        <v>0.007973615612809818</v>
+        <v>0.007176254051528836</v>
       </c>
       <c r="N4">
-        <v>0.007973615612809818</v>
+        <v>0.007176254051528836</v>
       </c>
       <c r="O4">
-        <v>0.007973615612809818</v>
+        <v>0.007176254051528836</v>
       </c>
       <c r="P4">
-        <v>0.007973615612809818</v>
+        <v>0.007176254051528836</v>
       </c>
       <c r="Q4">
-        <v>0.007973615612809818</v>
+        <v>0.007176254051528836</v>
       </c>
     </row>
     <row r="5" spans="1:17">
       <c r="A5">
-        <v>0.007033896185707779</v>
+        <v>0.006611862414565312</v>
       </c>
       <c r="B5">
-        <v>0.007033896185707779</v>
+        <v>0.006611862414565312</v>
       </c>
       <c r="C5">
-        <v>0.007605088950739593</v>
+        <v>0.007148783613695218</v>
       </c>
       <c r="D5">
-        <v>0.007605088950739593</v>
+        <v>0.007148783613695218</v>
       </c>
       <c r="E5">
-        <v>0.006497121446261215</v>
+        <v>0.006107294159485542</v>
       </c>
       <c r="F5">
-        <v>0.006497121446261215</v>
+        <v>0.006107294159485542</v>
       </c>
       <c r="G5">
         <v>0.006488989879995556</v>
       </c>
       <c r="H5">
-        <v>0.004054203782466998</v>
+        <v>0.003810844584442924</v>
       </c>
       <c r="I5">
-        <v>0.00743161875541942</v>
+        <v>0.007208670192756836</v>
       </c>
       <c r="J5">
-        <v>0.00743161875541942</v>
+        <v>0.007208670192756836</v>
       </c>
       <c r="K5">
-        <v>0.00743161875541942</v>
+        <v>0.007208670192756836</v>
       </c>
       <c r="L5">
-        <v>0.00743161875541942</v>
+        <v>0.007208670192756836</v>
       </c>
       <c r="M5">
-        <v>0.009846385835947482</v>
+        <v>0.008861747252352734</v>
       </c>
       <c r="N5">
-        <v>0.009846385835947482</v>
+        <v>0.008861747252352734</v>
       </c>
       <c r="O5">
-        <v>0.009846385835947482</v>
+        <v>0.008861747252352734</v>
       </c>
       <c r="P5">
-        <v>0.009846385835947482</v>
+        <v>0.008861747252352734</v>
       </c>
       <c r="Q5">
-        <v>0.009846385835947482</v>
+        <v>0.008861747252352734</v>
       </c>
     </row>
     <row r="6" spans="1:17">
       <c r="A6">
-        <v>0.004555769360293439</v>
+        <v>0.004282423198675833</v>
       </c>
       <c r="B6">
-        <v>0.004555769360293439</v>
+        <v>0.004282423198675833</v>
       </c>
       <c r="C6">
-        <v>0.004925723995541071</v>
+        <v>0.004630180555808607</v>
       </c>
       <c r="D6">
-        <v>0.004925723995541071</v>
+        <v>0.004630180555808607</v>
       </c>
       <c r="E6">
-        <v>0.004208106863323549</v>
+        <v>0.003955620451524137</v>
       </c>
       <c r="F6">
-        <v>0.004208106863323549</v>
+        <v>0.003955620451524137</v>
       </c>
       <c r="G6">
         <v>0.004202840146348175</v>
       </c>
       <c r="H6">
-        <v>0.002625858682713895</v>
+        <v>0.002468237877880805</v>
       </c>
       <c r="I6">
-        <v>0.004445313904236873</v>
+        <v>0.004311954487109766</v>
       </c>
       <c r="J6">
-        <v>0.004445313904236873</v>
+        <v>0.004311954487109766</v>
       </c>
       <c r="K6">
-        <v>0.004445313904236873</v>
+        <v>0.004311954487109766</v>
       </c>
       <c r="L6">
-        <v>0.004445313904236873</v>
+        <v>0.004311954487109766</v>
       </c>
       <c r="M6">
-        <v>0.005889736449558771</v>
+        <v>0.005300762804602894</v>
       </c>
       <c r="N6">
-        <v>0.005889736449558771</v>
+        <v>0.005300762804602894</v>
       </c>
       <c r="O6">
-        <v>0.005889736449558771</v>
+        <v>0.005300762804602894</v>
       </c>
       <c r="P6">
-        <v>0.005889736449558771</v>
+        <v>0.005300762804602894</v>
       </c>
       <c r="Q6">
-        <v>0.005889736449558771</v>
+        <v>0.005300762804602894</v>
       </c>
     </row>
     <row r="7" spans="1:17">
       <c r="A7">
-        <v>0.004555769360293439</v>
+        <v>0.004282423198675833</v>
       </c>
       <c r="B7">
-        <v>0.004555769360293439</v>
+        <v>0.004282423198675833</v>
       </c>
       <c r="C7">
-        <v>0.004925723995541071</v>
+        <v>0.004630180555808607</v>
       </c>
       <c r="D7">
-        <v>0.004925723995541071</v>
+        <v>0.004630180555808607</v>
       </c>
       <c r="E7">
-        <v>0.004208106863323549</v>
+        <v>0.003955620451524137</v>
       </c>
       <c r="F7">
-        <v>0.004208106863323549</v>
+        <v>0.003955620451524137</v>
       </c>
       <c r="G7">
         <v>0.004202840146348175</v>
       </c>
       <c r="H7">
-        <v>0.002625858682713895</v>
+        <v>0.002468237877880805</v>
       </c>
       <c r="I7">
-        <v>0.004370603400884284</v>
+        <v>0.004239485298857755</v>
       </c>
       <c r="J7">
-        <v>0.004370603400884284</v>
+        <v>0.004239485298857755</v>
       </c>
       <c r="K7">
-        <v>0.004370603400884284</v>
+        <v>0.004239485298857755</v>
       </c>
       <c r="L7">
-        <v>0.004370603400884284</v>
+        <v>0.004239485298857755</v>
       </c>
       <c r="M7">
-        <v>0.005790750149774354</v>
+        <v>0.005211675134796919</v>
       </c>
       <c r="N7">
-        <v>0.005790750149774354</v>
+        <v>0.005211675134796919</v>
       </c>
       <c r="O7">
-        <v>0.005790750149774354</v>
+        <v>0.005211675134796919</v>
       </c>
       <c r="P7">
-        <v>0.005790750149774354</v>
+        <v>0.005211675134796919</v>
       </c>
       <c r="Q7">
-        <v>0.005790750149774354</v>
+        <v>0.005211675134796919</v>
       </c>
     </row>
     <row r="8" spans="1:17">
       <c r="A8">
-        <v>0.00227788468014672</v>
+        <v>0.002141211599337917</v>
       </c>
       <c r="B8">
-        <v>0.00227788468014672</v>
+        <v>0.002141211599337917</v>
       </c>
       <c r="C8">
-        <v>0.002462861997770536</v>
+        <v>0.002315090277904303</v>
       </c>
       <c r="D8">
-        <v>0.002462861997770536</v>
+        <v>0.002315090277904303</v>
       </c>
       <c r="E8">
-        <v>0.002104053431661775</v>
+        <v>0.001977810225762068</v>
       </c>
       <c r="F8">
-        <v>0.002104053431661775</v>
+        <v>0.001977810225762068</v>
       </c>
       <c r="G8">
         <v>0.002101420073174088</v>
       </c>
       <c r="H8">
-        <v>0.001312929341356947</v>
+        <v>0.001234118938940402</v>
       </c>
       <c r="I8">
-        <v>0.002913735600589522</v>
+        <v>0.002826323532571836</v>
       </c>
       <c r="J8">
-        <v>0.002913735600589522</v>
+        <v>0.002826323532571836</v>
       </c>
       <c r="K8">
-        <v>0.002913735600589522</v>
+        <v>0.002826323532571836</v>
       </c>
       <c r="L8">
-        <v>0.002913735600589522</v>
+        <v>0.002826323532571836</v>
       </c>
       <c r="M8">
-        <v>0.00386050009984957</v>
+        <v>0.003474450089864613</v>
       </c>
       <c r="N8">
-        <v>0.00386050009984957</v>
+        <v>0.003474450089864613</v>
       </c>
       <c r="O8">
-        <v>0.00386050009984957</v>
+        <v>0.003474450089864613</v>
       </c>
       <c r="P8">
-        <v>0.00386050009984957</v>
+        <v>0.003474450089864613</v>
       </c>
       <c r="Q8">
-        <v>0.00386050009984957</v>
+        <v>0.003474450089864613</v>
       </c>
     </row>
     <row r="9" spans="1:17">
       <c r="A9">
-        <v>0.00227788468014672</v>
+        <v>0.002141211599337917</v>
       </c>
       <c r="B9">
-        <v>0.00227788468014672</v>
+        <v>0.002141211599337917</v>
       </c>
       <c r="C9">
-        <v>0.002462861997770536</v>
+        <v>0.002315090277904303</v>
       </c>
       <c r="D9">
-        <v>0.002462861997770536</v>
+        <v>0.002315090277904303</v>
       </c>
       <c r="E9">
-        <v>0.002104053431661775</v>
+        <v>0.001977810225762068</v>
       </c>
       <c r="F9">
-        <v>0.002104053431661775</v>
+        <v>0.001977810225762068</v>
       </c>
       <c r="G9">
         <v>0.002101420073174088</v>
       </c>
       <c r="H9">
-        <v>0.001312929341356947</v>
+        <v>0.001234118938940402</v>
       </c>
       <c r="I9">
-        <v>0.001456867800294761</v>
+        <v>0.001413161766285918</v>
       </c>
       <c r="J9">
-        <v>0.001456867800294761</v>
+        <v>0.001413161766285918</v>
       </c>
       <c r="K9">
-        <v>0.001456867800294761</v>
+        <v>0.001413161766285918</v>
       </c>
       <c r="L9">
-        <v>0.001456867800294761</v>
+        <v>0.001413161766285918</v>
       </c>
       <c r="M9">
-        <v>0.001930250049924785</v>
+        <v>0.001737225044932306</v>
       </c>
       <c r="N9">
-        <v>0.001930250049924785</v>
+        <v>0.001737225044932306</v>
       </c>
       <c r="O9">
-        <v>0.001930250049924785</v>
+        <v>0.001737225044932306</v>
       </c>
       <c r="P9">
-        <v>0.001930250049924785</v>
+        <v>0.001737225044932306</v>
       </c>
       <c r="Q9">
-        <v>0.001930250049924785</v>
+        <v>0.001737225044932306</v>
       </c>
     </row>
     <row r="10" spans="1:17">
       <c r="A10">
-        <v>0.06494816078782628</v>
+        <v>0.0610512711405567</v>
       </c>
       <c r="B10">
-        <v>0.06494816078782628</v>
+        <v>0.0610512711405567</v>
       </c>
       <c r="C10">
-        <v>0.07022232443265072</v>
+        <v>0.06600898496669168</v>
       </c>
       <c r="D10">
-        <v>0.07022232443265072</v>
+        <v>0.06600898496669168</v>
       </c>
       <c r="E10">
-        <v>0.05999179931134381</v>
+        <v>0.05639229135266317</v>
       </c>
       <c r="F10">
-        <v>0.05999179931134381</v>
+        <v>0.05639229135266317</v>
       </c>
       <c r="G10">
         <v>0.05991671570770007</v>
       </c>
       <c r="H10">
-        <v>0.03743488277027854</v>
+        <v>0.03518780207628425</v>
       </c>
       <c r="I10">
-        <v>0.02101439595319382</v>
+        <v>0.02038396407459801</v>
       </c>
       <c r="J10">
-        <v>0.02101439595319382</v>
+        <v>0.02038396407459801</v>
       </c>
       <c r="K10">
-        <v>0.02101439595319382</v>
+        <v>0.02038396407459801</v>
       </c>
       <c r="L10">
-        <v>0.02101439595319382</v>
+        <v>0.02038396407459801</v>
       </c>
       <c r="M10">
-        <v>0.02784263529579324</v>
+        <v>0.02505837176621392</v>
       </c>
       <c r="N10">
-        <v>0.02784263529579324</v>
+        <v>0.02505837176621392</v>
       </c>
       <c r="O10">
-        <v>0.02784263529579324</v>
+        <v>0.02505837176621392</v>
       </c>
       <c r="P10">
-        <v>0.02784263529579324</v>
+        <v>0.02505837176621392</v>
       </c>
       <c r="Q10">
-        <v>0.02784263529579324</v>
+        <v>0.02505837176621392</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Make k axis consistent across modules and inputs. Add harv speed for h&of to stop nan (this altereted profit a little because it changed harvest dep)
</commit_message>
<xml_diff>
--- a/stubble sim.xlsx
+++ b/stubble sim.xlsx
@@ -348,34 +348,34 @@
   <sheetData>
     <row r="1" spans="1:17">
       <c r="A1">
-        <v>0.03850847086992486</v>
+        <v>0.04163557985371009</v>
       </c>
       <c r="B1">
-        <v>0.03850847086992486</v>
+        <v>0.04163557985371009</v>
       </c>
       <c r="C1">
-        <v>0.04163557985371009</v>
+        <v>0.03812858876173155</v>
       </c>
       <c r="D1">
-        <v>0.04163557985371009</v>
+        <v>0.03779284293916666</v>
       </c>
       <c r="E1">
+        <v>0.03812858876173155</v>
+      </c>
+      <c r="F1">
+        <v>0.03812858876173155</v>
+      </c>
+      <c r="G1">
+        <v>0.03812858876173155</v>
+      </c>
+      <c r="H1">
         <v>0.0355697902479831</v>
       </c>
-      <c r="F1">
+      <c r="I1">
         <v>0.0355697902479831</v>
       </c>
-      <c r="G1">
-        <v>0.03779284293916666</v>
-      </c>
-      <c r="H1">
+      <c r="J1">
         <v>0.022194926099272</v>
-      </c>
-      <c r="I1">
-        <v>0.0310160528698903</v>
-      </c>
-      <c r="J1">
-        <v>0.0310160528698903</v>
       </c>
       <c r="K1">
         <v>0.0310160528698903</v>
@@ -387,48 +387,48 @@
         <v>0.03812858876173155</v>
       </c>
       <c r="N1">
-        <v>0.03812858876173155</v>
+        <v>0.03850847086992486</v>
       </c>
       <c r="O1">
-        <v>0.03812858876173155</v>
+        <v>0.03850847086992486</v>
       </c>
       <c r="P1">
-        <v>0.03812858876173155</v>
+        <v>0.0310160528698903</v>
       </c>
       <c r="Q1">
-        <v>0.03812858876173155</v>
+        <v>0.0310160528698903</v>
       </c>
     </row>
     <row r="2" spans="1:17">
       <c r="A2">
-        <v>0.006845453360348112</v>
+        <v>0.007401343485758047</v>
       </c>
       <c r="B2">
-        <v>0.006845453360348112</v>
+        <v>0.007401343485758047</v>
       </c>
       <c r="C2">
-        <v>0.007401343485758047</v>
+        <v>0.009413718043378096</v>
       </c>
       <c r="D2">
-        <v>0.007401343485758047</v>
+        <v>0.006718239853483219</v>
       </c>
       <c r="E2">
+        <v>0.009413718043378096</v>
+      </c>
+      <c r="F2">
+        <v>0.009413718043378096</v>
+      </c>
+      <c r="G2">
+        <v>0.009413718043378096</v>
+      </c>
+      <c r="H2">
         <v>0.006323059178392365</v>
       </c>
-      <c r="F2">
+      <c r="I2">
         <v>0.006323059178392365</v>
       </c>
-      <c r="G2">
-        <v>0.006718239853483219</v>
-      </c>
-      <c r="H2">
+      <c r="J2">
         <v>0.003945478177052217</v>
-      </c>
-      <c r="I2">
-        <v>0.007657675933411485</v>
-      </c>
-      <c r="J2">
-        <v>0.007657675933411485</v>
       </c>
       <c r="K2">
         <v>0.007657675933411485</v>
@@ -440,48 +440,48 @@
         <v>0.009413718043378096</v>
       </c>
       <c r="N2">
-        <v>0.009413718043378096</v>
+        <v>0.006845453360348112</v>
       </c>
       <c r="O2">
-        <v>0.009413718043378096</v>
+        <v>0.006845453360348112</v>
       </c>
       <c r="P2">
-        <v>0.009413718043378096</v>
+        <v>0.007657675933411485</v>
       </c>
       <c r="Q2">
-        <v>0.009413718043378096</v>
+        <v>0.007657675933411485</v>
       </c>
     </row>
     <row r="3" spans="1:17">
       <c r="A3">
-        <v>0.006767589711753846</v>
+        <v>0.007317156861737104</v>
       </c>
       <c r="B3">
-        <v>0.006767589711753846</v>
+        <v>0.007317156861737104</v>
       </c>
       <c r="C3">
-        <v>0.007317156861737104</v>
+        <v>0.01101267627921935</v>
       </c>
       <c r="D3">
-        <v>0.007317156861737104</v>
+        <v>0.006641823195653999</v>
       </c>
       <c r="E3">
+        <v>0.01101267627921935</v>
+      </c>
+      <c r="F3">
+        <v>0.01101267627921935</v>
+      </c>
+      <c r="G3">
+        <v>0.01101267627921935</v>
+      </c>
+      <c r="H3">
         <v>0.006251137505423425</v>
       </c>
-      <c r="F3">
+      <c r="I3">
         <v>0.006251137505423425</v>
       </c>
-      <c r="G3">
-        <v>0.006641823195653999</v>
-      </c>
-      <c r="H3">
+      <c r="J3">
         <v>0.00390060031284912</v>
-      </c>
-      <c r="I3">
-        <v>0.008958363286135491</v>
-      </c>
-      <c r="J3">
-        <v>0.008958363286135491</v>
       </c>
       <c r="K3">
         <v>0.008958363286135491</v>
@@ -493,48 +493,48 @@
         <v>0.01101267627921935</v>
       </c>
       <c r="N3">
-        <v>0.01101267627921935</v>
+        <v>0.006767589711753846</v>
       </c>
       <c r="O3">
-        <v>0.01101267627921935</v>
+        <v>0.006767589711753846</v>
       </c>
       <c r="P3">
-        <v>0.01101267627921935</v>
+        <v>0.008958363286135491</v>
       </c>
       <c r="Q3">
-        <v>0.01101267627921935</v>
+        <v>0.008958363286135491</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="A4">
-        <v>0.006611862414565312</v>
+        <v>0.007148783613695218</v>
       </c>
       <c r="B4">
-        <v>0.006611862414565312</v>
+        <v>0.007148783613695218</v>
       </c>
       <c r="C4">
-        <v>0.007148783613695218</v>
+        <v>0.007176254051528836</v>
       </c>
       <c r="D4">
-        <v>0.007148783613695218</v>
+        <v>0.006488989879995556</v>
       </c>
       <c r="E4">
+        <v>0.007176254051528836</v>
+      </c>
+      <c r="F4">
+        <v>0.007176254051528836</v>
+      </c>
+      <c r="G4">
+        <v>0.007176254051528836</v>
+      </c>
+      <c r="H4">
         <v>0.006107294159485542</v>
       </c>
-      <c r="F4">
+      <c r="I4">
         <v>0.006107294159485542</v>
       </c>
-      <c r="G4">
-        <v>0.006488989879995556</v>
-      </c>
-      <c r="H4">
+      <c r="J4">
         <v>0.003810844584442924</v>
-      </c>
-      <c r="I4">
-        <v>0.005837590173108594</v>
-      </c>
-      <c r="J4">
-        <v>0.005837590173108594</v>
       </c>
       <c r="K4">
         <v>0.005837590173108594</v>
@@ -546,48 +546,48 @@
         <v>0.007176254051528836</v>
       </c>
       <c r="N4">
-        <v>0.007176254051528836</v>
+        <v>0.006611862414565312</v>
       </c>
       <c r="O4">
-        <v>0.007176254051528836</v>
+        <v>0.006611862414565312</v>
       </c>
       <c r="P4">
-        <v>0.007176254051528836</v>
+        <v>0.005837590173108594</v>
       </c>
       <c r="Q4">
-        <v>0.007176254051528836</v>
+        <v>0.005837590173108594</v>
       </c>
     </row>
     <row r="5" spans="1:17">
       <c r="A5">
-        <v>0.006611862414565312</v>
+        <v>0.007148783613695218</v>
       </c>
       <c r="B5">
-        <v>0.006611862414565312</v>
+        <v>0.007148783613695218</v>
       </c>
       <c r="C5">
-        <v>0.007148783613695218</v>
+        <v>0.008861747252352734</v>
       </c>
       <c r="D5">
-        <v>0.007148783613695218</v>
+        <v>0.006488989879995556</v>
       </c>
       <c r="E5">
+        <v>0.008861747252352734</v>
+      </c>
+      <c r="F5">
+        <v>0.008861747252352734</v>
+      </c>
+      <c r="G5">
+        <v>0.008861747252352734</v>
+      </c>
+      <c r="H5">
         <v>0.006107294159485542</v>
       </c>
-      <c r="F5">
+      <c r="I5">
         <v>0.006107294159485542</v>
       </c>
-      <c r="G5">
-        <v>0.006488989879995556</v>
-      </c>
-      <c r="H5">
+      <c r="J5">
         <v>0.003810844584442924</v>
-      </c>
-      <c r="I5">
-        <v>0.007208670192756836</v>
-      </c>
-      <c r="J5">
-        <v>0.007208670192756836</v>
       </c>
       <c r="K5">
         <v>0.007208670192756836</v>
@@ -599,48 +599,48 @@
         <v>0.008861747252352734</v>
       </c>
       <c r="N5">
-        <v>0.008861747252352734</v>
+        <v>0.006611862414565312</v>
       </c>
       <c r="O5">
-        <v>0.008861747252352734</v>
+        <v>0.006611862414565312</v>
       </c>
       <c r="P5">
-        <v>0.008861747252352734</v>
+        <v>0.007208670192756836</v>
       </c>
       <c r="Q5">
-        <v>0.008861747252352734</v>
+        <v>0.007208670192756836</v>
       </c>
     </row>
     <row r="6" spans="1:17">
       <c r="A6">
-        <v>0.004282423198675833</v>
+        <v>0.004630180555808607</v>
       </c>
       <c r="B6">
-        <v>0.004282423198675833</v>
+        <v>0.004630180555808607</v>
       </c>
       <c r="C6">
-        <v>0.004630180555808607</v>
+        <v>0.005300762804602894</v>
       </c>
       <c r="D6">
-        <v>0.004630180555808607</v>
+        <v>0.004202840146348175</v>
       </c>
       <c r="E6">
+        <v>0.005300762804602894</v>
+      </c>
+      <c r="F6">
+        <v>0.005300762804602894</v>
+      </c>
+      <c r="G6">
+        <v>0.005300762804602894</v>
+      </c>
+      <c r="H6">
         <v>0.003955620451524137</v>
       </c>
-      <c r="F6">
+      <c r="I6">
         <v>0.003955620451524137</v>
       </c>
-      <c r="G6">
-        <v>0.004202840146348175</v>
-      </c>
-      <c r="H6">
+      <c r="J6">
         <v>0.002468237877880805</v>
-      </c>
-      <c r="I6">
-        <v>0.004311954487109766</v>
-      </c>
-      <c r="J6">
-        <v>0.004311954487109766</v>
       </c>
       <c r="K6">
         <v>0.004311954487109766</v>
@@ -652,48 +652,48 @@
         <v>0.005300762804602894</v>
       </c>
       <c r="N6">
-        <v>0.005300762804602894</v>
+        <v>0.004282423198675833</v>
       </c>
       <c r="O6">
-        <v>0.005300762804602894</v>
+        <v>0.004282423198675833</v>
       </c>
       <c r="P6">
-        <v>0.005300762804602894</v>
+        <v>0.004311954487109766</v>
       </c>
       <c r="Q6">
-        <v>0.005300762804602894</v>
+        <v>0.004311954487109766</v>
       </c>
     </row>
     <row r="7" spans="1:17">
       <c r="A7">
-        <v>0.004282423198675833</v>
+        <v>0.004630180555808607</v>
       </c>
       <c r="B7">
-        <v>0.004282423198675833</v>
+        <v>0.004630180555808607</v>
       </c>
       <c r="C7">
-        <v>0.004630180555808607</v>
+        <v>0.005211675134796919</v>
       </c>
       <c r="D7">
-        <v>0.004630180555808607</v>
+        <v>0.004202840146348175</v>
       </c>
       <c r="E7">
+        <v>0.005211675134796919</v>
+      </c>
+      <c r="F7">
+        <v>0.005211675134796919</v>
+      </c>
+      <c r="G7">
+        <v>0.005211675134796919</v>
+      </c>
+      <c r="H7">
         <v>0.003955620451524137</v>
       </c>
-      <c r="F7">
+      <c r="I7">
         <v>0.003955620451524137</v>
       </c>
-      <c r="G7">
-        <v>0.004202840146348175</v>
-      </c>
-      <c r="H7">
+      <c r="J7">
         <v>0.002468237877880805</v>
-      </c>
-      <c r="I7">
-        <v>0.004239485298857755</v>
-      </c>
-      <c r="J7">
-        <v>0.004239485298857755</v>
       </c>
       <c r="K7">
         <v>0.004239485298857755</v>
@@ -705,48 +705,48 @@
         <v>0.005211675134796919</v>
       </c>
       <c r="N7">
-        <v>0.005211675134796919</v>
+        <v>0.004282423198675833</v>
       </c>
       <c r="O7">
-        <v>0.005211675134796919</v>
+        <v>0.004282423198675833</v>
       </c>
       <c r="P7">
-        <v>0.005211675134796919</v>
+        <v>0.004239485298857755</v>
       </c>
       <c r="Q7">
-        <v>0.005211675134796919</v>
+        <v>0.004239485298857755</v>
       </c>
     </row>
     <row r="8" spans="1:17">
       <c r="A8">
-        <v>0.002141211599337917</v>
+        <v>0.002315090277904303</v>
       </c>
       <c r="B8">
-        <v>0.002141211599337917</v>
+        <v>0.002315090277904303</v>
       </c>
       <c r="C8">
-        <v>0.002315090277904303</v>
+        <v>0.003474450089864613</v>
       </c>
       <c r="D8">
-        <v>0.002315090277904303</v>
+        <v>0.002101420073174088</v>
       </c>
       <c r="E8">
+        <v>0.003474450089864613</v>
+      </c>
+      <c r="F8">
+        <v>0.003474450089864613</v>
+      </c>
+      <c r="G8">
+        <v>0.003474450089864613</v>
+      </c>
+      <c r="H8">
         <v>0.001977810225762068</v>
       </c>
-      <c r="F8">
+      <c r="I8">
         <v>0.001977810225762068</v>
       </c>
-      <c r="G8">
-        <v>0.002101420073174088</v>
-      </c>
-      <c r="H8">
+      <c r="J8">
         <v>0.001234118938940402</v>
-      </c>
-      <c r="I8">
-        <v>0.002826323532571836</v>
-      </c>
-      <c r="J8">
-        <v>0.002826323532571836</v>
       </c>
       <c r="K8">
         <v>0.002826323532571836</v>
@@ -758,48 +758,48 @@
         <v>0.003474450089864613</v>
       </c>
       <c r="N8">
-        <v>0.003474450089864613</v>
+        <v>0.002141211599337917</v>
       </c>
       <c r="O8">
-        <v>0.003474450089864613</v>
+        <v>0.002141211599337917</v>
       </c>
       <c r="P8">
-        <v>0.003474450089864613</v>
+        <v>0.002826323532571836</v>
       </c>
       <c r="Q8">
-        <v>0.003474450089864613</v>
+        <v>0.002826323532571836</v>
       </c>
     </row>
     <row r="9" spans="1:17">
       <c r="A9">
-        <v>0.002141211599337917</v>
+        <v>0.002315090277904303</v>
       </c>
       <c r="B9">
-        <v>0.002141211599337917</v>
+        <v>0.002315090277904303</v>
       </c>
       <c r="C9">
-        <v>0.002315090277904303</v>
+        <v>0.001737225044932306</v>
       </c>
       <c r="D9">
-        <v>0.002315090277904303</v>
+        <v>0.002101420073174088</v>
       </c>
       <c r="E9">
+        <v>0.001737225044932306</v>
+      </c>
+      <c r="F9">
+        <v>0.001737225044932306</v>
+      </c>
+      <c r="G9">
+        <v>0.001737225044932306</v>
+      </c>
+      <c r="H9">
         <v>0.001977810225762068</v>
       </c>
-      <c r="F9">
+      <c r="I9">
         <v>0.001977810225762068</v>
       </c>
-      <c r="G9">
-        <v>0.002101420073174088</v>
-      </c>
-      <c r="H9">
+      <c r="J9">
         <v>0.001234118938940402</v>
-      </c>
-      <c r="I9">
-        <v>0.001413161766285918</v>
-      </c>
-      <c r="J9">
-        <v>0.001413161766285918</v>
       </c>
       <c r="K9">
         <v>0.001413161766285918</v>
@@ -811,48 +811,48 @@
         <v>0.001737225044932306</v>
       </c>
       <c r="N9">
-        <v>0.001737225044932306</v>
+        <v>0.002141211599337917</v>
       </c>
       <c r="O9">
-        <v>0.001737225044932306</v>
+        <v>0.002141211599337917</v>
       </c>
       <c r="P9">
-        <v>0.001737225044932306</v>
+        <v>0.001413161766285918</v>
       </c>
       <c r="Q9">
-        <v>0.001737225044932306</v>
+        <v>0.001413161766285918</v>
       </c>
     </row>
     <row r="10" spans="1:17">
       <c r="A10">
-        <v>0.0610512711405567</v>
+        <v>0.06600898496669168</v>
       </c>
       <c r="B10">
-        <v>0.0610512711405567</v>
+        <v>0.06600898496669168</v>
       </c>
       <c r="C10">
-        <v>0.06600898496669168</v>
+        <v>0.02505837176621392</v>
       </c>
       <c r="D10">
-        <v>0.06600898496669168</v>
+        <v>0.05991671570770007</v>
       </c>
       <c r="E10">
+        <v>0.02505837176621392</v>
+      </c>
+      <c r="F10">
+        <v>0.02505837176621392</v>
+      </c>
+      <c r="G10">
+        <v>0.02505837176621392</v>
+      </c>
+      <c r="H10">
         <v>0.05639229135266317</v>
       </c>
-      <c r="F10">
+      <c r="I10">
         <v>0.05639229135266317</v>
       </c>
-      <c r="G10">
-        <v>0.05991671570770007</v>
-      </c>
-      <c r="H10">
+      <c r="J10">
         <v>0.03518780207628425</v>
-      </c>
-      <c r="I10">
-        <v>0.02038396407459801</v>
-      </c>
-      <c r="J10">
-        <v>0.02038396407459801</v>
       </c>
       <c r="K10">
         <v>0.02038396407459801</v>
@@ -864,16 +864,16 @@
         <v>0.02505837176621392</v>
       </c>
       <c r="N10">
-        <v>0.02505837176621392</v>
+        <v>0.0610512711405567</v>
       </c>
       <c r="O10">
-        <v>0.02505837176621392</v>
+        <v>0.0610512711405567</v>
       </c>
       <c r="P10">
-        <v>0.02505837176621392</v>
+        <v>0.02038396407459801</v>
       </c>
       <c r="Q10">
-        <v>0.02505837176621392</v>
+        <v>0.02038396407459801</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add s2 to stub
</commit_message>
<xml_diff>
--- a/stubble sim.xlsx
+++ b/stubble sim.xlsx
@@ -340,540 +340,1560 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q10"/>
+  <dimension ref="A1:AY10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:51">
       <c r="A1">
         <v>0.04163557985371009</v>
       </c>
       <c r="B1">
+        <v>0.0244151040262156</v>
+      </c>
+      <c r="C1">
+        <v>0.05194702984301191</v>
+      </c>
+      <c r="D1">
         <v>0.04163557985371009</v>
       </c>
-      <c r="C1">
-        <v>0.03812858876173155</v>
-      </c>
-      <c r="D1">
-        <v>0.03779284293916666</v>
-      </c>
       <c r="E1">
-        <v>0.03812858876173155</v>
+        <v>0.0244151040262156</v>
       </c>
       <c r="F1">
-        <v>0.03812858876173155</v>
+        <v>0.05194702984301191</v>
       </c>
       <c r="G1">
         <v>0.03812858876173155</v>
       </c>
       <c r="H1">
-        <v>0.0355697902479831</v>
+        <v>0.02783386979606403</v>
       </c>
       <c r="I1">
-        <v>0.0355697902479831</v>
+        <v>0.05922099956609368</v>
       </c>
       <c r="J1">
-        <v>0.022194926099272</v>
+        <v>0.00636146938450756</v>
       </c>
       <c r="K1">
-        <v>0.0310160528698903</v>
+        <v>0.004567535018076429</v>
       </c>
       <c r="L1">
-        <v>0.0310160528698903</v>
+        <v>0.00971815961292857</v>
       </c>
       <c r="M1">
         <v>0.03812858876173155</v>
       </c>
       <c r="N1">
+        <v>0.02783386979606403</v>
+      </c>
+      <c r="O1">
+        <v>0.05922099956609368</v>
+      </c>
+      <c r="P1">
+        <v>0.03812858876173155</v>
+      </c>
+      <c r="Q1">
+        <v>0.02783386979606403</v>
+      </c>
+      <c r="R1">
+        <v>0.05922099956609368</v>
+      </c>
+      <c r="S1">
+        <v>0.03812858876173155</v>
+      </c>
+      <c r="T1">
+        <v>0.02783386979606403</v>
+      </c>
+      <c r="U1">
+        <v>0.05922099956609368</v>
+      </c>
+      <c r="V1">
+        <v>0.0355697902479831</v>
+      </c>
+      <c r="W1">
+        <v>0.02219554911474146</v>
+      </c>
+      <c r="X1">
+        <v>0.04722457258455628</v>
+      </c>
+      <c r="Y1">
+        <v>0.0355697902479831</v>
+      </c>
+      <c r="Z1">
+        <v>0.02219554911474146</v>
+      </c>
+      <c r="AA1">
+        <v>0.04722457258455628</v>
+      </c>
+      <c r="AB1">
+        <v>0.03556879182575642</v>
+      </c>
+      <c r="AC1">
+        <v>0.022194926099272</v>
+      </c>
+      <c r="AD1">
+        <v>0.04722324701972765</v>
+      </c>
+      <c r="AE1">
+        <v>0.03101605286989031</v>
+      </c>
+      <c r="AF1">
+        <v>0.02499893861313159</v>
+      </c>
+      <c r="AG1">
+        <v>0.05318923109176933</v>
+      </c>
+      <c r="AH1">
+        <v>0.03101605286989031</v>
+      </c>
+      <c r="AI1">
+        <v>0.02499893861313159</v>
+      </c>
+      <c r="AJ1">
+        <v>0.05318923109176933</v>
+      </c>
+      <c r="AK1">
+        <v>0.03812858876173155</v>
+      </c>
+      <c r="AL1">
+        <v>0.02783386979606403</v>
+      </c>
+      <c r="AM1">
+        <v>0.05922099956609368</v>
+      </c>
+      <c r="AN1">
         <v>0.03850847086992486</v>
       </c>
-      <c r="O1">
+      <c r="AO1">
+        <v>0.02330532657047853</v>
+      </c>
+      <c r="AP1">
+        <v>0.04958580121378409</v>
+      </c>
+      <c r="AQ1">
         <v>0.03850847086992486</v>
       </c>
-      <c r="P1">
-        <v>0.0310160528698903</v>
-      </c>
-      <c r="Q1">
-        <v>0.0310160528698903</v>
+      <c r="AR1">
+        <v>0.02330532657047853</v>
+      </c>
+      <c r="AS1">
+        <v>0.04958580121378409</v>
+      </c>
+      <c r="AT1">
+        <v>0.03101605286989031</v>
+      </c>
+      <c r="AU1">
+        <v>0.02499893861313159</v>
+      </c>
+      <c r="AV1">
+        <v>0.05318923109176933</v>
+      </c>
+      <c r="AW1">
+        <v>0.03101605286989031</v>
+      </c>
+      <c r="AX1">
+        <v>0.02499893861313159</v>
+      </c>
+      <c r="AY1">
+        <v>0.05318923109176933</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:51">
       <c r="A2">
-        <v>0.007401343485758047</v>
+        <v>0.007401343485758048</v>
       </c>
       <c r="B2">
-        <v>0.007401343485758047</v>
+        <v>0.004340147820048519</v>
       </c>
       <c r="C2">
-        <v>0.009413718043378096</v>
+        <v>0.009234357063933019</v>
       </c>
       <c r="D2">
-        <v>0.006718239853483219</v>
+        <v>0.007401343485758048</v>
       </c>
       <c r="E2">
-        <v>0.009413718043378096</v>
+        <v>0.004340147820048519</v>
       </c>
       <c r="F2">
-        <v>0.009413718043378096</v>
+        <v>0.009234357063933019</v>
       </c>
       <c r="G2">
         <v>0.009413718043378096</v>
       </c>
       <c r="H2">
-        <v>0.006323059178392365</v>
+        <v>0.00687201417166601</v>
       </c>
       <c r="I2">
-        <v>0.006323059178392365</v>
+        <v>0.01462130674822555</v>
       </c>
       <c r="J2">
-        <v>0.003945478177052217</v>
+        <v>0.001130845785126702</v>
       </c>
       <c r="K2">
-        <v>0.007657675933411485</v>
+        <v>0.000811947273720972</v>
       </c>
       <c r="L2">
-        <v>0.007657675933411485</v>
+        <v>0.001727547390895685</v>
       </c>
       <c r="M2">
         <v>0.009413718043378096</v>
       </c>
       <c r="N2">
+        <v>0.00687201417166601</v>
+      </c>
+      <c r="O2">
+        <v>0.01462130674822555</v>
+      </c>
+      <c r="P2">
+        <v>0.009413718043378096</v>
+      </c>
+      <c r="Q2">
+        <v>0.00687201417166601</v>
+      </c>
+      <c r="R2">
+        <v>0.01462130674822555</v>
+      </c>
+      <c r="S2">
+        <v>0.009413718043378096</v>
+      </c>
+      <c r="T2">
+        <v>0.00687201417166601</v>
+      </c>
+      <c r="U2">
+        <v>0.01462130674822555</v>
+      </c>
+      <c r="V2">
+        <v>0.006323059178392366</v>
+      </c>
+      <c r="W2">
+        <v>0.003945588927316836</v>
+      </c>
+      <c r="X2">
+        <v>0.008394870058120927</v>
+      </c>
+      <c r="Y2">
+        <v>0.006323059178392366</v>
+      </c>
+      <c r="Z2">
+        <v>0.003945588927316836</v>
+      </c>
+      <c r="AA2">
+        <v>0.008394870058120927</v>
+      </c>
+      <c r="AB2">
+        <v>0.006322881693993938</v>
+      </c>
+      <c r="AC2">
+        <v>0.003945478177052217</v>
+      </c>
+      <c r="AD2">
+        <v>0.008394634419260034</v>
+      </c>
+      <c r="AE2">
+        <v>0.007657675933411487</v>
+      </c>
+      <c r="AF2">
+        <v>0.006172086802329659</v>
+      </c>
+      <c r="AG2">
+        <v>0.0131320995794248</v>
+      </c>
+      <c r="AH2">
+        <v>0.007657675933411487</v>
+      </c>
+      <c r="AI2">
+        <v>0.006172086802329659</v>
+      </c>
+      <c r="AJ2">
+        <v>0.0131320995794248</v>
+      </c>
+      <c r="AK2">
+        <v>0.009413718043378096</v>
+      </c>
+      <c r="AL2">
+        <v>0.00687201417166601</v>
+      </c>
+      <c r="AM2">
+        <v>0.01462130674822555</v>
+      </c>
+      <c r="AN2">
         <v>0.006845453360348112</v>
       </c>
-      <c r="O2">
+      <c r="AO2">
+        <v>0.004142868373682678</v>
+      </c>
+      <c r="AP2">
+        <v>0.008814613561026972</v>
+      </c>
+      <c r="AQ2">
         <v>0.006845453360348112</v>
       </c>
-      <c r="P2">
-        <v>0.007657675933411485</v>
-      </c>
-      <c r="Q2">
-        <v>0.007657675933411485</v>
+      <c r="AR2">
+        <v>0.004142868373682678</v>
+      </c>
+      <c r="AS2">
+        <v>0.008814613561026972</v>
+      </c>
+      <c r="AT2">
+        <v>0.007657675933411487</v>
+      </c>
+      <c r="AU2">
+        <v>0.006172086802329659</v>
+      </c>
+      <c r="AV2">
+        <v>0.0131320995794248</v>
+      </c>
+      <c r="AW2">
+        <v>0.007657675933411487</v>
+      </c>
+      <c r="AX2">
+        <v>0.006172086802329659</v>
+      </c>
+      <c r="AY2">
+        <v>0.0131320995794248</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:51">
       <c r="A3">
-        <v>0.007317156861737104</v>
+        <v>0.007317156861737105</v>
       </c>
       <c r="B3">
-        <v>0.007317156861737104</v>
+        <v>0.004290780783722639</v>
       </c>
       <c r="C3">
-        <v>0.01101267627921935</v>
+        <v>0.009129320816431145</v>
       </c>
       <c r="D3">
-        <v>0.006641823195653999</v>
+        <v>0.007317156861737105</v>
       </c>
       <c r="E3">
-        <v>0.01101267627921935</v>
+        <v>0.004290780783722639</v>
       </c>
       <c r="F3">
-        <v>0.01101267627921935</v>
+        <v>0.009129320816431145</v>
       </c>
       <c r="G3">
         <v>0.01101267627921935</v>
       </c>
       <c r="H3">
-        <v>0.006251137505423425</v>
+        <v>0.008039253683830126</v>
       </c>
       <c r="I3">
-        <v>0.006251137505423425</v>
+        <v>0.01710479507197899</v>
       </c>
       <c r="J3">
-        <v>0.00390060031284912</v>
+        <v>0.001117982973243789</v>
       </c>
       <c r="K3">
-        <v>0.008958363286135491</v>
+        <v>0.0008027117747890405</v>
       </c>
       <c r="L3">
-        <v>0.008958363286135491</v>
+        <v>0.001707897393168171</v>
       </c>
       <c r="M3">
         <v>0.01101267627921935</v>
       </c>
       <c r="N3">
+        <v>0.008039253683830126</v>
+      </c>
+      <c r="O3">
+        <v>0.01710479507197899</v>
+      </c>
+      <c r="P3">
+        <v>0.01101267627921935</v>
+      </c>
+      <c r="Q3">
+        <v>0.008039253683830126</v>
+      </c>
+      <c r="R3">
+        <v>0.01710479507197899</v>
+      </c>
+      <c r="S3">
+        <v>0.01101267627921935</v>
+      </c>
+      <c r="T3">
+        <v>0.008039253683830126</v>
+      </c>
+      <c r="U3">
+        <v>0.01710479507197899</v>
+      </c>
+      <c r="V3">
+        <v>0.006251137505423426</v>
+      </c>
+      <c r="W3">
+        <v>0.003900709803384218</v>
+      </c>
+      <c r="X3">
+        <v>0.008299382560391951</v>
+      </c>
+      <c r="Y3">
+        <v>0.006251137505423426</v>
+      </c>
+      <c r="Z3">
+        <v>0.003900709803384218</v>
+      </c>
+      <c r="AA3">
+        <v>0.008299382560391951</v>
+      </c>
+      <c r="AB3">
+        <v>0.006250962039822307</v>
+      </c>
+      <c r="AC3">
+        <v>0.00390060031284912</v>
+      </c>
+      <c r="AD3">
+        <v>0.008299149601806636</v>
+      </c>
+      <c r="AE3">
+        <v>0.008958363286135492</v>
+      </c>
+      <c r="AF3">
+        <v>0.007220440808625207</v>
+      </c>
+      <c r="AG3">
+        <v>0.0153626400183515</v>
+      </c>
+      <c r="AH3">
+        <v>0.008958363286135492</v>
+      </c>
+      <c r="AI3">
+        <v>0.007220440808625207</v>
+      </c>
+      <c r="AJ3">
+        <v>0.0153626400183515</v>
+      </c>
+      <c r="AK3">
+        <v>0.01101267627921935</v>
+      </c>
+      <c r="AL3">
+        <v>0.008039253683830126</v>
+      </c>
+      <c r="AM3">
+        <v>0.01710479507197899</v>
+      </c>
+      <c r="AN3">
         <v>0.006767589711753846</v>
       </c>
-      <c r="O3">
+      <c r="AO3">
+        <v>0.004095745293553428</v>
+      </c>
+      <c r="AP3">
+        <v>0.008714351688411547</v>
+      </c>
+      <c r="AQ3">
         <v>0.006767589711753846</v>
       </c>
-      <c r="P3">
-        <v>0.008958363286135491</v>
-      </c>
-      <c r="Q3">
-        <v>0.008958363286135491</v>
+      <c r="AR3">
+        <v>0.004095745293553428</v>
+      </c>
+      <c r="AS3">
+        <v>0.008714351688411547</v>
+      </c>
+      <c r="AT3">
+        <v>0.008958363286135492</v>
+      </c>
+      <c r="AU3">
+        <v>0.007220440808625207</v>
+      </c>
+      <c r="AV3">
+        <v>0.0153626400183515</v>
+      </c>
+      <c r="AW3">
+        <v>0.008958363286135492</v>
+      </c>
+      <c r="AX3">
+        <v>0.007220440808625207</v>
+      </c>
+      <c r="AY3">
+        <v>0.0153626400183515</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:51">
       <c r="A4">
         <v>0.007148783613695218</v>
       </c>
       <c r="B4">
+        <v>0.004192046711070876</v>
+      </c>
+      <c r="C4">
+        <v>0.008919248321427395</v>
+      </c>
+      <c r="D4">
         <v>0.007148783613695218</v>
       </c>
-      <c r="C4">
-        <v>0.007176254051528836</v>
-      </c>
-      <c r="D4">
-        <v>0.006488989879995556</v>
-      </c>
       <c r="E4">
-        <v>0.007176254051528836</v>
+        <v>0.004192046711070876</v>
       </c>
       <c r="F4">
-        <v>0.007176254051528836</v>
+        <v>0.008919248321427395</v>
       </c>
       <c r="G4">
         <v>0.007176254051528836</v>
       </c>
       <c r="H4">
-        <v>0.006107294159485542</v>
+        <v>0.00523866545761605</v>
       </c>
       <c r="I4">
-        <v>0.006107294159485542</v>
+        <v>0.01114609671833202</v>
       </c>
       <c r="J4">
-        <v>0.003810844584442924</v>
+        <v>0.001092257349477963</v>
       </c>
       <c r="K4">
-        <v>0.005837590173108594</v>
+        <v>0.0007842407769251773</v>
       </c>
       <c r="L4">
-        <v>0.005837590173108594</v>
+        <v>0.001668597397713143</v>
       </c>
       <c r="M4">
         <v>0.007176254051528836</v>
       </c>
       <c r="N4">
+        <v>0.00523866545761605</v>
+      </c>
+      <c r="O4">
+        <v>0.01114609671833202</v>
+      </c>
+      <c r="P4">
+        <v>0.007176254051528836</v>
+      </c>
+      <c r="Q4">
+        <v>0.00523866545761605</v>
+      </c>
+      <c r="R4">
+        <v>0.01114609671833202</v>
+      </c>
+      <c r="S4">
+        <v>0.007176254051528836</v>
+      </c>
+      <c r="T4">
+        <v>0.00523866545761605</v>
+      </c>
+      <c r="U4">
+        <v>0.01114609671833202</v>
+      </c>
+      <c r="V4">
+        <v>0.006107294159485543</v>
+      </c>
+      <c r="W4">
+        <v>0.003810951555518979</v>
+      </c>
+      <c r="X4">
+        <v>0.008108407564933995</v>
+      </c>
+      <c r="Y4">
+        <v>0.006107294159485543</v>
+      </c>
+      <c r="Z4">
+        <v>0.003810951555518979</v>
+      </c>
+      <c r="AA4">
+        <v>0.008108407564933995</v>
+      </c>
+      <c r="AB4">
+        <v>0.006107122731479044</v>
+      </c>
+      <c r="AC4">
+        <v>0.003810844584442924</v>
+      </c>
+      <c r="AD4">
+        <v>0.008108179966899836</v>
+      </c>
+      <c r="AE4">
+        <v>0.005837590173108594</v>
+      </c>
+      <c r="AF4">
+        <v>0.004705097679525528</v>
+      </c>
+      <c r="AG4">
+        <v>0.01001084612665006</v>
+      </c>
+      <c r="AH4">
+        <v>0.005837590173108594</v>
+      </c>
+      <c r="AI4">
+        <v>0.004705097679525528</v>
+      </c>
+      <c r="AJ4">
+        <v>0.01001084612665006</v>
+      </c>
+      <c r="AK4">
+        <v>0.007176254051528836</v>
+      </c>
+      <c r="AL4">
+        <v>0.00523866545761605</v>
+      </c>
+      <c r="AM4">
+        <v>0.01114609671833202</v>
+      </c>
+      <c r="AN4">
         <v>0.006611862414565312</v>
       </c>
-      <c r="O4">
+      <c r="AO4">
+        <v>0.004001499133294928</v>
+      </c>
+      <c r="AP4">
+        <v>0.008513827943180695</v>
+      </c>
+      <c r="AQ4">
         <v>0.006611862414565312</v>
       </c>
-      <c r="P4">
+      <c r="AR4">
+        <v>0.004001499133294928</v>
+      </c>
+      <c r="AS4">
+        <v>0.008513827943180695</v>
+      </c>
+      <c r="AT4">
         <v>0.005837590173108594</v>
       </c>
-      <c r="Q4">
+      <c r="AU4">
+        <v>0.004705097679525528</v>
+      </c>
+      <c r="AV4">
+        <v>0.01001084612665006</v>
+      </c>
+      <c r="AW4">
         <v>0.005837590173108594</v>
       </c>
+      <c r="AX4">
+        <v>0.004705097679525528</v>
+      </c>
+      <c r="AY4">
+        <v>0.01001084612665006</v>
+      </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:51">
       <c r="A5">
         <v>0.007148783613695218</v>
       </c>
       <c r="B5">
+        <v>0.004192046711070876</v>
+      </c>
+      <c r="C5">
+        <v>0.008919248321427395</v>
+      </c>
+      <c r="D5">
         <v>0.007148783613695218</v>
       </c>
-      <c r="C5">
-        <v>0.008861747252352734</v>
-      </c>
-      <c r="D5">
-        <v>0.006488989879995556</v>
-      </c>
       <c r="E5">
-        <v>0.008861747252352734</v>
+        <v>0.004192046711070876</v>
       </c>
       <c r="F5">
-        <v>0.008861747252352734</v>
+        <v>0.008919248321427395</v>
       </c>
       <c r="G5">
         <v>0.008861747252352734</v>
       </c>
       <c r="H5">
-        <v>0.006107294159485542</v>
+        <v>0.006469075494217495</v>
       </c>
       <c r="I5">
-        <v>0.006107294159485542</v>
+        <v>0.01376399041322871</v>
       </c>
       <c r="J5">
-        <v>0.003810844584442924</v>
+        <v>0.001092257349477963</v>
       </c>
       <c r="K5">
-        <v>0.007208670192756836</v>
+        <v>0.0007842407769251773</v>
       </c>
       <c r="L5">
-        <v>0.007208670192756836</v>
+        <v>0.001668597397713143</v>
       </c>
       <c r="M5">
         <v>0.008861747252352734</v>
       </c>
       <c r="N5">
+        <v>0.006469075494217495</v>
+      </c>
+      <c r="O5">
+        <v>0.01376399041322871</v>
+      </c>
+      <c r="P5">
+        <v>0.008861747252352734</v>
+      </c>
+      <c r="Q5">
+        <v>0.006469075494217495</v>
+      </c>
+      <c r="R5">
+        <v>0.01376399041322871</v>
+      </c>
+      <c r="S5">
+        <v>0.008861747252352734</v>
+      </c>
+      <c r="T5">
+        <v>0.006469075494217495</v>
+      </c>
+      <c r="U5">
+        <v>0.01376399041322871</v>
+      </c>
+      <c r="V5">
+        <v>0.006107294159485543</v>
+      </c>
+      <c r="W5">
+        <v>0.003810951555518979</v>
+      </c>
+      <c r="X5">
+        <v>0.008108407564933995</v>
+      </c>
+      <c r="Y5">
+        <v>0.006107294159485543</v>
+      </c>
+      <c r="Z5">
+        <v>0.003810951555518979</v>
+      </c>
+      <c r="AA5">
+        <v>0.008108407564933995</v>
+      </c>
+      <c r="AB5">
+        <v>0.006107122731479044</v>
+      </c>
+      <c r="AC5">
+        <v>0.003810844584442924</v>
+      </c>
+      <c r="AD5">
+        <v>0.008108179966899836</v>
+      </c>
+      <c r="AE5">
+        <v>0.007208670192756837</v>
+      </c>
+      <c r="AF5">
+        <v>0.005810188175362011</v>
+      </c>
+      <c r="AG5">
+        <v>0.01236210250077023</v>
+      </c>
+      <c r="AH5">
+        <v>0.007208670192756837</v>
+      </c>
+      <c r="AI5">
+        <v>0.005810188175362011</v>
+      </c>
+      <c r="AJ5">
+        <v>0.01236210250077023</v>
+      </c>
+      <c r="AK5">
+        <v>0.008861747252352734</v>
+      </c>
+      <c r="AL5">
+        <v>0.006469075494217495</v>
+      </c>
+      <c r="AM5">
+        <v>0.01376399041322871</v>
+      </c>
+      <c r="AN5">
         <v>0.006611862414565312</v>
       </c>
-      <c r="O5">
+      <c r="AO5">
+        <v>0.004001499133294928</v>
+      </c>
+      <c r="AP5">
+        <v>0.008513827943180695</v>
+      </c>
+      <c r="AQ5">
         <v>0.006611862414565312</v>
       </c>
-      <c r="P5">
-        <v>0.007208670192756836</v>
-      </c>
-      <c r="Q5">
-        <v>0.007208670192756836</v>
+      <c r="AR5">
+        <v>0.004001499133294928</v>
+      </c>
+      <c r="AS5">
+        <v>0.008513827943180695</v>
+      </c>
+      <c r="AT5">
+        <v>0.007208670192756837</v>
+      </c>
+      <c r="AU5">
+        <v>0.005810188175362011</v>
+      </c>
+      <c r="AV5">
+        <v>0.01236210250077023</v>
+      </c>
+      <c r="AW5">
+        <v>0.007208670192756837</v>
+      </c>
+      <c r="AX5">
+        <v>0.005810188175362011</v>
+      </c>
+      <c r="AY5">
+        <v>0.01236210250077023</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:51">
       <c r="A6">
         <v>0.004630180555808607</v>
       </c>
       <c r="B6">
+        <v>0.002715137877926167</v>
+      </c>
+      <c r="C6">
+        <v>0.005776889101970568</v>
+      </c>
+      <c r="D6">
         <v>0.004630180555808607</v>
       </c>
-      <c r="C6">
-        <v>0.005300762804602894</v>
-      </c>
-      <c r="D6">
-        <v>0.004202840146348175</v>
-      </c>
       <c r="E6">
-        <v>0.005300762804602894</v>
+        <v>0.002715137877926167</v>
       </c>
       <c r="F6">
-        <v>0.005300762804602894</v>
+        <v>0.005776889101970568</v>
       </c>
       <c r="G6">
         <v>0.005300762804602894</v>
       </c>
       <c r="H6">
-        <v>0.003955620451524137</v>
+        <v>0.003869556847360113</v>
       </c>
       <c r="I6">
-        <v>0.003955620451524137</v>
+        <v>0.008233099675234281</v>
       </c>
       <c r="J6">
-        <v>0.002468237877880805</v>
+        <v>0.0007074418551155107</v>
       </c>
       <c r="K6">
-        <v>0.004311954487109766</v>
+        <v>0.0005079432519729367</v>
       </c>
       <c r="L6">
-        <v>0.004311954487109766</v>
+        <v>0.001080730323346673</v>
       </c>
       <c r="M6">
         <v>0.005300762804602894</v>
       </c>
       <c r="N6">
+        <v>0.003869556847360113</v>
+      </c>
+      <c r="O6">
+        <v>0.008233099675234281</v>
+      </c>
+      <c r="P6">
+        <v>0.005300762804602894</v>
+      </c>
+      <c r="Q6">
+        <v>0.003869556847360113</v>
+      </c>
+      <c r="R6">
+        <v>0.008233099675234281</v>
+      </c>
+      <c r="S6">
+        <v>0.005300762804602894</v>
+      </c>
+      <c r="T6">
+        <v>0.003869556847360113</v>
+      </c>
+      <c r="U6">
+        <v>0.008233099675234281</v>
+      </c>
+      <c r="V6">
+        <v>0.003955620451524137</v>
+      </c>
+      <c r="W6">
+        <v>0.002468307161751061</v>
+      </c>
+      <c r="X6">
+        <v>0.005251717365427789</v>
+      </c>
+      <c r="Y6">
+        <v>0.003955620451524137</v>
+      </c>
+      <c r="Z6">
+        <v>0.002468307161751061</v>
+      </c>
+      <c r="AA6">
+        <v>0.005251717365427789</v>
+      </c>
+      <c r="AB6">
+        <v>0.003955509419680777</v>
+      </c>
+      <c r="AC6">
+        <v>0.002468237877880805</v>
+      </c>
+      <c r="AD6">
+        <v>0.005251569952937882</v>
+      </c>
+      <c r="AE6">
+        <v>0.004311954487109766</v>
+      </c>
+      <c r="AF6">
+        <v>0.003475435316610472</v>
+      </c>
+      <c r="AG6">
+        <v>0.007394543226830791</v>
+      </c>
+      <c r="AH6">
+        <v>0.004311954487109766</v>
+      </c>
+      <c r="AI6">
+        <v>0.003475435316610472</v>
+      </c>
+      <c r="AJ6">
+        <v>0.007394543226830791</v>
+      </c>
+      <c r="AK6">
+        <v>0.005300762804602894</v>
+      </c>
+      <c r="AL6">
+        <v>0.003869556847360113</v>
+      </c>
+      <c r="AM6">
+        <v>0.008233099675234281</v>
+      </c>
+      <c r="AN6">
         <v>0.004282423198675833</v>
       </c>
-      <c r="O6">
+      <c r="AO6">
+        <v>0.002591722519838614</v>
+      </c>
+      <c r="AP6">
+        <v>0.005514303233699178</v>
+      </c>
+      <c r="AQ6">
         <v>0.004282423198675833</v>
       </c>
-      <c r="P6">
+      <c r="AR6">
+        <v>0.002591722519838614</v>
+      </c>
+      <c r="AS6">
+        <v>0.005514303233699178</v>
+      </c>
+      <c r="AT6">
         <v>0.004311954487109766</v>
       </c>
-      <c r="Q6">
+      <c r="AU6">
+        <v>0.003475435316610472</v>
+      </c>
+      <c r="AV6">
+        <v>0.007394543226830791</v>
+      </c>
+      <c r="AW6">
         <v>0.004311954487109766</v>
       </c>
+      <c r="AX6">
+        <v>0.003475435316610472</v>
+      </c>
+      <c r="AY6">
+        <v>0.007394543226830791</v>
+      </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:51">
       <c r="A7">
         <v>0.004630180555808607</v>
       </c>
       <c r="B7">
+        <v>0.002715137877926167</v>
+      </c>
+      <c r="C7">
+        <v>0.005776889101970568</v>
+      </c>
+      <c r="D7">
         <v>0.004630180555808607</v>
       </c>
-      <c r="C7">
-        <v>0.005211675134796919</v>
-      </c>
-      <c r="D7">
-        <v>0.004202840146348175</v>
-      </c>
       <c r="E7">
-        <v>0.005211675134796919</v>
+        <v>0.002715137877926167</v>
       </c>
       <c r="F7">
-        <v>0.005211675134796919</v>
+        <v>0.005776889101970568</v>
       </c>
       <c r="G7">
         <v>0.005211675134796919</v>
       </c>
       <c r="H7">
-        <v>0.003955620451524137</v>
+        <v>0.003804522848401751</v>
       </c>
       <c r="I7">
-        <v>0.003955620451524137</v>
+        <v>0.008094729464684576</v>
       </c>
       <c r="J7">
-        <v>0.002468237877880805</v>
+        <v>0.0007074418551155107</v>
       </c>
       <c r="K7">
-        <v>0.004239485298857755</v>
+        <v>0.0005079432519729367</v>
       </c>
       <c r="L7">
-        <v>0.004239485298857755</v>
+        <v>0.001080730323346673</v>
       </c>
       <c r="M7">
         <v>0.005211675134796919</v>
       </c>
       <c r="N7">
+        <v>0.003804522848401751</v>
+      </c>
+      <c r="O7">
+        <v>0.008094729464684576</v>
+      </c>
+      <c r="P7">
+        <v>0.005211675134796919</v>
+      </c>
+      <c r="Q7">
+        <v>0.003804522848401751</v>
+      </c>
+      <c r="R7">
+        <v>0.008094729464684576</v>
+      </c>
+      <c r="S7">
+        <v>0.005211675134796919</v>
+      </c>
+      <c r="T7">
+        <v>0.003804522848401751</v>
+      </c>
+      <c r="U7">
+        <v>0.008094729464684576</v>
+      </c>
+      <c r="V7">
+        <v>0.003955620451524137</v>
+      </c>
+      <c r="W7">
+        <v>0.002468307161751061</v>
+      </c>
+      <c r="X7">
+        <v>0.005251717365427789</v>
+      </c>
+      <c r="Y7">
+        <v>0.003955620451524137</v>
+      </c>
+      <c r="Z7">
+        <v>0.002468307161751061</v>
+      </c>
+      <c r="AA7">
+        <v>0.005251717365427789</v>
+      </c>
+      <c r="AB7">
+        <v>0.003955509419680777</v>
+      </c>
+      <c r="AC7">
+        <v>0.002468237877880805</v>
+      </c>
+      <c r="AD7">
+        <v>0.005251569952937882</v>
+      </c>
+      <c r="AE7">
+        <v>0.004239485298857756</v>
+      </c>
+      <c r="AF7">
+        <v>0.003417025150879351</v>
+      </c>
+      <c r="AG7">
+        <v>0.007270266278466703</v>
+      </c>
+      <c r="AH7">
+        <v>0.004239485298857756</v>
+      </c>
+      <c r="AI7">
+        <v>0.003417025150879351</v>
+      </c>
+      <c r="AJ7">
+        <v>0.007270266278466703</v>
+      </c>
+      <c r="AK7">
+        <v>0.005211675134796919</v>
+      </c>
+      <c r="AL7">
+        <v>0.003804522848401751</v>
+      </c>
+      <c r="AM7">
+        <v>0.008094729464684576</v>
+      </c>
+      <c r="AN7">
         <v>0.004282423198675833</v>
       </c>
-      <c r="O7">
+      <c r="AO7">
+        <v>0.002591722519838614</v>
+      </c>
+      <c r="AP7">
+        <v>0.005514303233699178</v>
+      </c>
+      <c r="AQ7">
         <v>0.004282423198675833</v>
       </c>
-      <c r="P7">
-        <v>0.004239485298857755</v>
-      </c>
-      <c r="Q7">
-        <v>0.004239485298857755</v>
+      <c r="AR7">
+        <v>0.002591722519838614</v>
+      </c>
+      <c r="AS7">
+        <v>0.005514303233699178</v>
+      </c>
+      <c r="AT7">
+        <v>0.004239485298857756</v>
+      </c>
+      <c r="AU7">
+        <v>0.003417025150879351</v>
+      </c>
+      <c r="AV7">
+        <v>0.007270266278466703</v>
+      </c>
+      <c r="AW7">
+        <v>0.004239485298857756</v>
+      </c>
+      <c r="AX7">
+        <v>0.003417025150879351</v>
+      </c>
+      <c r="AY7">
+        <v>0.007270266278466703</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:51">
       <c r="A8">
         <v>0.002315090277904303</v>
       </c>
       <c r="B8">
+        <v>0.001357568938963084</v>
+      </c>
+      <c r="C8">
+        <v>0.002888444550985284</v>
+      </c>
+      <c r="D8">
         <v>0.002315090277904303</v>
       </c>
-      <c r="C8">
-        <v>0.003474450089864613</v>
-      </c>
-      <c r="D8">
-        <v>0.002101420073174088</v>
-      </c>
       <c r="E8">
-        <v>0.003474450089864613</v>
+        <v>0.001357568938963084</v>
       </c>
       <c r="F8">
-        <v>0.003474450089864613</v>
+        <v>0.002888444550985284</v>
       </c>
       <c r="G8">
         <v>0.003474450089864613</v>
       </c>
       <c r="H8">
-        <v>0.001977810225762068</v>
+        <v>0.002536348565601167</v>
       </c>
       <c r="I8">
-        <v>0.001977810225762068</v>
+        <v>0.005396486309789717</v>
       </c>
       <c r="J8">
-        <v>0.001234118938940402</v>
+        <v>0.0003537209275577553</v>
       </c>
       <c r="K8">
-        <v>0.002826323532571836</v>
+        <v>0.0002539716259864684</v>
       </c>
       <c r="L8">
-        <v>0.002826323532571836</v>
+        <v>0.0005403651616733367</v>
       </c>
       <c r="M8">
         <v>0.003474450089864613</v>
       </c>
       <c r="N8">
+        <v>0.002536348565601167</v>
+      </c>
+      <c r="O8">
+        <v>0.005396486309789717</v>
+      </c>
+      <c r="P8">
+        <v>0.003474450089864613</v>
+      </c>
+      <c r="Q8">
+        <v>0.002536348565601167</v>
+      </c>
+      <c r="R8">
+        <v>0.005396486309789717</v>
+      </c>
+      <c r="S8">
+        <v>0.003474450089864613</v>
+      </c>
+      <c r="T8">
+        <v>0.002536348565601167</v>
+      </c>
+      <c r="U8">
+        <v>0.005396486309789717</v>
+      </c>
+      <c r="V8">
+        <v>0.001977810225762068</v>
+      </c>
+      <c r="W8">
+        <v>0.001234153580875531</v>
+      </c>
+      <c r="X8">
+        <v>0.002625858682713895</v>
+      </c>
+      <c r="Y8">
+        <v>0.001977810225762068</v>
+      </c>
+      <c r="Z8">
+        <v>0.001234153580875531</v>
+      </c>
+      <c r="AA8">
+        <v>0.002625858682713895</v>
+      </c>
+      <c r="AB8">
+        <v>0.001977754709840389</v>
+      </c>
+      <c r="AC8">
+        <v>0.001234118938940402</v>
+      </c>
+      <c r="AD8">
+        <v>0.002625784976468941</v>
+      </c>
+      <c r="AE8">
+        <v>0.002826323532571837</v>
+      </c>
+      <c r="AF8">
+        <v>0.002278016767252901</v>
+      </c>
+      <c r="AG8">
+        <v>0.004846844185644469</v>
+      </c>
+      <c r="AH8">
+        <v>0.002826323532571837</v>
+      </c>
+      <c r="AI8">
+        <v>0.002278016767252901</v>
+      </c>
+      <c r="AJ8">
+        <v>0.004846844185644469</v>
+      </c>
+      <c r="AK8">
+        <v>0.003474450089864613</v>
+      </c>
+      <c r="AL8">
+        <v>0.002536348565601167</v>
+      </c>
+      <c r="AM8">
+        <v>0.005396486309789717</v>
+      </c>
+      <c r="AN8">
         <v>0.002141211599337917</v>
       </c>
-      <c r="O8">
+      <c r="AO8">
+        <v>0.001295861259919307</v>
+      </c>
+      <c r="AP8">
+        <v>0.002757151616849589</v>
+      </c>
+      <c r="AQ8">
         <v>0.002141211599337917</v>
       </c>
-      <c r="P8">
-        <v>0.002826323532571836</v>
-      </c>
-      <c r="Q8">
-        <v>0.002826323532571836</v>
+      <c r="AR8">
+        <v>0.001295861259919307</v>
+      </c>
+      <c r="AS8">
+        <v>0.002757151616849589</v>
+      </c>
+      <c r="AT8">
+        <v>0.002826323532571837</v>
+      </c>
+      <c r="AU8">
+        <v>0.002278016767252901</v>
+      </c>
+      <c r="AV8">
+        <v>0.004846844185644469</v>
+      </c>
+      <c r="AW8">
+        <v>0.002826323532571837</v>
+      </c>
+      <c r="AX8">
+        <v>0.002278016767252901</v>
+      </c>
+      <c r="AY8">
+        <v>0.004846844185644469</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:51">
       <c r="A9">
         <v>0.002315090277904303</v>
       </c>
       <c r="B9">
+        <v>0.001357568938963084</v>
+      </c>
+      <c r="C9">
+        <v>0.002888444550985284</v>
+      </c>
+      <c r="D9">
         <v>0.002315090277904303</v>
       </c>
-      <c r="C9">
-        <v>0.001737225044932306</v>
-      </c>
-      <c r="D9">
-        <v>0.002101420073174088</v>
-      </c>
       <c r="E9">
-        <v>0.001737225044932306</v>
+        <v>0.001357568938963084</v>
       </c>
       <c r="F9">
-        <v>0.001737225044932306</v>
+        <v>0.002888444550985284</v>
       </c>
       <c r="G9">
         <v>0.001737225044932306</v>
       </c>
       <c r="H9">
-        <v>0.001977810225762068</v>
+        <v>0.001268174282800584</v>
       </c>
       <c r="I9">
-        <v>0.001977810225762068</v>
+        <v>0.002698243154894859</v>
       </c>
       <c r="J9">
-        <v>0.001234118938940402</v>
+        <v>0.0003537209275577553</v>
       </c>
       <c r="K9">
-        <v>0.001413161766285918</v>
+        <v>0.0002539716259864684</v>
       </c>
       <c r="L9">
-        <v>0.001413161766285918</v>
+        <v>0.0005403651616733367</v>
       </c>
       <c r="M9">
         <v>0.001737225044932306</v>
       </c>
       <c r="N9">
+        <v>0.001268174282800584</v>
+      </c>
+      <c r="O9">
+        <v>0.002698243154894859</v>
+      </c>
+      <c r="P9">
+        <v>0.001737225044932306</v>
+      </c>
+      <c r="Q9">
+        <v>0.001268174282800584</v>
+      </c>
+      <c r="R9">
+        <v>0.002698243154894859</v>
+      </c>
+      <c r="S9">
+        <v>0.001737225044932306</v>
+      </c>
+      <c r="T9">
+        <v>0.001268174282800584</v>
+      </c>
+      <c r="U9">
+        <v>0.002698243154894859</v>
+      </c>
+      <c r="V9">
+        <v>0.001977810225762068</v>
+      </c>
+      <c r="W9">
+        <v>0.001234153580875531</v>
+      </c>
+      <c r="X9">
+        <v>0.002625858682713895</v>
+      </c>
+      <c r="Y9">
+        <v>0.001977810225762068</v>
+      </c>
+      <c r="Z9">
+        <v>0.001234153580875531</v>
+      </c>
+      <c r="AA9">
+        <v>0.002625858682713895</v>
+      </c>
+      <c r="AB9">
+        <v>0.001977754709840389</v>
+      </c>
+      <c r="AC9">
+        <v>0.001234118938940402</v>
+      </c>
+      <c r="AD9">
+        <v>0.002625784976468941</v>
+      </c>
+      <c r="AE9">
+        <v>0.001413161766285918</v>
+      </c>
+      <c r="AF9">
+        <v>0.00113900838362645</v>
+      </c>
+      <c r="AG9">
+        <v>0.002423422092822234</v>
+      </c>
+      <c r="AH9">
+        <v>0.001413161766285918</v>
+      </c>
+      <c r="AI9">
+        <v>0.00113900838362645</v>
+      </c>
+      <c r="AJ9">
+        <v>0.002423422092822234</v>
+      </c>
+      <c r="AK9">
+        <v>0.001737225044932306</v>
+      </c>
+      <c r="AL9">
+        <v>0.001268174282800584</v>
+      </c>
+      <c r="AM9">
+        <v>0.002698243154894859</v>
+      </c>
+      <c r="AN9">
         <v>0.002141211599337917</v>
       </c>
-      <c r="O9">
+      <c r="AO9">
+        <v>0.001295861259919307</v>
+      </c>
+      <c r="AP9">
+        <v>0.002757151616849589</v>
+      </c>
+      <c r="AQ9">
         <v>0.002141211599337917</v>
       </c>
-      <c r="P9">
+      <c r="AR9">
+        <v>0.001295861259919307</v>
+      </c>
+      <c r="AS9">
+        <v>0.002757151616849589</v>
+      </c>
+      <c r="AT9">
         <v>0.001413161766285918</v>
       </c>
-      <c r="Q9">
+      <c r="AU9">
+        <v>0.00113900838362645</v>
+      </c>
+      <c r="AV9">
+        <v>0.002423422092822234</v>
+      </c>
+      <c r="AW9">
         <v>0.001413161766285918</v>
       </c>
+      <c r="AX9">
+        <v>0.00113900838362645</v>
+      </c>
+      <c r="AY9">
+        <v>0.002423422092822234</v>
+      </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:51">
       <c r="A10">
-        <v>0.06600898496669168</v>
+        <v>0.06600898496669169</v>
       </c>
       <c r="B10">
-        <v>0.06600898496669168</v>
+        <v>0.03870766878446801</v>
       </c>
       <c r="C10">
-        <v>0.02505837176621392</v>
+        <v>0.08235674209461277</v>
       </c>
       <c r="D10">
-        <v>0.05991671570770007</v>
+        <v>0.06600898496669169</v>
       </c>
       <c r="E10">
-        <v>0.02505837176621392</v>
+        <v>0.03870766878446801</v>
       </c>
       <c r="F10">
-        <v>0.02505837176621392</v>
+        <v>0.08235674209461277</v>
       </c>
       <c r="G10">
         <v>0.02505837176621392</v>
       </c>
       <c r="H10">
-        <v>0.05639229135266317</v>
+        <v>0.01829261138933616</v>
       </c>
       <c r="I10">
-        <v>0.05639229135266317</v>
+        <v>0.03892044976454501</v>
       </c>
       <c r="J10">
-        <v>0.03518780207628425</v>
+        <v>0.01008546388553805</v>
       </c>
       <c r="K10">
-        <v>0.02038396407459801</v>
+        <v>0.007241363069816324</v>
       </c>
       <c r="L10">
-        <v>0.02038396407459801</v>
+        <v>0.0154071554676943</v>
       </c>
       <c r="M10">
         <v>0.02505837176621392</v>
       </c>
       <c r="N10">
+        <v>0.01829261138933616</v>
+      </c>
+      <c r="O10">
+        <v>0.03892044976454501</v>
+      </c>
+      <c r="P10">
+        <v>0.02505837176621392</v>
+      </c>
+      <c r="Q10">
+        <v>0.01829261138933616</v>
+      </c>
+      <c r="R10">
+        <v>0.03892044976454501</v>
+      </c>
+      <c r="S10">
+        <v>0.02505837176621392</v>
+      </c>
+      <c r="T10">
+        <v>0.01829261138933616</v>
+      </c>
+      <c r="U10">
+        <v>0.03892044976454501</v>
+      </c>
+      <c r="V10">
+        <v>0.05639229135266319</v>
+      </c>
+      <c r="W10">
+        <v>0.03518878980406183</v>
+      </c>
+      <c r="X10">
+        <v>0.07486976554055706</v>
+      </c>
+      <c r="Y10">
+        <v>0.05639229135266319</v>
+      </c>
+      <c r="Z10">
+        <v>0.03518878980406183</v>
+      </c>
+      <c r="AA10">
+        <v>0.07486976554055706</v>
+      </c>
+      <c r="AB10">
+        <v>0.05639070845558373</v>
+      </c>
+      <c r="AC10">
+        <v>0.03518780207628425</v>
+      </c>
+      <c r="AD10">
+        <v>0.07486766399209413</v>
+      </c>
+      <c r="AE10">
+        <v>0.02038396407459801</v>
+      </c>
+      <c r="AF10">
+        <v>0.016429475044126</v>
+      </c>
+      <c r="AG10">
+        <v>0.03495632988111914</v>
+      </c>
+      <c r="AH10">
+        <v>0.02038396407459801</v>
+      </c>
+      <c r="AI10">
+        <v>0.016429475044126</v>
+      </c>
+      <c r="AJ10">
+        <v>0.03495632988111914</v>
+      </c>
+      <c r="AK10">
+        <v>0.02505837176621392</v>
+      </c>
+      <c r="AL10">
+        <v>0.01829261138933616</v>
+      </c>
+      <c r="AM10">
+        <v>0.03892044976454501</v>
+      </c>
+      <c r="AN10">
         <v>0.0610512711405567</v>
       </c>
-      <c r="O10">
+      <c r="AO10">
+        <v>0.03694822929426492</v>
+      </c>
+      <c r="AP10">
+        <v>0.07861325381758491</v>
+      </c>
+      <c r="AQ10">
         <v>0.0610512711405567</v>
       </c>
-      <c r="P10">
+      <c r="AR10">
+        <v>0.03694822929426492</v>
+      </c>
+      <c r="AS10">
+        <v>0.07861325381758491</v>
+      </c>
+      <c r="AT10">
         <v>0.02038396407459801</v>
       </c>
-      <c r="Q10">
+      <c r="AU10">
+        <v>0.016429475044126</v>
+      </c>
+      <c r="AV10">
+        <v>0.03495632988111914</v>
+      </c>
+      <c r="AW10">
         <v>0.02038396407459801</v>
+      </c>
+      <c r="AX10">
+        <v>0.016429475044126</v>
+      </c>
+      <c r="AY10">
+        <v>0.03495632988111914</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FIX: stubble deterioration in CropResidueSim.py. ADD: trample decay to stubsim and add min consumption to each cat so that the transfer always works 30k profit increase (10 due to decay and 20k due to trample)
</commit_message>
<xml_diff>
--- a/stubble sim.xlsx
+++ b/stubble sim.xlsx
@@ -348,1552 +348,1552 @@
   <sheetData>
     <row r="1" spans="1:51">
       <c r="A1">
-        <v>0.04163557985371009</v>
+        <v>0.05630272974597433</v>
       </c>
       <c r="B1">
-        <v>0.0244151040262156</v>
+        <v>0.03301592072303935</v>
       </c>
       <c r="C1">
-        <v>0.05194702984301191</v>
+        <v>0.07024663983625393</v>
       </c>
       <c r="D1">
-        <v>0.04163557985371009</v>
+        <v>0.05630272974597433</v>
       </c>
       <c r="E1">
-        <v>0.0244151040262156</v>
+        <v>0.03301592072303935</v>
       </c>
       <c r="F1">
-        <v>0.05194702984301191</v>
+        <v>0.07024663983625393</v>
       </c>
       <c r="G1">
-        <v>0.03812858876173155</v>
+        <v>0.04939719860297297</v>
       </c>
       <c r="H1">
-        <v>0.02783386979606403</v>
+        <v>0.03605995498017027</v>
       </c>
       <c r="I1">
-        <v>0.05922099956609368</v>
+        <v>0.07672330846844737</v>
       </c>
       <c r="J1">
-        <v>0.00636146938450756</v>
+        <v>0.00860245234488557</v>
       </c>
       <c r="K1">
-        <v>0.004567535018076429</v>
+        <v>0.00617656078362784</v>
       </c>
       <c r="L1">
-        <v>0.00971815961292857</v>
+        <v>0.01314161868856987</v>
       </c>
       <c r="M1">
-        <v>0.03812858876173155</v>
+        <v>0.04939719860297297</v>
       </c>
       <c r="N1">
-        <v>0.02783386979606403</v>
+        <v>0.03605995498017027</v>
       </c>
       <c r="O1">
-        <v>0.05922099956609368</v>
+        <v>0.07672330846844737</v>
       </c>
       <c r="P1">
-        <v>0.03812858876173155</v>
+        <v>0.04939719860297297</v>
       </c>
       <c r="Q1">
-        <v>0.02783386979606403</v>
+        <v>0.03605995498017027</v>
       </c>
       <c r="R1">
-        <v>0.05922099956609368</v>
+        <v>0.07672330846844737</v>
       </c>
       <c r="S1">
-        <v>0.03812858876173155</v>
+        <v>0.04939719860297297</v>
       </c>
       <c r="T1">
-        <v>0.02783386979606403</v>
+        <v>0.03605995498017027</v>
       </c>
       <c r="U1">
-        <v>0.05922099956609368</v>
+        <v>0.07672330846844737</v>
       </c>
       <c r="V1">
-        <v>0.0355697902479831</v>
+        <v>0.04810011760349556</v>
       </c>
       <c r="W1">
-        <v>0.02219554911474146</v>
+        <v>0.03001447338458123</v>
       </c>
       <c r="X1">
-        <v>0.04722457258455628</v>
+        <v>0.06386058166932175</v>
       </c>
       <c r="Y1">
-        <v>0.0355697902479831</v>
+        <v>0.04810011760349556</v>
       </c>
       <c r="Z1">
-        <v>0.02219554911474146</v>
+        <v>0.03001447338458123</v>
       </c>
       <c r="AA1">
-        <v>0.04722457258455628</v>
+        <v>0.06386058166932175</v>
       </c>
       <c r="AB1">
-        <v>0.03556879182575642</v>
+        <v>0.0480987674626545</v>
       </c>
       <c r="AC1">
-        <v>0.022194926099272</v>
+        <v>0.03001363089669641</v>
       </c>
       <c r="AD1">
-        <v>0.04722324701972765</v>
+        <v>0.06385878914190724</v>
       </c>
       <c r="AE1">
-        <v>0.03101605286989031</v>
+        <v>0.04018260767710363</v>
       </c>
       <c r="AF1">
-        <v>0.02499893861313159</v>
+        <v>0.03238718178774552</v>
       </c>
       <c r="AG1">
-        <v>0.05318923109176933</v>
+        <v>0.06890889742073515</v>
       </c>
       <c r="AH1">
-        <v>0.03101605286989031</v>
+        <v>0.04018260767710363</v>
       </c>
       <c r="AI1">
-        <v>0.02499893861313159</v>
+        <v>0.03238718178774552</v>
       </c>
       <c r="AJ1">
-        <v>0.05318923109176933</v>
+        <v>0.06890889742073515</v>
       </c>
       <c r="AK1">
-        <v>0.03812858876173155</v>
+        <v>0.04939719860297297</v>
       </c>
       <c r="AL1">
-        <v>0.02783386979606403</v>
+        <v>0.03605995498017027</v>
       </c>
       <c r="AM1">
-        <v>0.05922099956609368</v>
+        <v>0.07672330846844737</v>
       </c>
       <c r="AN1">
-        <v>0.03850847086992486</v>
+        <v>0.05207402024753847</v>
       </c>
       <c r="AO1">
-        <v>0.02330532657047853</v>
+        <v>0.03151519705381028</v>
       </c>
       <c r="AP1">
-        <v>0.04958580121378409</v>
+        <v>0.06705361075278783</v>
       </c>
       <c r="AQ1">
-        <v>0.03850847086992486</v>
+        <v>0.05207402024753847</v>
       </c>
       <c r="AR1">
-        <v>0.02330532657047853</v>
+        <v>0.03151519705381028</v>
       </c>
       <c r="AS1">
-        <v>0.04958580121378409</v>
+        <v>0.06705361075278783</v>
       </c>
       <c r="AT1">
-        <v>0.03101605286989031</v>
+        <v>0.04018260767710363</v>
       </c>
       <c r="AU1">
-        <v>0.02499893861313159</v>
+        <v>0.03238718178774552</v>
       </c>
       <c r="AV1">
-        <v>0.05318923109176933</v>
+        <v>0.06890889742073515</v>
       </c>
       <c r="AW1">
-        <v>0.03101605286989031</v>
+        <v>0.04018260767710363</v>
       </c>
       <c r="AX1">
-        <v>0.02499893861313159</v>
+        <v>0.03238718178774552</v>
       </c>
       <c r="AY1">
-        <v>0.05318923109176933</v>
+        <v>0.06890889742073515</v>
       </c>
     </row>
     <row r="2" spans="1:51">
       <c r="A2">
-        <v>0.007401343485758048</v>
+        <v>0.01233679495482404</v>
       </c>
       <c r="B2">
-        <v>0.004340147820048519</v>
+        <v>0.007234296561508821</v>
       </c>
       <c r="C2">
-        <v>0.009234357063933019</v>
+        <v>0.01539212034363579</v>
       </c>
       <c r="D2">
-        <v>0.007401343485758048</v>
+        <v>0.01233679495482404</v>
       </c>
       <c r="E2">
-        <v>0.004340147820048519</v>
+        <v>0.007234296561508821</v>
       </c>
       <c r="F2">
-        <v>0.009234357063933019</v>
+        <v>0.01539212034363579</v>
       </c>
       <c r="G2">
-        <v>0.009413718043378096</v>
+        <v>0.0186693753286726</v>
       </c>
       <c r="H2">
-        <v>0.00687201417166601</v>
+        <v>0.013628643989931</v>
       </c>
       <c r="I2">
-        <v>0.01462130674822555</v>
+        <v>0.02899711487219362</v>
       </c>
       <c r="J2">
-        <v>0.001130845785126702</v>
+        <v>0.001884929756804317</v>
       </c>
       <c r="K2">
-        <v>0.000811947273720972</v>
+        <v>0.0013533795653855</v>
       </c>
       <c r="L2">
-        <v>0.001727547390895685</v>
+        <v>0.002879530990181913</v>
       </c>
       <c r="M2">
-        <v>0.009413718043378096</v>
+        <v>0.0186693753286726</v>
       </c>
       <c r="N2">
-        <v>0.00687201417166601</v>
+        <v>0.013628643989931</v>
       </c>
       <c r="O2">
-        <v>0.01462130674822555</v>
+        <v>0.02899711487219362</v>
       </c>
       <c r="P2">
-        <v>0.009413718043378096</v>
+        <v>0.0186693753286726</v>
       </c>
       <c r="Q2">
-        <v>0.00687201417166601</v>
+        <v>0.013628643989931</v>
       </c>
       <c r="R2">
-        <v>0.01462130674822555</v>
+        <v>0.02899711487219362</v>
       </c>
       <c r="S2">
-        <v>0.009413718043378096</v>
+        <v>0.0186693753286726</v>
       </c>
       <c r="T2">
-        <v>0.00687201417166601</v>
+        <v>0.013628643989931</v>
       </c>
       <c r="U2">
-        <v>0.01462130674822555</v>
+        <v>0.02899711487219362</v>
       </c>
       <c r="V2">
-        <v>0.006323059178392366</v>
+        <v>0.01053947634252451</v>
       </c>
       <c r="W2">
-        <v>0.003945588927316836</v>
+        <v>0.006576633237735292</v>
       </c>
       <c r="X2">
-        <v>0.008394870058120927</v>
+        <v>0.01399283667603253</v>
       </c>
       <c r="Y2">
-        <v>0.006323059178392366</v>
+        <v>0.01053947634252451</v>
       </c>
       <c r="Z2">
-        <v>0.003945588927316836</v>
+        <v>0.006576633237735292</v>
       </c>
       <c r="AA2">
-        <v>0.008394870058120927</v>
+        <v>0.01399283667603253</v>
       </c>
       <c r="AB2">
-        <v>0.006322881693993938</v>
+        <v>0.01053918050587873</v>
       </c>
       <c r="AC2">
-        <v>0.003945478177052217</v>
+        <v>0.006576448635668326</v>
       </c>
       <c r="AD2">
-        <v>0.008394634419260034</v>
+        <v>0.01399244390567729</v>
       </c>
       <c r="AE2">
-        <v>0.007657675933411487</v>
+        <v>0.0151867758825396</v>
       </c>
       <c r="AF2">
-        <v>0.006172086802329659</v>
+        <v>0.01224054136132692</v>
       </c>
       <c r="AG2">
-        <v>0.0131320995794248</v>
+        <v>0.02604370502409983</v>
       </c>
       <c r="AH2">
-        <v>0.007657675933411487</v>
+        <v>0.0151867758825396</v>
       </c>
       <c r="AI2">
-        <v>0.006172086802329659</v>
+        <v>0.01224054136132692</v>
       </c>
       <c r="AJ2">
-        <v>0.0131320995794248</v>
+        <v>0.02604370502409983</v>
       </c>
       <c r="AK2">
-        <v>0.009413718043378096</v>
+        <v>0.0186693753286726</v>
       </c>
       <c r="AL2">
-        <v>0.00687201417166601</v>
+        <v>0.013628643989931</v>
       </c>
       <c r="AM2">
-        <v>0.01462130674822555</v>
+        <v>0.02899711487219362</v>
       </c>
       <c r="AN2">
-        <v>0.006845453360348112</v>
+        <v>0.011410219596203</v>
       </c>
       <c r="AO2">
-        <v>0.004142868373682678</v>
+        <v>0.006905464899622056</v>
       </c>
       <c r="AP2">
-        <v>0.008814613561026972</v>
+        <v>0.01469247850983416</v>
       </c>
       <c r="AQ2">
-        <v>0.006845453360348112</v>
+        <v>0.011410219596203</v>
       </c>
       <c r="AR2">
-        <v>0.004142868373682678</v>
+        <v>0.006905464899622056</v>
       </c>
       <c r="AS2">
-        <v>0.008814613561026972</v>
+        <v>0.01469247850983416</v>
       </c>
       <c r="AT2">
-        <v>0.007657675933411487</v>
+        <v>0.0151867758825396</v>
       </c>
       <c r="AU2">
-        <v>0.006172086802329659</v>
+        <v>0.01224054136132692</v>
       </c>
       <c r="AV2">
-        <v>0.0131320995794248</v>
+        <v>0.02604370502409983</v>
       </c>
       <c r="AW2">
-        <v>0.007657675933411487</v>
+        <v>0.0151867758825396</v>
       </c>
       <c r="AX2">
-        <v>0.006172086802329659</v>
+        <v>0.01224054136132692</v>
       </c>
       <c r="AY2">
-        <v>0.0131320995794248</v>
+        <v>0.02604370502409983</v>
       </c>
     </row>
     <row r="3" spans="1:51">
       <c r="A3">
-        <v>0.007317156861737105</v>
+        <v>0.02028415697728426</v>
       </c>
       <c r="B3">
-        <v>0.004290780783722639</v>
+        <v>0.01189462965147949</v>
       </c>
       <c r="C3">
-        <v>0.009129320816431145</v>
+        <v>0.02530772266272232</v>
       </c>
       <c r="D3">
-        <v>0.007317156861737105</v>
+        <v>0.02028415697728426</v>
       </c>
       <c r="E3">
-        <v>0.004290780783722639</v>
+        <v>0.01189462965147949</v>
       </c>
       <c r="F3">
-        <v>0.009129320816431145</v>
+        <v>0.02530772266272232</v>
       </c>
       <c r="G3">
-        <v>0.01101267627921935</v>
+        <v>0.01725592169446037</v>
       </c>
       <c r="H3">
-        <v>0.008039253683830126</v>
+        <v>0.01259682283695607</v>
       </c>
       <c r="I3">
-        <v>0.01710479507197899</v>
+        <v>0.02680175071692781</v>
       </c>
       <c r="J3">
-        <v>0.001117982973243789</v>
+        <v>0.003099201309431047</v>
       </c>
       <c r="K3">
-        <v>0.0008027117747890405</v>
+        <v>0.002225226540171492</v>
       </c>
       <c r="L3">
-        <v>0.001707897393168171</v>
+        <v>0.004734524553556364</v>
       </c>
       <c r="M3">
-        <v>0.01101267627921935</v>
+        <v>0.01725592169446037</v>
       </c>
       <c r="N3">
-        <v>0.008039253683830126</v>
+        <v>0.01259682283695607</v>
       </c>
       <c r="O3">
-        <v>0.01710479507197899</v>
+        <v>0.02680175071692781</v>
       </c>
       <c r="P3">
-        <v>0.01101267627921935</v>
+        <v>0.01725592169446037</v>
       </c>
       <c r="Q3">
-        <v>0.008039253683830126</v>
+        <v>0.01259682283695607</v>
       </c>
       <c r="R3">
-        <v>0.01710479507197899</v>
+        <v>0.02680175071692781</v>
       </c>
       <c r="S3">
-        <v>0.01101267627921935</v>
+        <v>0.01725592169446037</v>
       </c>
       <c r="T3">
-        <v>0.008039253683830126</v>
+        <v>0.01259682283695607</v>
       </c>
       <c r="U3">
-        <v>0.01710479507197899</v>
+        <v>0.02680175071692781</v>
       </c>
       <c r="V3">
-        <v>0.006251137505423426</v>
+        <v>0.01732900590250509</v>
       </c>
       <c r="W3">
-        <v>0.003900709803384218</v>
+        <v>0.01081329968316318</v>
       </c>
       <c r="X3">
-        <v>0.008299382560391951</v>
+        <v>0.02300702060247484</v>
       </c>
       <c r="Y3">
-        <v>0.006251137505423426</v>
+        <v>0.01732900590250509</v>
       </c>
       <c r="Z3">
-        <v>0.003900709803384218</v>
+        <v>0.01081329968316318</v>
       </c>
       <c r="AA3">
-        <v>0.008299382560391951</v>
+        <v>0.02300702060247484</v>
       </c>
       <c r="AB3">
-        <v>0.006250962039822307</v>
+        <v>0.01732851948792297</v>
       </c>
       <c r="AC3">
-        <v>0.00390060031284912</v>
+        <v>0.01081299616046393</v>
       </c>
       <c r="AD3">
-        <v>0.008299149601806636</v>
+        <v>0.02300637480949773</v>
       </c>
       <c r="AE3">
-        <v>0.008958363286135492</v>
+        <v>0.01403698896223623</v>
       </c>
       <c r="AF3">
-        <v>0.007220440808625207</v>
+        <v>0.0113138131035624</v>
       </c>
       <c r="AG3">
-        <v>0.0153626400183515</v>
+        <v>0.02407194277353702</v>
       </c>
       <c r="AH3">
-        <v>0.008958363286135492</v>
+        <v>0.01403698896223623</v>
       </c>
       <c r="AI3">
-        <v>0.007220440808625207</v>
+        <v>0.0113138131035624</v>
       </c>
       <c r="AJ3">
-        <v>0.0153626400183515</v>
+        <v>0.02407194277353702</v>
       </c>
       <c r="AK3">
-        <v>0.01101267627921935</v>
+        <v>0.01725592169446037</v>
       </c>
       <c r="AL3">
-        <v>0.008039253683830126</v>
+        <v>0.01259682283695607</v>
       </c>
       <c r="AM3">
-        <v>0.01710479507197899</v>
+        <v>0.02680175071692781</v>
       </c>
       <c r="AN3">
-        <v>0.006767589711753846</v>
+        <v>0.01876068186933465</v>
       </c>
       <c r="AO3">
-        <v>0.004095745293553428</v>
+        <v>0.01135396466732133</v>
       </c>
       <c r="AP3">
-        <v>0.008714351688411547</v>
+        <v>0.02415737163259857</v>
       </c>
       <c r="AQ3">
-        <v>0.006767589711753846</v>
+        <v>0.01876068186933465</v>
       </c>
       <c r="AR3">
-        <v>0.004095745293553428</v>
+        <v>0.01135396466732133</v>
       </c>
       <c r="AS3">
-        <v>0.008714351688411547</v>
+        <v>0.02415737163259857</v>
       </c>
       <c r="AT3">
-        <v>0.008958363286135492</v>
+        <v>0.01403698896223623</v>
       </c>
       <c r="AU3">
-        <v>0.007220440808625207</v>
+        <v>0.0113138131035624</v>
       </c>
       <c r="AV3">
-        <v>0.0153626400183515</v>
+        <v>0.02407194277353702</v>
       </c>
       <c r="AW3">
-        <v>0.008958363286135492</v>
+        <v>0.01403698896223623</v>
       </c>
       <c r="AX3">
-        <v>0.007220440808625207</v>
+        <v>0.0113138131035624</v>
       </c>
       <c r="AY3">
-        <v>0.0153626400183515</v>
+        <v>0.02407194277353702</v>
       </c>
     </row>
     <row r="4" spans="1:51">
       <c r="A4">
-        <v>0.007148783613695218</v>
+        <v>0.01813958512709789</v>
       </c>
       <c r="B4">
-        <v>0.004192046711070876</v>
+        <v>0.0106370527185302</v>
       </c>
       <c r="C4">
-        <v>0.008919248321427395</v>
+        <v>0.02263202706070255</v>
       </c>
       <c r="D4">
-        <v>0.007148783613695218</v>
+        <v>0.01813958512709789</v>
       </c>
       <c r="E4">
-        <v>0.004192046711070876</v>
+        <v>0.0106370527185302</v>
       </c>
       <c r="F4">
-        <v>0.008919248321427395</v>
+        <v>0.02263202706070255</v>
       </c>
       <c r="G4">
-        <v>0.007176254051528836</v>
+        <v>0.02440570488739656</v>
       </c>
       <c r="H4">
-        <v>0.00523866545761605</v>
+        <v>0.01781616456779949</v>
       </c>
       <c r="I4">
-        <v>0.01114609671833202</v>
+        <v>0.03790673312297763</v>
       </c>
       <c r="J4">
-        <v>0.001092257349477963</v>
+        <v>0.002771533766051759</v>
       </c>
       <c r="K4">
-        <v>0.0007842407769251773</v>
+        <v>0.001989961244025163</v>
       </c>
       <c r="L4">
-        <v>0.001668597397713143</v>
+        <v>0.004233960093670558</v>
       </c>
       <c r="M4">
-        <v>0.007176254051528836</v>
+        <v>0.02440570488739656</v>
       </c>
       <c r="N4">
-        <v>0.00523866545761605</v>
+        <v>0.01781616456779949</v>
       </c>
       <c r="O4">
-        <v>0.01114609671833202</v>
+        <v>0.03790673312297763</v>
       </c>
       <c r="P4">
-        <v>0.007176254051528836</v>
+        <v>0.02440570488739656</v>
       </c>
       <c r="Q4">
-        <v>0.00523866545761605</v>
+        <v>0.01781616456779949</v>
       </c>
       <c r="R4">
-        <v>0.01114609671833202</v>
+        <v>0.03790673312297763</v>
       </c>
       <c r="S4">
-        <v>0.007176254051528836</v>
+        <v>0.02440570488739656</v>
       </c>
       <c r="T4">
-        <v>0.00523866545761605</v>
+        <v>0.01781616456779949</v>
       </c>
       <c r="U4">
-        <v>0.01114609671833202</v>
+        <v>0.03790673312297763</v>
       </c>
       <c r="V4">
-        <v>0.006107294159485543</v>
+        <v>0.01549687167618037</v>
       </c>
       <c r="W4">
-        <v>0.003810951555518979</v>
+        <v>0.009670047925936547</v>
       </c>
       <c r="X4">
-        <v>0.008108407564933995</v>
+        <v>0.02057457005518414</v>
       </c>
       <c r="Y4">
-        <v>0.006107294159485543</v>
+        <v>0.01549687167618037</v>
       </c>
       <c r="Z4">
-        <v>0.003810951555518979</v>
+        <v>0.009670047925936547</v>
       </c>
       <c r="AA4">
-        <v>0.008108407564933995</v>
+        <v>0.02057457005518414</v>
       </c>
       <c r="AB4">
-        <v>0.006107122731479044</v>
+        <v>0.01549643668848385</v>
       </c>
       <c r="AC4">
-        <v>0.003810844584442924</v>
+        <v>0.00966977649361392</v>
       </c>
       <c r="AD4">
-        <v>0.008108179966899836</v>
+        <v>0.02057399253960408</v>
       </c>
       <c r="AE4">
-        <v>0.005837590173108594</v>
+        <v>0.01985304617080864</v>
       </c>
       <c r="AF4">
-        <v>0.004705097679525528</v>
+        <v>0.01600155521367176</v>
       </c>
       <c r="AG4">
-        <v>0.01001084612665006</v>
+        <v>0.03404586215674843</v>
       </c>
       <c r="AH4">
-        <v>0.005837590173108594</v>
+        <v>0.01985304617080864</v>
       </c>
       <c r="AI4">
-        <v>0.004705097679525528</v>
+        <v>0.01600155521367176</v>
       </c>
       <c r="AJ4">
-        <v>0.01001084612665006</v>
+        <v>0.03404586215674843</v>
       </c>
       <c r="AK4">
-        <v>0.007176254051528836</v>
+        <v>0.02440570488739656</v>
       </c>
       <c r="AL4">
-        <v>0.00523866545761605</v>
+        <v>0.01781616456779949</v>
       </c>
       <c r="AM4">
-        <v>0.01114609671833202</v>
+        <v>0.03790673312297763</v>
       </c>
       <c r="AN4">
-        <v>0.006611862414565312</v>
+        <v>0.0167771816295991</v>
       </c>
       <c r="AO4">
-        <v>0.004001499133294928</v>
+        <v>0.01015355032223337</v>
       </c>
       <c r="AP4">
-        <v>0.008513827943180695</v>
+        <v>0.02160329855794335</v>
       </c>
       <c r="AQ4">
-        <v>0.006611862414565312</v>
+        <v>0.0167771816295991</v>
       </c>
       <c r="AR4">
-        <v>0.004001499133294928</v>
+        <v>0.01015355032223337</v>
       </c>
       <c r="AS4">
-        <v>0.008513827943180695</v>
+        <v>0.02160329855794335</v>
       </c>
       <c r="AT4">
-        <v>0.005837590173108594</v>
+        <v>0.01985304617080864</v>
       </c>
       <c r="AU4">
-        <v>0.004705097679525528</v>
+        <v>0.01600155521367176</v>
       </c>
       <c r="AV4">
-        <v>0.01001084612665006</v>
+        <v>0.03404586215674843</v>
       </c>
       <c r="AW4">
-        <v>0.005837590173108594</v>
+        <v>0.01985304617080864</v>
       </c>
       <c r="AX4">
-        <v>0.004705097679525528</v>
+        <v>0.01600155521367176</v>
       </c>
       <c r="AY4">
-        <v>0.01001084612665006</v>
+        <v>0.03404586215674843</v>
       </c>
     </row>
     <row r="5" spans="1:51">
       <c r="A5">
-        <v>0.007148783613695218</v>
+        <v>0.01546179273763673</v>
       </c>
       <c r="B5">
-        <v>0.004192046711070876</v>
+        <v>0.009066795261350177</v>
       </c>
       <c r="C5">
-        <v>0.008919248321427395</v>
+        <v>0.01929105374755357</v>
       </c>
       <c r="D5">
-        <v>0.007148783613695218</v>
+        <v>0.01546179273763673</v>
       </c>
       <c r="E5">
-        <v>0.004192046711070876</v>
+        <v>0.009066795261350177</v>
       </c>
       <c r="F5">
-        <v>0.008919248321427395</v>
+        <v>0.01929105374755357</v>
       </c>
       <c r="G5">
-        <v>0.008861747252352734</v>
+        <v>0.02349023500221596</v>
       </c>
       <c r="H5">
-        <v>0.006469075494217495</v>
+        <v>0.01714787155161765</v>
       </c>
       <c r="I5">
-        <v>0.01376399041322871</v>
+        <v>0.03648483308854818</v>
       </c>
       <c r="J5">
-        <v>0.001092257349477963</v>
+        <v>0.002362395851713175</v>
       </c>
       <c r="K5">
-        <v>0.0007842407769251773</v>
+        <v>0.00169620022153006</v>
       </c>
       <c r="L5">
-        <v>0.001668597397713143</v>
+        <v>0.003608936641553318</v>
       </c>
       <c r="M5">
-        <v>0.008861747252352734</v>
+        <v>0.02349023500221596</v>
       </c>
       <c r="N5">
-        <v>0.006469075494217495</v>
+        <v>0.01714787155161765</v>
       </c>
       <c r="O5">
-        <v>0.01376399041322871</v>
+        <v>0.03648483308854818</v>
       </c>
       <c r="P5">
-        <v>0.008861747252352734</v>
+        <v>0.02349023500221596</v>
       </c>
       <c r="Q5">
-        <v>0.006469075494217495</v>
+        <v>0.01714787155161765</v>
       </c>
       <c r="R5">
-        <v>0.01376399041322871</v>
+        <v>0.03648483308854818</v>
       </c>
       <c r="S5">
-        <v>0.008861747252352734</v>
+        <v>0.02349023500221596</v>
       </c>
       <c r="T5">
-        <v>0.006469075494217495</v>
+        <v>0.01714787155161765</v>
       </c>
       <c r="U5">
-        <v>0.01376399041322871</v>
+        <v>0.03648483308854818</v>
       </c>
       <c r="V5">
-        <v>0.006107294159485543</v>
+        <v>0.0132092005555801</v>
       </c>
       <c r="W5">
-        <v>0.003810951555518979</v>
+        <v>0.00824254114668198</v>
       </c>
       <c r="X5">
-        <v>0.008108407564933995</v>
+        <v>0.01753732158868506</v>
       </c>
       <c r="Y5">
-        <v>0.006107294159485543</v>
+        <v>0.0132092005555801</v>
       </c>
       <c r="Z5">
-        <v>0.003810951555518979</v>
+        <v>0.00824254114668198</v>
       </c>
       <c r="AA5">
-        <v>0.008108407564933995</v>
+        <v>0.01753732158868506</v>
       </c>
       <c r="AB5">
-        <v>0.006107122731479044</v>
+        <v>0.01320882978141079</v>
       </c>
       <c r="AC5">
-        <v>0.003810844584442924</v>
+        <v>0.008242309783600335</v>
       </c>
       <c r="AD5">
-        <v>0.008108179966899836</v>
+        <v>0.01753682932680922</v>
       </c>
       <c r="AE5">
-        <v>0.007208670192756837</v>
+        <v>0.01910834873296241</v>
       </c>
       <c r="AF5">
-        <v>0.005810188175362011</v>
+        <v>0.01540132907876771</v>
       </c>
       <c r="AG5">
-        <v>0.01236210250077023</v>
+        <v>0.03276878527397384</v>
       </c>
       <c r="AH5">
-        <v>0.007208670192756837</v>
+        <v>0.01910834873296241</v>
       </c>
       <c r="AI5">
-        <v>0.005810188175362011</v>
+        <v>0.01540132907876771</v>
       </c>
       <c r="AJ5">
-        <v>0.01236210250077023</v>
+        <v>0.03276878527397384</v>
       </c>
       <c r="AK5">
-        <v>0.008861747252352734</v>
+        <v>0.02349023500221596</v>
       </c>
       <c r="AL5">
-        <v>0.006469075494217495</v>
+        <v>0.01714787155161765</v>
       </c>
       <c r="AM5">
-        <v>0.01376399041322871</v>
+        <v>0.03648483308854818</v>
       </c>
       <c r="AN5">
-        <v>0.006611862414565312</v>
+        <v>0.01430050925977541</v>
       </c>
       <c r="AO5">
-        <v>0.004001499133294928</v>
+        <v>0.008654668204016079</v>
       </c>
       <c r="AP5">
-        <v>0.008513827943180695</v>
+        <v>0.01841418766811931</v>
       </c>
       <c r="AQ5">
-        <v>0.006611862414565312</v>
+        <v>0.01430050925977541</v>
       </c>
       <c r="AR5">
-        <v>0.004001499133294928</v>
+        <v>0.008654668204016079</v>
       </c>
       <c r="AS5">
-        <v>0.008513827943180695</v>
+        <v>0.01841418766811931</v>
       </c>
       <c r="AT5">
-        <v>0.007208670192756837</v>
+        <v>0.01910834873296241</v>
       </c>
       <c r="AU5">
-        <v>0.005810188175362011</v>
+        <v>0.01540132907876771</v>
       </c>
       <c r="AV5">
-        <v>0.01236210250077023</v>
+        <v>0.03276878527397384</v>
       </c>
       <c r="AW5">
-        <v>0.007208670192756837</v>
+        <v>0.01910834873296241</v>
       </c>
       <c r="AX5">
-        <v>0.005810188175362011</v>
+        <v>0.01540132907876771</v>
       </c>
       <c r="AY5">
-        <v>0.01236210250077023</v>
+        <v>0.03276878527397384</v>
       </c>
     </row>
     <row r="6" spans="1:51">
       <c r="A6">
-        <v>0.004630180555808607</v>
+        <v>0.0200649905390628</v>
       </c>
       <c r="B6">
-        <v>0.002715137877926167</v>
+        <v>0.01176611045210643</v>
       </c>
       <c r="C6">
-        <v>0.005776889101970568</v>
+        <v>0.02503427755767324</v>
       </c>
       <c r="D6">
-        <v>0.004630180555808607</v>
+        <v>0.0200649905390628</v>
       </c>
       <c r="E6">
-        <v>0.002715137877926167</v>
+        <v>0.01176611045210643</v>
       </c>
       <c r="F6">
-        <v>0.005776889101970568</v>
+        <v>0.02503427755767324</v>
       </c>
       <c r="G6">
-        <v>0.005300762804602894</v>
+        <v>0.01897465115387807</v>
       </c>
       <c r="H6">
-        <v>0.003869556847360113</v>
+        <v>0.01385149534233099</v>
       </c>
       <c r="I6">
-        <v>0.008233099675234281</v>
+        <v>0.02947126668581062</v>
       </c>
       <c r="J6">
-        <v>0.0007074418551155107</v>
+        <v>0.003065715031786876</v>
       </c>
       <c r="K6">
-        <v>0.0005079432519729367</v>
+        <v>0.002201183392822977</v>
       </c>
       <c r="L6">
-        <v>0.001080730323346673</v>
+        <v>0.004683368920899949</v>
       </c>
       <c r="M6">
-        <v>0.005300762804602894</v>
+        <v>0.01897465115387807</v>
       </c>
       <c r="N6">
-        <v>0.003869556847360113</v>
+        <v>0.01385149534233099</v>
       </c>
       <c r="O6">
-        <v>0.008233099675234281</v>
+        <v>0.02947126668581062</v>
       </c>
       <c r="P6">
-        <v>0.005300762804602894</v>
+        <v>0.01897465115387807</v>
       </c>
       <c r="Q6">
-        <v>0.003869556847360113</v>
+        <v>0.01385149534233099</v>
       </c>
       <c r="R6">
-        <v>0.008233099675234281</v>
+        <v>0.02947126668581062</v>
       </c>
       <c r="S6">
-        <v>0.005300762804602894</v>
+        <v>0.01897465115387807</v>
       </c>
       <c r="T6">
-        <v>0.003869556847360113</v>
+        <v>0.01385149534233099</v>
       </c>
       <c r="U6">
-        <v>0.008233099675234281</v>
+        <v>0.02947126668581062</v>
       </c>
       <c r="V6">
-        <v>0.003955620451524137</v>
+        <v>0.01714176930668186</v>
       </c>
       <c r="W6">
-        <v>0.002468307161751061</v>
+        <v>0.01069646404736948</v>
       </c>
       <c r="X6">
-        <v>0.005251717365427789</v>
+        <v>0.02275843414333931</v>
       </c>
       <c r="Y6">
-        <v>0.003955620451524137</v>
+        <v>0.01714176930668186</v>
       </c>
       <c r="Z6">
-        <v>0.002468307161751061</v>
+        <v>0.01069646404736948</v>
       </c>
       <c r="AA6">
-        <v>0.005251717365427789</v>
+        <v>0.02275843414333931</v>
       </c>
       <c r="AB6">
-        <v>0.003955509419680777</v>
+        <v>0.01714128814771631</v>
       </c>
       <c r="AC6">
-        <v>0.002468237877880805</v>
+        <v>0.01069616380417497</v>
       </c>
       <c r="AD6">
-        <v>0.005251569952937882</v>
+        <v>0.02275779532803186</v>
       </c>
       <c r="AE6">
-        <v>0.004311954487109766</v>
+        <v>0.01543510532356983</v>
       </c>
       <c r="AF6">
-        <v>0.003475435316610472</v>
+        <v>0.01244069489079728</v>
       </c>
       <c r="AG6">
-        <v>0.007394543226830791</v>
+        <v>0.02646956359744102</v>
       </c>
       <c r="AH6">
-        <v>0.004311954487109766</v>
+        <v>0.01543510532356983</v>
       </c>
       <c r="AI6">
-        <v>0.003475435316610472</v>
+        <v>0.01244069489079728</v>
       </c>
       <c r="AJ6">
-        <v>0.007394543226830791</v>
+        <v>0.02646956359744102</v>
       </c>
       <c r="AK6">
-        <v>0.005300762804602894</v>
+        <v>0.01897465115387807</v>
       </c>
       <c r="AL6">
-        <v>0.003869556847360113</v>
+        <v>0.01385149534233099</v>
       </c>
       <c r="AM6">
-        <v>0.008233099675234281</v>
+        <v>0.02947126668581062</v>
       </c>
       <c r="AN6">
-        <v>0.004282423198675833</v>
+        <v>0.01855797628839714</v>
       </c>
       <c r="AO6">
-        <v>0.002591722519838614</v>
+        <v>0.01123128724973795</v>
       </c>
       <c r="AP6">
-        <v>0.005514303233699178</v>
+        <v>0.02389635585050628</v>
       </c>
       <c r="AQ6">
-        <v>0.004282423198675833</v>
+        <v>0.01855797628839714</v>
       </c>
       <c r="AR6">
-        <v>0.002591722519838614</v>
+        <v>0.01123128724973795</v>
       </c>
       <c r="AS6">
-        <v>0.005514303233699178</v>
+        <v>0.02389635585050628</v>
       </c>
       <c r="AT6">
-        <v>0.004311954487109766</v>
+        <v>0.01543510532356983</v>
       </c>
       <c r="AU6">
-        <v>0.003475435316610472</v>
+        <v>0.01244069489079728</v>
       </c>
       <c r="AV6">
-        <v>0.007394543226830791</v>
+        <v>0.02646956359744102</v>
       </c>
       <c r="AW6">
-        <v>0.004311954487109766</v>
+        <v>0.01543510532356983</v>
       </c>
       <c r="AX6">
-        <v>0.003475435316610472</v>
+        <v>0.01244069489079728</v>
       </c>
       <c r="AY6">
-        <v>0.007394543226830791</v>
+        <v>0.02646956359744102</v>
       </c>
     </row>
     <row r="7" spans="1:51">
       <c r="A7">
-        <v>0.004630180555808607</v>
+        <v>0.01741008771037907</v>
       </c>
       <c r="B7">
-        <v>0.002715137877926167</v>
+        <v>0.01020927543336629</v>
       </c>
       <c r="C7">
-        <v>0.005776889101970568</v>
+        <v>0.02172186262418358</v>
       </c>
       <c r="D7">
-        <v>0.004630180555808607</v>
+        <v>0.01741008771037907</v>
       </c>
       <c r="E7">
-        <v>0.002715137877926167</v>
+        <v>0.01020927543336629</v>
       </c>
       <c r="F7">
-        <v>0.005776889101970568</v>
+        <v>0.02172186262418358</v>
       </c>
       <c r="G7">
-        <v>0.005211675134796919</v>
+        <v>0.0200711055068446</v>
       </c>
       <c r="H7">
-        <v>0.003804522848401751</v>
+        <v>0.01465190701999656</v>
       </c>
       <c r="I7">
-        <v>0.008094729464684576</v>
+        <v>0.03117427025531182</v>
       </c>
       <c r="J7">
-        <v>0.0007074418551155107</v>
+        <v>0.002660074396473156</v>
       </c>
       <c r="K7">
-        <v>0.0005079432519729367</v>
+        <v>0.001909933416667726</v>
       </c>
       <c r="L7">
-        <v>0.001080730323346673</v>
+        <v>0.004063688120569628</v>
       </c>
       <c r="M7">
-        <v>0.005211675134796919</v>
+        <v>0.0200711055068446</v>
       </c>
       <c r="N7">
-        <v>0.003804522848401751</v>
+        <v>0.01465190701999656</v>
       </c>
       <c r="O7">
-        <v>0.008094729464684576</v>
+        <v>0.03117427025531182</v>
       </c>
       <c r="P7">
-        <v>0.005211675134796919</v>
+        <v>0.0200711055068446</v>
       </c>
       <c r="Q7">
-        <v>0.003804522848401751</v>
+        <v>0.01465190701999656</v>
       </c>
       <c r="R7">
-        <v>0.008094729464684576</v>
+        <v>0.03117427025531182</v>
       </c>
       <c r="S7">
-        <v>0.005211675134796919</v>
+        <v>0.0200711055068446</v>
       </c>
       <c r="T7">
-        <v>0.003804522848401751</v>
+        <v>0.01465190701999656</v>
       </c>
       <c r="U7">
-        <v>0.008094729464684576</v>
+        <v>0.03117427025531182</v>
       </c>
       <c r="V7">
-        <v>0.003955620451524137</v>
+        <v>0.01487365302063853</v>
       </c>
       <c r="W7">
-        <v>0.002468307161751061</v>
+        <v>0.009281159484878442</v>
       </c>
       <c r="X7">
-        <v>0.005251717365427789</v>
+        <v>0.01974714784016689</v>
       </c>
       <c r="Y7">
-        <v>0.003955620451524137</v>
+        <v>0.01487365302063853</v>
       </c>
       <c r="Z7">
-        <v>0.002468307161751061</v>
+        <v>0.009281159484878442</v>
       </c>
       <c r="AA7">
-        <v>0.005251717365427789</v>
+        <v>0.01974714784016689</v>
       </c>
       <c r="AB7">
-        <v>0.003955509419680777</v>
+        <v>0.01487323552630796</v>
       </c>
       <c r="AC7">
-        <v>0.002468237877880805</v>
+        <v>0.009280898968416171</v>
       </c>
       <c r="AD7">
-        <v>0.005251569952937882</v>
+        <v>0.01974659354982164</v>
       </c>
       <c r="AE7">
-        <v>0.004239485298857756</v>
+        <v>0.01632702624919201</v>
       </c>
       <c r="AF7">
-        <v>0.003417025150879351</v>
+        <v>0.01315958315684876</v>
       </c>
       <c r="AG7">
-        <v>0.007270266278466703</v>
+        <v>0.02799911309967821</v>
       </c>
       <c r="AH7">
-        <v>0.004239485298857756</v>
+        <v>0.01632702624919201</v>
       </c>
       <c r="AI7">
-        <v>0.003417025150879351</v>
+        <v>0.01315958315684876</v>
       </c>
       <c r="AJ7">
-        <v>0.007270266278466703</v>
+        <v>0.02799911309967821</v>
       </c>
       <c r="AK7">
-        <v>0.005211675134796919</v>
+        <v>0.0200711055068446</v>
       </c>
       <c r="AL7">
-        <v>0.003804522848401751</v>
+        <v>0.01465190701999656</v>
       </c>
       <c r="AM7">
-        <v>0.008094729464684576</v>
+        <v>0.03117427025531182</v>
       </c>
       <c r="AN7">
-        <v>0.004282423198675833</v>
+        <v>0.01610247432108784</v>
       </c>
       <c r="AO7">
-        <v>0.002591722519838614</v>
+        <v>0.009745217459122364</v>
       </c>
       <c r="AP7">
-        <v>0.005514303233699178</v>
+        <v>0.02073450523217524</v>
       </c>
       <c r="AQ7">
-        <v>0.004282423198675833</v>
+        <v>0.01610247432108784</v>
       </c>
       <c r="AR7">
-        <v>0.002591722519838614</v>
+        <v>0.009745217459122364</v>
       </c>
       <c r="AS7">
-        <v>0.005514303233699178</v>
+        <v>0.02073450523217524</v>
       </c>
       <c r="AT7">
-        <v>0.004239485298857756</v>
+        <v>0.01632702624919201</v>
       </c>
       <c r="AU7">
-        <v>0.003417025150879351</v>
+        <v>0.01315958315684876</v>
       </c>
       <c r="AV7">
-        <v>0.007270266278466703</v>
+        <v>0.02799911309967821</v>
       </c>
       <c r="AW7">
-        <v>0.004239485298857756</v>
+        <v>0.01632702624919201</v>
       </c>
       <c r="AX7">
-        <v>0.003417025150879351</v>
+        <v>0.01315958315684876</v>
       </c>
       <c r="AY7">
-        <v>0.007270266278466703</v>
+        <v>0.02799911309967821</v>
       </c>
     </row>
     <row r="8" spans="1:51">
       <c r="A8">
-        <v>0.002315090277904303</v>
+        <v>0.01429456824873684</v>
       </c>
       <c r="B8">
-        <v>0.001357568938963084</v>
+        <v>0.008382334821059285</v>
       </c>
       <c r="C8">
-        <v>0.002888444550985284</v>
+        <v>0.01783475493842401</v>
       </c>
       <c r="D8">
-        <v>0.002315090277904303</v>
+        <v>0.01429456824873684</v>
       </c>
       <c r="E8">
-        <v>0.001357568938963084</v>
+        <v>0.008382334821059285</v>
       </c>
       <c r="F8">
-        <v>0.002888444550985284</v>
+        <v>0.01783475493842401</v>
       </c>
       <c r="G8">
-        <v>0.003474450089864613</v>
+        <v>0.01786861076156478</v>
       </c>
       <c r="H8">
-        <v>0.002536348565601167</v>
+        <v>0.01304408585594229</v>
       </c>
       <c r="I8">
-        <v>0.005396486309789717</v>
+        <v>0.02775337416157934</v>
       </c>
       <c r="J8">
-        <v>0.0003537209275577553</v>
+        <v>0.002184056487230361</v>
       </c>
       <c r="K8">
-        <v>0.0002539716259864684</v>
+        <v>0.0015681525578314</v>
       </c>
       <c r="L8">
-        <v>0.0005403651616733367</v>
+        <v>0.003336494803896594</v>
       </c>
       <c r="M8">
-        <v>0.003474450089864613</v>
+        <v>0.01786861076156478</v>
       </c>
       <c r="N8">
-        <v>0.002536348565601167</v>
+        <v>0.01304408585594229</v>
       </c>
       <c r="O8">
-        <v>0.005396486309789717</v>
+        <v>0.02775337416157934</v>
       </c>
       <c r="P8">
-        <v>0.003474450089864613</v>
+        <v>0.01786861076156478</v>
       </c>
       <c r="Q8">
-        <v>0.002536348565601167</v>
+        <v>0.01304408585594229</v>
       </c>
       <c r="R8">
-        <v>0.005396486309789717</v>
+        <v>0.02775337416157934</v>
       </c>
       <c r="S8">
-        <v>0.003474450089864613</v>
+        <v>0.01786861076156478</v>
       </c>
       <c r="T8">
-        <v>0.002536348565601167</v>
+        <v>0.01304408585594229</v>
       </c>
       <c r="U8">
-        <v>0.005396486309789717</v>
+        <v>0.02775337416157934</v>
       </c>
       <c r="V8">
-        <v>0.001977810225762068</v>
+        <v>0.012212026254457</v>
       </c>
       <c r="W8">
-        <v>0.001234153580875531</v>
+        <v>0.007620304382781169</v>
       </c>
       <c r="X8">
-        <v>0.002625858682713895</v>
+        <v>0.01621341358038546</v>
       </c>
       <c r="Y8">
-        <v>0.001977810225762068</v>
+        <v>0.012212026254457</v>
       </c>
       <c r="Z8">
-        <v>0.001234153580875531</v>
+        <v>0.007620304382781169</v>
       </c>
       <c r="AA8">
-        <v>0.002625858682713895</v>
+        <v>0.01621341358038546</v>
       </c>
       <c r="AB8">
-        <v>0.001977754709840389</v>
+        <v>0.01221168347035959</v>
       </c>
       <c r="AC8">
-        <v>0.001234118938940402</v>
+        <v>0.007620090485504383</v>
       </c>
       <c r="AD8">
-        <v>0.002625784976468941</v>
+        <v>0.01621295847979656</v>
       </c>
       <c r="AE8">
-        <v>0.002826323532571837</v>
+        <v>0.01453538654565759</v>
       </c>
       <c r="AF8">
-        <v>0.002278016767252901</v>
+        <v>0.01171552155580002</v>
       </c>
       <c r="AG8">
-        <v>0.004846844185644469</v>
+        <v>0.02492664160808515</v>
       </c>
       <c r="AH8">
-        <v>0.002826323532571837</v>
+        <v>0.01453538654565759</v>
       </c>
       <c r="AI8">
-        <v>0.002278016767252901</v>
+        <v>0.01171552155580002</v>
       </c>
       <c r="AJ8">
-        <v>0.004846844185644469</v>
+        <v>0.02492664160808515</v>
       </c>
       <c r="AK8">
-        <v>0.003474450089864613</v>
+        <v>0.01786861076156478</v>
       </c>
       <c r="AL8">
-        <v>0.002536348565601167</v>
+        <v>0.01304408585594229</v>
       </c>
       <c r="AM8">
-        <v>0.005396486309789717</v>
+        <v>0.02775337416157934</v>
       </c>
       <c r="AN8">
-        <v>0.002141211599337917</v>
+        <v>0.01322095109372146</v>
       </c>
       <c r="AO8">
-        <v>0.001295861259919307</v>
+        <v>0.008001319601920227</v>
       </c>
       <c r="AP8">
-        <v>0.002757151616849589</v>
+        <v>0.01702408425940474</v>
       </c>
       <c r="AQ8">
-        <v>0.002141211599337917</v>
+        <v>0.01322095109372146</v>
       </c>
       <c r="AR8">
-        <v>0.001295861259919307</v>
+        <v>0.008001319601920227</v>
       </c>
       <c r="AS8">
-        <v>0.002757151616849589</v>
+        <v>0.01702408425940474</v>
       </c>
       <c r="AT8">
-        <v>0.002826323532571837</v>
+        <v>0.01453538654565759</v>
       </c>
       <c r="AU8">
-        <v>0.002278016767252901</v>
+        <v>0.01171552155580002</v>
       </c>
       <c r="AV8">
-        <v>0.004846844185644469</v>
+        <v>0.02492664160808515</v>
       </c>
       <c r="AW8">
-        <v>0.002826323532571837</v>
+        <v>0.01453538654565759</v>
       </c>
       <c r="AX8">
-        <v>0.002278016767252901</v>
+        <v>0.01171552155580002</v>
       </c>
       <c r="AY8">
-        <v>0.004846844185644469</v>
+        <v>0.02492664160808515</v>
       </c>
     </row>
     <row r="9" spans="1:51">
       <c r="A9">
-        <v>0.002315090277904303</v>
+        <v>0.0146407370778082</v>
       </c>
       <c r="B9">
-        <v>0.001357568938963084</v>
+        <v>0.00858532822242673</v>
       </c>
       <c r="C9">
-        <v>0.002888444550985284</v>
+        <v>0.01826665579239729</v>
       </c>
       <c r="D9">
-        <v>0.002315090277904303</v>
+        <v>0.0146407370778082</v>
       </c>
       <c r="E9">
-        <v>0.001357568938963084</v>
+        <v>0.00858532822242673</v>
       </c>
       <c r="F9">
-        <v>0.002888444550985284</v>
+        <v>0.01826665579239729</v>
       </c>
       <c r="G9">
-        <v>0.001737225044932306</v>
+        <v>0.01844896179112502</v>
       </c>
       <c r="H9">
-        <v>0.001268174282800584</v>
+        <v>0.01346774210752127</v>
       </c>
       <c r="I9">
-        <v>0.002698243154894859</v>
+        <v>0.0286547704415346</v>
       </c>
       <c r="J9">
-        <v>0.0003537209275577553</v>
+        <v>0.002236947366035116</v>
       </c>
       <c r="K9">
-        <v>0.0002539716259864684</v>
+        <v>0.001606128208813214</v>
       </c>
       <c r="L9">
-        <v>0.0005403651616733367</v>
+        <v>0.003417294061304709</v>
       </c>
       <c r="M9">
-        <v>0.001737225044932306</v>
+        <v>0.01844896179112502</v>
       </c>
       <c r="N9">
-        <v>0.001268174282800584</v>
+        <v>0.01346774210752127</v>
       </c>
       <c r="O9">
-        <v>0.002698243154894859</v>
+        <v>0.0286547704415346</v>
       </c>
       <c r="P9">
-        <v>0.001737225044932306</v>
+        <v>0.01844896179112502</v>
       </c>
       <c r="Q9">
-        <v>0.001268174282800584</v>
+        <v>0.01346774210752127</v>
       </c>
       <c r="R9">
-        <v>0.002698243154894859</v>
+        <v>0.0286547704415346</v>
       </c>
       <c r="S9">
-        <v>0.001737225044932306</v>
+        <v>0.01844896179112502</v>
       </c>
       <c r="T9">
-        <v>0.001268174282800584</v>
+        <v>0.01346774210752127</v>
       </c>
       <c r="U9">
-        <v>0.002698243154894859</v>
+        <v>0.0286547704415346</v>
       </c>
       <c r="V9">
-        <v>0.001977810225762068</v>
+        <v>0.0125077625618105</v>
       </c>
       <c r="W9">
-        <v>0.001234153580875531</v>
+        <v>0.007804843838569755</v>
       </c>
       <c r="X9">
-        <v>0.002625858682713895</v>
+        <v>0.01660605072036118</v>
       </c>
       <c r="Y9">
-        <v>0.001977810225762068</v>
+        <v>0.0125077625618105</v>
       </c>
       <c r="Z9">
-        <v>0.001234153580875531</v>
+        <v>0.007804843838569755</v>
       </c>
       <c r="AA9">
-        <v>0.002625858682713895</v>
+        <v>0.01660605072036118</v>
       </c>
       <c r="AB9">
-        <v>0.001977754709840389</v>
+        <v>0.01250741147657607</v>
       </c>
       <c r="AC9">
-        <v>0.001234118938940402</v>
+        <v>0.00780462476138347</v>
       </c>
       <c r="AD9">
-        <v>0.002625784976468941</v>
+        <v>0.01660558459868823</v>
       </c>
       <c r="AE9">
-        <v>0.001413161766285918</v>
+        <v>0.01500747845360678</v>
       </c>
       <c r="AF9">
-        <v>0.00113900838362645</v>
+        <v>0.01209602763360706</v>
       </c>
       <c r="AG9">
-        <v>0.002423422092822234</v>
+        <v>0.0257362290076746</v>
       </c>
       <c r="AH9">
-        <v>0.001413161766285918</v>
+        <v>0.01500747845360678</v>
       </c>
       <c r="AI9">
-        <v>0.00113900838362645</v>
+        <v>0.01209602763360706</v>
       </c>
       <c r="AJ9">
-        <v>0.002423422092822234</v>
+        <v>0.0257362290076746</v>
       </c>
       <c r="AK9">
-        <v>0.001737225044932306</v>
+        <v>0.01844896179112502</v>
       </c>
       <c r="AL9">
-        <v>0.001268174282800584</v>
+        <v>0.01346774210752127</v>
       </c>
       <c r="AM9">
-        <v>0.002698243154894859</v>
+        <v>0.0286547704415346</v>
       </c>
       <c r="AN9">
-        <v>0.002141211599337917</v>
+        <v>0.01354112034120661</v>
       </c>
       <c r="AO9">
-        <v>0.001295861259919307</v>
+        <v>0.008195086030498242</v>
       </c>
       <c r="AP9">
-        <v>0.002757151616849589</v>
+        <v>0.01743635325637924</v>
       </c>
       <c r="AQ9">
-        <v>0.002141211599337917</v>
+        <v>0.01354112034120661</v>
       </c>
       <c r="AR9">
-        <v>0.001295861259919307</v>
+        <v>0.008195086030498242</v>
       </c>
       <c r="AS9">
-        <v>0.002757151616849589</v>
+        <v>0.01743635325637924</v>
       </c>
       <c r="AT9">
-        <v>0.001413161766285918</v>
+        <v>0.01500747845360678</v>
       </c>
       <c r="AU9">
-        <v>0.00113900838362645</v>
+        <v>0.01209602763360706</v>
       </c>
       <c r="AV9">
-        <v>0.002423422092822234</v>
+        <v>0.0257362290076746</v>
       </c>
       <c r="AW9">
-        <v>0.001413161766285918</v>
+        <v>0.01500747845360678</v>
       </c>
       <c r="AX9">
-        <v>0.00113900838362645</v>
+        <v>0.01209602763360706</v>
       </c>
       <c r="AY9">
-        <v>0.002423422092822234</v>
+        <v>0.0257362290076746</v>
       </c>
     </row>
     <row r="10" spans="1:51">
       <c r="A10">
-        <v>0.06600898496669169</v>
+        <v>0.1354320786390941</v>
       </c>
       <c r="B10">
-        <v>0.03870766878446801</v>
+        <v>0.07941737091396478</v>
       </c>
       <c r="C10">
-        <v>0.08235674209461277</v>
+        <v>0.1689731296041803</v>
       </c>
       <c r="D10">
-        <v>0.06600898496669169</v>
+        <v>0.1354320786390941</v>
       </c>
       <c r="E10">
-        <v>0.03870766878446801</v>
+        <v>0.07941737091396478</v>
       </c>
       <c r="F10">
-        <v>0.08235674209461277</v>
+        <v>0.1689731296041803</v>
       </c>
       <c r="G10">
-        <v>0.02505837176621392</v>
+        <v>0.06244974959713444</v>
       </c>
       <c r="H10">
-        <v>0.01829261138933616</v>
+        <v>0.04558831720590814</v>
       </c>
       <c r="I10">
-        <v>0.03892044976454501</v>
+        <v>0.09699641958703858</v>
       </c>
       <c r="J10">
-        <v>0.01008546388553805</v>
+        <v>0.02069256690959826</v>
       </c>
       <c r="K10">
-        <v>0.007241363069816324</v>
+        <v>0.01485726304109155</v>
       </c>
       <c r="L10">
-        <v>0.0154071554676943</v>
+        <v>0.03161119795976924</v>
       </c>
       <c r="M10">
-        <v>0.02505837176621392</v>
+        <v>0.06244974959713444</v>
       </c>
       <c r="N10">
-        <v>0.01829261138933616</v>
+        <v>0.04558831720590814</v>
       </c>
       <c r="O10">
-        <v>0.03892044976454501</v>
+        <v>0.09699641958703858</v>
       </c>
       <c r="P10">
-        <v>0.02505837176621392</v>
+        <v>0.06244974959713444</v>
       </c>
       <c r="Q10">
-        <v>0.01829261138933616</v>
+        <v>0.04558831720590814</v>
       </c>
       <c r="R10">
-        <v>0.03892044976454501</v>
+        <v>0.09699641958703858</v>
       </c>
       <c r="S10">
-        <v>0.02505837176621392</v>
+        <v>0.06244974959713444</v>
       </c>
       <c r="T10">
-        <v>0.01829261138933616</v>
+        <v>0.04558831720590814</v>
       </c>
       <c r="U10">
-        <v>0.03892044976454501</v>
+        <v>0.09699641958703858</v>
       </c>
       <c r="V10">
-        <v>0.05639229135266319</v>
+        <v>0.1157012979515804</v>
       </c>
       <c r="W10">
-        <v>0.03518878980406183</v>
+        <v>0.07219760992178617</v>
       </c>
       <c r="X10">
-        <v>0.07486976554055706</v>
+        <v>0.1536119360038003</v>
       </c>
       <c r="Y10">
-        <v>0.05639229135266319</v>
+        <v>0.1157012979515804</v>
       </c>
       <c r="Z10">
-        <v>0.03518878980406183</v>
+        <v>0.07219760992178617</v>
       </c>
       <c r="AA10">
-        <v>0.07486976554055706</v>
+        <v>0.1536119360038003</v>
       </c>
       <c r="AB10">
-        <v>0.05639070845558373</v>
+        <v>0.1156980502870109</v>
       </c>
       <c r="AC10">
-        <v>0.03518780207628425</v>
+        <v>0.07219558337909482</v>
       </c>
       <c r="AD10">
-        <v>0.07486766399209413</v>
+        <v>0.15360762421084</v>
       </c>
       <c r="AE10">
-        <v>0.02038396407459801</v>
+        <v>0.05080032590034337</v>
       </c>
       <c r="AF10">
-        <v>0.016429475044126</v>
+        <v>0.04094506267567676</v>
       </c>
       <c r="AG10">
-        <v>0.03495632988111914</v>
+        <v>0.08711715462909948</v>
       </c>
       <c r="AH10">
-        <v>0.02038396407459801</v>
+        <v>0.05080032590034337</v>
       </c>
       <c r="AI10">
-        <v>0.016429475044126</v>
+        <v>0.04094506267567676</v>
       </c>
       <c r="AJ10">
-        <v>0.03495632988111914</v>
+        <v>0.08711715462909948</v>
       </c>
       <c r="AK10">
-        <v>0.02505837176621392</v>
+        <v>0.06244974959713444</v>
       </c>
       <c r="AL10">
-        <v>0.01829261138933616</v>
+        <v>0.04558831720590814</v>
       </c>
       <c r="AM10">
-        <v>0.03892044976454501</v>
+        <v>0.09699641958703858</v>
       </c>
       <c r="AN10">
-        <v>0.0610512711405567</v>
+        <v>0.1252602287142688</v>
       </c>
       <c r="AO10">
-        <v>0.03694822929426492</v>
+        <v>0.07580749041787546</v>
       </c>
       <c r="AP10">
-        <v>0.07861325381758491</v>
+        <v>0.1612925328039903</v>
       </c>
       <c r="AQ10">
-        <v>0.0610512711405567</v>
+        <v>0.1252602287142688</v>
       </c>
       <c r="AR10">
-        <v>0.03694822929426492</v>
+        <v>0.07580749041787546</v>
       </c>
       <c r="AS10">
-        <v>0.07861325381758491</v>
+        <v>0.1612925328039903</v>
       </c>
       <c r="AT10">
-        <v>0.02038396407459801</v>
+        <v>0.05080032590034337</v>
       </c>
       <c r="AU10">
-        <v>0.016429475044126</v>
+        <v>0.04094506267567676</v>
       </c>
       <c r="AV10">
-        <v>0.03495632988111914</v>
+        <v>0.08711715462909948</v>
       </c>
       <c r="AW10">
-        <v>0.02038396407459801</v>
+        <v>0.05080032590034337</v>
       </c>
       <c r="AX10">
-        <v>0.016429475044126</v>
+        <v>0.04094506267567676</v>
       </c>
       <c r="AY10">
-        <v>0.03495632988111914</v>
+        <v>0.08711715462909948</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
get stubble sim working (slight change in profit due to sgen changes)
</commit_message>
<xml_diff>
--- a/stubble sim.xlsx
+++ b/stubble sim.xlsx
@@ -348,1552 +348,1552 @@
   <sheetData>
     <row r="1" spans="1:51">
       <c r="A1">
-        <v>0.05630272974597433</v>
+        <v>0.05988132675614952</v>
       </c>
       <c r="B1">
-        <v>0.03301592072303935</v>
+        <v>0.03511441000980608</v>
       </c>
       <c r="C1">
-        <v>0.07024663983625393</v>
+        <v>0.07471151065916186</v>
       </c>
       <c r="D1">
-        <v>0.05630272974597433</v>
+        <v>0.05988132675614952</v>
       </c>
       <c r="E1">
-        <v>0.03301592072303935</v>
+        <v>0.03511441000980608</v>
       </c>
       <c r="F1">
-        <v>0.07024663983625393</v>
+        <v>0.07471151065916186</v>
       </c>
       <c r="G1">
-        <v>0.04939719860297297</v>
+        <v>0.0521744500435975</v>
       </c>
       <c r="H1">
-        <v>0.03605995498017027</v>
+        <v>0.03808734853182617</v>
       </c>
       <c r="I1">
-        <v>0.07672330846844737</v>
+        <v>0.08103691176984291</v>
       </c>
       <c r="J1">
-        <v>0.00860245234488557</v>
+        <v>0.00914922352952397</v>
       </c>
       <c r="K1">
-        <v>0.00617656078362784</v>
+        <v>0.00656914249419821</v>
       </c>
       <c r="L1">
-        <v>0.01314161868856987</v>
+        <v>0.01397689892382598</v>
       </c>
       <c r="M1">
-        <v>0.04939719860297297</v>
+        <v>0.0521744500435975</v>
       </c>
       <c r="N1">
-        <v>0.03605995498017027</v>
+        <v>0.03808734853182617</v>
       </c>
       <c r="O1">
-        <v>0.07672330846844737</v>
+        <v>0.08103691176984291</v>
       </c>
       <c r="P1">
-        <v>0.04939719860297297</v>
+        <v>0.0521744500435975</v>
       </c>
       <c r="Q1">
-        <v>0.03605995498017027</v>
+        <v>0.03808734853182617</v>
       </c>
       <c r="R1">
-        <v>0.07672330846844737</v>
+        <v>0.08103691176984291</v>
       </c>
       <c r="S1">
-        <v>0.04939719860297297</v>
+        <v>0.0521744500435975</v>
       </c>
       <c r="T1">
-        <v>0.03605995498017027</v>
+        <v>0.03808734853182617</v>
       </c>
       <c r="U1">
-        <v>0.07672330846844737</v>
+        <v>0.08103691176984291</v>
       </c>
       <c r="V1">
-        <v>0.04810011760349556</v>
+        <v>0.05115735724039348</v>
       </c>
       <c r="W1">
-        <v>0.03001447338458123</v>
+        <v>0.03192219091800553</v>
       </c>
       <c r="X1">
-        <v>0.06386058166932175</v>
+        <v>0.06791955514469261</v>
       </c>
       <c r="Y1">
-        <v>0.04810011760349556</v>
+        <v>0.05115735724039348</v>
       </c>
       <c r="Z1">
-        <v>0.03001447338458123</v>
+        <v>0.03192219091800553</v>
       </c>
       <c r="AA1">
-        <v>0.06386058166932175</v>
+        <v>0.06791955514469261</v>
       </c>
       <c r="AB1">
-        <v>0.0480987674626545</v>
+        <v>0.05115592128470829</v>
       </c>
       <c r="AC1">
-        <v>0.03001363089669641</v>
+        <v>0.03192129488165797</v>
       </c>
       <c r="AD1">
-        <v>0.06385878914190724</v>
+        <v>0.06791764868437865</v>
       </c>
       <c r="AE1">
-        <v>0.04018260767710363</v>
+        <v>0.04244178852572304</v>
       </c>
       <c r="AF1">
-        <v>0.03238718178774552</v>
+        <v>0.03420808155173277</v>
       </c>
       <c r="AG1">
-        <v>0.06890889742073515</v>
+        <v>0.0727831522377293</v>
       </c>
       <c r="AH1">
-        <v>0.04018260767710363</v>
+        <v>0.04244178852572304</v>
       </c>
       <c r="AI1">
-        <v>0.03238718178774552</v>
+        <v>0.03420808155173277</v>
       </c>
       <c r="AJ1">
-        <v>0.06890889742073515</v>
+        <v>0.0727831522377293</v>
       </c>
       <c r="AK1">
-        <v>0.04939719860297297</v>
+        <v>0.0521744500435975</v>
       </c>
       <c r="AL1">
-        <v>0.03605995498017027</v>
+        <v>0.03808734853182617</v>
       </c>
       <c r="AM1">
-        <v>0.07672330846844737</v>
+        <v>0.08103691176984291</v>
       </c>
       <c r="AN1">
-        <v>0.05207402024753847</v>
+        <v>0.05538384081940814</v>
       </c>
       <c r="AO1">
-        <v>0.03151519705381028</v>
+        <v>0.0335183004639058</v>
       </c>
       <c r="AP1">
-        <v>0.06705361075278783</v>
+        <v>0.07131553290192723</v>
       </c>
       <c r="AQ1">
-        <v>0.05207402024753847</v>
+        <v>0.05538384081940814</v>
       </c>
       <c r="AR1">
-        <v>0.03151519705381028</v>
+        <v>0.0335183004639058</v>
       </c>
       <c r="AS1">
-        <v>0.06705361075278783</v>
+        <v>0.07131553290192723</v>
       </c>
       <c r="AT1">
-        <v>0.04018260767710363</v>
+        <v>0.04244178852572304</v>
       </c>
       <c r="AU1">
-        <v>0.03238718178774552</v>
+        <v>0.03420808155173277</v>
       </c>
       <c r="AV1">
-        <v>0.06890889742073515</v>
+        <v>0.0727831522377293</v>
       </c>
       <c r="AW1">
-        <v>0.04018260767710363</v>
+        <v>0.04244178852572304</v>
       </c>
       <c r="AX1">
-        <v>0.03238718178774552</v>
+        <v>0.03420808155173277</v>
       </c>
       <c r="AY1">
-        <v>0.06890889742073515</v>
+        <v>0.0727831522377293</v>
       </c>
     </row>
     <row r="2" spans="1:51">
       <c r="A2">
-        <v>0.01233679495482404</v>
+        <v>0.0126434043002024</v>
       </c>
       <c r="B2">
-        <v>0.007234296561508821</v>
+        <v>0.00741409228163869</v>
       </c>
       <c r="C2">
-        <v>0.01539212034363579</v>
+        <v>0.01577466442901848</v>
       </c>
       <c r="D2">
-        <v>0.01233679495482404</v>
+        <v>0.0126434043002024</v>
       </c>
       <c r="E2">
-        <v>0.007234296561508821</v>
+        <v>0.00741409228163869</v>
       </c>
       <c r="F2">
-        <v>0.01539212034363579</v>
+        <v>0.01577466442901848</v>
       </c>
       <c r="G2">
-        <v>0.0186693753286726</v>
+        <v>0.01893955208721895</v>
       </c>
       <c r="H2">
-        <v>0.013628643989931</v>
+        <v>0.01382587302366983</v>
       </c>
       <c r="I2">
-        <v>0.02899711487219362</v>
+        <v>0.02941675111419113</v>
       </c>
       <c r="J2">
-        <v>0.001884929756804317</v>
+        <v>0.001931776371418104</v>
       </c>
       <c r="K2">
-        <v>0.0013533795653855</v>
+        <v>0.001387015434678199</v>
       </c>
       <c r="L2">
-        <v>0.002879530990181913</v>
+        <v>0.002951096669528083</v>
       </c>
       <c r="M2">
-        <v>0.0186693753286726</v>
+        <v>0.01893955208721895</v>
       </c>
       <c r="N2">
-        <v>0.013628643989931</v>
+        <v>0.01382587302366983</v>
       </c>
       <c r="O2">
-        <v>0.02899711487219362</v>
+        <v>0.02941675111419113</v>
       </c>
       <c r="P2">
-        <v>0.0186693753286726</v>
+        <v>0.01893955208721895</v>
       </c>
       <c r="Q2">
-        <v>0.013628643989931</v>
+        <v>0.01382587302366983</v>
       </c>
       <c r="R2">
-        <v>0.02899711487219362</v>
+        <v>0.02941675111419113</v>
       </c>
       <c r="S2">
-        <v>0.0186693753286726</v>
+        <v>0.01893955208721895</v>
       </c>
       <c r="T2">
-        <v>0.013628643989931</v>
+        <v>0.01382587302366983</v>
       </c>
       <c r="U2">
-        <v>0.02899711487219362</v>
+        <v>0.02941675111419113</v>
       </c>
       <c r="V2">
-        <v>0.01053947634252451</v>
+        <v>0.01080141649422886</v>
       </c>
       <c r="W2">
-        <v>0.006576633237735292</v>
+        <v>0.006740083892398809</v>
       </c>
       <c r="X2">
-        <v>0.01399283667603253</v>
+        <v>0.01434060402638044</v>
       </c>
       <c r="Y2">
-        <v>0.01053947634252451</v>
+        <v>0.01080141649422886</v>
       </c>
       <c r="Z2">
-        <v>0.006576633237735292</v>
+        <v>0.006740083892398809</v>
       </c>
       <c r="AA2">
-        <v>0.01399283667603253</v>
+        <v>0.01434060402638044</v>
       </c>
       <c r="AB2">
-        <v>0.01053918050587873</v>
+        <v>0.01080111330508345</v>
       </c>
       <c r="AC2">
-        <v>0.006576448635668326</v>
+        <v>0.006739894702372076</v>
       </c>
       <c r="AD2">
-        <v>0.01399244390567729</v>
+        <v>0.01434020149440867</v>
       </c>
       <c r="AE2">
-        <v>0.0151867758825396</v>
+        <v>0.01540655366344975</v>
       </c>
       <c r="AF2">
-        <v>0.01224054136132692</v>
+        <v>0.0124176822527405</v>
       </c>
       <c r="AG2">
-        <v>0.02604370502409983</v>
+        <v>0.02642060053774574</v>
       </c>
       <c r="AH2">
-        <v>0.0151867758825396</v>
+        <v>0.01540655366344975</v>
       </c>
       <c r="AI2">
-        <v>0.01224054136132692</v>
+        <v>0.0124176822527405</v>
       </c>
       <c r="AJ2">
-        <v>0.02604370502409983</v>
+        <v>0.02642060053774574</v>
       </c>
       <c r="AK2">
-        <v>0.0186693753286726</v>
+        <v>0.01893955208721895</v>
       </c>
       <c r="AL2">
-        <v>0.013628643989931</v>
+        <v>0.01382587302366983</v>
       </c>
       <c r="AM2">
-        <v>0.02899711487219362</v>
+        <v>0.02941675111419113</v>
       </c>
       <c r="AN2">
-        <v>0.011410219596203</v>
+        <v>0.01169380054034823</v>
       </c>
       <c r="AO2">
-        <v>0.006905464899622056</v>
+        <v>0.007077088087018749</v>
       </c>
       <c r="AP2">
-        <v>0.01469247850983416</v>
+        <v>0.01505763422769946</v>
       </c>
       <c r="AQ2">
-        <v>0.011410219596203</v>
+        <v>0.01169380054034823</v>
       </c>
       <c r="AR2">
-        <v>0.006905464899622056</v>
+        <v>0.007077088087018749</v>
       </c>
       <c r="AS2">
-        <v>0.01469247850983416</v>
+        <v>0.01505763422769946</v>
       </c>
       <c r="AT2">
-        <v>0.0151867758825396</v>
+        <v>0.01540655366344975</v>
       </c>
       <c r="AU2">
-        <v>0.01224054136132692</v>
+        <v>0.0124176822527405</v>
       </c>
       <c r="AV2">
-        <v>0.02604370502409983</v>
+        <v>0.02642060053774574</v>
       </c>
       <c r="AW2">
-        <v>0.0151867758825396</v>
+        <v>0.01540655366344975</v>
       </c>
       <c r="AX2">
-        <v>0.01224054136132692</v>
+        <v>0.0124176822527405</v>
       </c>
       <c r="AY2">
-        <v>0.02604370502409983</v>
+        <v>0.02642060053774574</v>
       </c>
     </row>
     <row r="3" spans="1:51">
       <c r="A3">
-        <v>0.02028415697728426</v>
+        <v>0.02064126044938914</v>
       </c>
       <c r="B3">
-        <v>0.01189462965147949</v>
+        <v>0.01210403512752179</v>
       </c>
       <c r="C3">
-        <v>0.02530772266272232</v>
+        <v>0.02575326622876977</v>
       </c>
       <c r="D3">
-        <v>0.02028415697728426</v>
+        <v>0.02064126044938914</v>
       </c>
       <c r="E3">
-        <v>0.01189462965147949</v>
+        <v>0.01210403512752179</v>
       </c>
       <c r="F3">
-        <v>0.02530772266272232</v>
+        <v>0.02575326622876977</v>
       </c>
       <c r="G3">
-        <v>0.01725592169446037</v>
+        <v>0.02039971166164056</v>
       </c>
       <c r="H3">
-        <v>0.01259682283695607</v>
+        <v>0.01489178951299761</v>
       </c>
       <c r="I3">
-        <v>0.02680175071692781</v>
+        <v>0.03168465853829278</v>
       </c>
       <c r="J3">
-        <v>0.003099201309431047</v>
+        <v>0.003153762884239861</v>
       </c>
       <c r="K3">
-        <v>0.002225226540171492</v>
+        <v>0.00226440175088422</v>
       </c>
       <c r="L3">
-        <v>0.004734524553556364</v>
+        <v>0.004817876065711105</v>
       </c>
       <c r="M3">
-        <v>0.01725592169446037</v>
+        <v>0.02039971166164056</v>
       </c>
       <c r="N3">
-        <v>0.01259682283695607</v>
+        <v>0.01489178951299761</v>
       </c>
       <c r="O3">
-        <v>0.02680175071692781</v>
+        <v>0.03168465853829278</v>
       </c>
       <c r="P3">
-        <v>0.01725592169446037</v>
+        <v>0.02039971166164056</v>
       </c>
       <c r="Q3">
-        <v>0.01259682283695607</v>
+        <v>0.01489178951299761</v>
       </c>
       <c r="R3">
-        <v>0.02680175071692781</v>
+        <v>0.03168465853829278</v>
       </c>
       <c r="S3">
-        <v>0.01725592169446037</v>
+        <v>0.02039971166164056</v>
       </c>
       <c r="T3">
-        <v>0.01259682283695607</v>
+        <v>0.01489178951299761</v>
       </c>
       <c r="U3">
-        <v>0.02680175071692781</v>
+        <v>0.03168465853829278</v>
       </c>
       <c r="V3">
-        <v>0.01732900590250509</v>
+        <v>0.01763408381049212</v>
       </c>
       <c r="W3">
-        <v>0.01081329968316318</v>
+        <v>0.01100366829774709</v>
       </c>
       <c r="X3">
-        <v>0.02300702060247484</v>
+        <v>0.02341206020797252</v>
       </c>
       <c r="Y3">
-        <v>0.01732900590250509</v>
+        <v>0.01763408381049212</v>
       </c>
       <c r="Z3">
-        <v>0.01081329968316318</v>
+        <v>0.01100366829774709</v>
       </c>
       <c r="AA3">
-        <v>0.02300702060247484</v>
+        <v>0.02341206020797252</v>
       </c>
       <c r="AB3">
-        <v>0.01732851948792297</v>
+        <v>0.01763358883255998</v>
       </c>
       <c r="AC3">
-        <v>0.01081299616046393</v>
+        <v>0.01100335943151743</v>
       </c>
       <c r="AD3">
-        <v>0.02300637480949773</v>
+        <v>0.02341140304578176</v>
       </c>
       <c r="AE3">
-        <v>0.01403698896223623</v>
+        <v>0.01659433396242037</v>
       </c>
       <c r="AF3">
-        <v>0.0113138131035624</v>
+        <v>0.01337503317371082</v>
       </c>
       <c r="AG3">
-        <v>0.02407194277353702</v>
+        <v>0.02845751739087408</v>
       </c>
       <c r="AH3">
-        <v>0.01403698896223623</v>
+        <v>0.01659433396242037</v>
       </c>
       <c r="AI3">
-        <v>0.0113138131035624</v>
+        <v>0.01337503317371082</v>
       </c>
       <c r="AJ3">
-        <v>0.02407194277353702</v>
+        <v>0.02845751739087408</v>
       </c>
       <c r="AK3">
-        <v>0.01725592169446037</v>
+        <v>0.02039971166164056</v>
       </c>
       <c r="AL3">
-        <v>0.01259682283695607</v>
+        <v>0.01489178951299761</v>
       </c>
       <c r="AM3">
-        <v>0.02680175071692781</v>
+        <v>0.03168465853829278</v>
       </c>
       <c r="AN3">
-        <v>0.01876068186933465</v>
+        <v>0.01909096449543033</v>
       </c>
       <c r="AO3">
-        <v>0.01135396466732133</v>
+        <v>0.01155385171263444</v>
       </c>
       <c r="AP3">
-        <v>0.02415737163259857</v>
+        <v>0.02458266321837114</v>
       </c>
       <c r="AQ3">
-        <v>0.01876068186933465</v>
+        <v>0.01909096449543033</v>
       </c>
       <c r="AR3">
-        <v>0.01135396466732133</v>
+        <v>0.01155385171263444</v>
       </c>
       <c r="AS3">
-        <v>0.02415737163259857</v>
+        <v>0.02458266321837114</v>
       </c>
       <c r="AT3">
-        <v>0.01403698896223623</v>
+        <v>0.01659433396242037</v>
       </c>
       <c r="AU3">
-        <v>0.0113138131035624</v>
+        <v>0.01337503317371082</v>
       </c>
       <c r="AV3">
-        <v>0.02407194277353702</v>
+        <v>0.02845751739087408</v>
       </c>
       <c r="AW3">
-        <v>0.01403698896223623</v>
+        <v>0.01659433396242037</v>
       </c>
       <c r="AX3">
-        <v>0.0113138131035624</v>
+        <v>0.01337503317371082</v>
       </c>
       <c r="AY3">
-        <v>0.02407194277353702</v>
+        <v>0.02845751739087408</v>
       </c>
     </row>
     <row r="4" spans="1:51">
       <c r="A4">
-        <v>0.01813958512709789</v>
+        <v>0.01843537451228727</v>
       </c>
       <c r="B4">
-        <v>0.0106370527185302</v>
+        <v>0.01081050361400525</v>
       </c>
       <c r="C4">
-        <v>0.02263202706070255</v>
+        <v>0.02300107151916011</v>
       </c>
       <c r="D4">
-        <v>0.01813958512709789</v>
+        <v>0.01843537451228727</v>
       </c>
       <c r="E4">
-        <v>0.0106370527185302</v>
+        <v>0.01081050361400525</v>
       </c>
       <c r="F4">
-        <v>0.02263202706070255</v>
+        <v>0.02300107151916011</v>
       </c>
       <c r="G4">
-        <v>0.02440570488739656</v>
+        <v>0.02194479730016959</v>
       </c>
       <c r="H4">
-        <v>0.01781616456779949</v>
+        <v>0.0160197020291238</v>
       </c>
       <c r="I4">
-        <v>0.03790673312297763</v>
+        <v>0.03408447240239106</v>
       </c>
       <c r="J4">
-        <v>0.002771533766051759</v>
+        <v>0.002816727206968299</v>
       </c>
       <c r="K4">
-        <v>0.001989961244025163</v>
+        <v>0.002022410134603239</v>
       </c>
       <c r="L4">
-        <v>0.004233960093670558</v>
+        <v>0.00430300028638987</v>
       </c>
       <c r="M4">
-        <v>0.02440570488739656</v>
+        <v>0.02194479730016959</v>
       </c>
       <c r="N4">
-        <v>0.01781616456779949</v>
+        <v>0.0160197020291238</v>
       </c>
       <c r="O4">
-        <v>0.03790673312297763</v>
+        <v>0.03408447240239106</v>
       </c>
       <c r="P4">
-        <v>0.02440570488739656</v>
+        <v>0.02194479730016959</v>
       </c>
       <c r="Q4">
-        <v>0.01781616456779949</v>
+        <v>0.0160197020291238</v>
       </c>
       <c r="R4">
-        <v>0.03790673312297763</v>
+        <v>0.03408447240239106</v>
       </c>
       <c r="S4">
-        <v>0.02440570488739656</v>
+        <v>0.02194479730016959</v>
       </c>
       <c r="T4">
-        <v>0.01781616456779949</v>
+        <v>0.0160197020291238</v>
       </c>
       <c r="U4">
-        <v>0.03790673312297763</v>
+        <v>0.03408447240239106</v>
       </c>
       <c r="V4">
-        <v>0.01549687167618037</v>
+        <v>0.01574956820222211</v>
       </c>
       <c r="W4">
-        <v>0.009670047925936547</v>
+        <v>0.009827730558186596</v>
       </c>
       <c r="X4">
-        <v>0.02057457005518414</v>
+        <v>0.02091006501741828</v>
       </c>
       <c r="Y4">
-        <v>0.01549687167618037</v>
+        <v>0.01574956820222211</v>
       </c>
       <c r="Z4">
-        <v>0.009670047925936547</v>
+        <v>0.009827730558186596</v>
       </c>
       <c r="AA4">
-        <v>0.02057457005518414</v>
+        <v>0.02091006501741828</v>
       </c>
       <c r="AB4">
-        <v>0.01549643668848385</v>
+        <v>0.01574912612148887</v>
       </c>
       <c r="AC4">
-        <v>0.00966977649361392</v>
+        <v>0.009827454699809056</v>
       </c>
       <c r="AD4">
-        <v>0.02057399253960408</v>
+        <v>0.02090947808470011</v>
       </c>
       <c r="AE4">
-        <v>0.01985304617080864</v>
+        <v>0.01785119815303061</v>
       </c>
       <c r="AF4">
-        <v>0.01600155521367176</v>
+        <v>0.01438806571134268</v>
       </c>
       <c r="AG4">
-        <v>0.03404586215674843</v>
+        <v>0.0306129057688142</v>
       </c>
       <c r="AH4">
-        <v>0.01985304617080864</v>
+        <v>0.01785119815303061</v>
       </c>
       <c r="AI4">
-        <v>0.01600155521367176</v>
+        <v>0.01438806571134268</v>
       </c>
       <c r="AJ4">
-        <v>0.03404586215674843</v>
+        <v>0.0306129057688142</v>
       </c>
       <c r="AK4">
-        <v>0.02440570488739656</v>
+        <v>0.02194479730016959</v>
       </c>
       <c r="AL4">
-        <v>0.01781616456779949</v>
+        <v>0.0160197020291238</v>
       </c>
       <c r="AM4">
-        <v>0.03790673312297763</v>
+        <v>0.03408447240239106</v>
       </c>
       <c r="AN4">
-        <v>0.0167771816295991</v>
+        <v>0.01705075526453391</v>
       </c>
       <c r="AO4">
-        <v>0.01015355032223337</v>
+        <v>0.01031911708609592</v>
       </c>
       <c r="AP4">
-        <v>0.02160329855794335</v>
+        <v>0.0219555682682892</v>
       </c>
       <c r="AQ4">
-        <v>0.0167771816295991</v>
+        <v>0.01705075526453391</v>
       </c>
       <c r="AR4">
-        <v>0.01015355032223337</v>
+        <v>0.01031911708609592</v>
       </c>
       <c r="AS4">
-        <v>0.02160329855794335</v>
+        <v>0.0219555682682892</v>
       </c>
       <c r="AT4">
-        <v>0.01985304617080864</v>
+        <v>0.01785119815303061</v>
       </c>
       <c r="AU4">
-        <v>0.01600155521367176</v>
+        <v>0.01438806571134268</v>
       </c>
       <c r="AV4">
-        <v>0.03404586215674843</v>
+        <v>0.0306129057688142</v>
       </c>
       <c r="AW4">
-        <v>0.01985304617080864</v>
+        <v>0.01785119815303061</v>
       </c>
       <c r="AX4">
-        <v>0.01600155521367176</v>
+        <v>0.01438806571134268</v>
       </c>
       <c r="AY4">
-        <v>0.03404586215674843</v>
+        <v>0.0306129057688142</v>
       </c>
     </row>
     <row r="5" spans="1:51">
       <c r="A5">
-        <v>0.01546179273763673</v>
+        <v>0.01953414552244474</v>
       </c>
       <c r="B5">
-        <v>0.009066795261350177</v>
+        <v>0.01145482293436159</v>
       </c>
       <c r="C5">
-        <v>0.01929105374755357</v>
+        <v>0.02437196369013105</v>
       </c>
       <c r="D5">
-        <v>0.01546179273763673</v>
+        <v>0.01953414552244474</v>
       </c>
       <c r="E5">
-        <v>0.009066795261350177</v>
+        <v>0.01145482293436159</v>
       </c>
       <c r="F5">
-        <v>0.01929105374755357</v>
+        <v>0.02437196369013105</v>
       </c>
       <c r="G5">
-        <v>0.02349023500221596</v>
+        <v>0.02374497521172172</v>
       </c>
       <c r="H5">
-        <v>0.01714787155161765</v>
+        <v>0.01733383190455685</v>
       </c>
       <c r="I5">
-        <v>0.03648483308854818</v>
+        <v>0.03688049341395075</v>
       </c>
       <c r="J5">
-        <v>0.002362395851713175</v>
+        <v>0.002984607615173503</v>
       </c>
       <c r="K5">
-        <v>0.00169620022153006</v>
+        <v>0.002142948267694575</v>
       </c>
       <c r="L5">
-        <v>0.003608936641553318</v>
+        <v>0.00455946439935016</v>
       </c>
       <c r="M5">
-        <v>0.02349023500221596</v>
+        <v>0.02374497521172172</v>
       </c>
       <c r="N5">
-        <v>0.01714787155161765</v>
+        <v>0.01733383190455685</v>
       </c>
       <c r="O5">
-        <v>0.03648483308854818</v>
+        <v>0.03688049341395075</v>
       </c>
       <c r="P5">
-        <v>0.02349023500221596</v>
+        <v>0.02374497521172172</v>
       </c>
       <c r="Q5">
-        <v>0.01714787155161765</v>
+        <v>0.01733383190455685</v>
       </c>
       <c r="R5">
-        <v>0.03648483308854818</v>
+        <v>0.03688049341395075</v>
       </c>
       <c r="S5">
-        <v>0.02349023500221596</v>
+        <v>0.02374497521172172</v>
       </c>
       <c r="T5">
-        <v>0.01714787155161765</v>
+        <v>0.01733383190455685</v>
       </c>
       <c r="U5">
-        <v>0.03648483308854818</v>
+        <v>0.03688049341395075</v>
       </c>
       <c r="V5">
-        <v>0.0132092005555801</v>
+        <v>0.0166882618507599</v>
       </c>
       <c r="W5">
-        <v>0.00824254114668198</v>
+        <v>0.01041347539487418</v>
       </c>
       <c r="X5">
-        <v>0.01753732158868506</v>
+        <v>0.02215633062739187</v>
       </c>
       <c r="Y5">
-        <v>0.0132092005555801</v>
+        <v>0.0166882618507599</v>
       </c>
       <c r="Z5">
-        <v>0.00824254114668198</v>
+        <v>0.01041347539487418</v>
       </c>
       <c r="AA5">
-        <v>0.01753732158868506</v>
+        <v>0.02215633062739187</v>
       </c>
       <c r="AB5">
-        <v>0.01320882978141079</v>
+        <v>0.01668779342147088</v>
       </c>
       <c r="AC5">
-        <v>0.008242309783600335</v>
+        <v>0.01041318309499783</v>
       </c>
       <c r="AD5">
-        <v>0.01753682932680922</v>
+        <v>0.02215570871276133</v>
       </c>
       <c r="AE5">
-        <v>0.01910834873296241</v>
+        <v>0.01931556951040822</v>
       </c>
       <c r="AF5">
-        <v>0.01540132907876771</v>
+        <v>0.01556834902538903</v>
       </c>
       <c r="AG5">
-        <v>0.03276878527397384</v>
+        <v>0.03312414686252985</v>
       </c>
       <c r="AH5">
-        <v>0.01910834873296241</v>
+        <v>0.01931556951040822</v>
       </c>
       <c r="AI5">
-        <v>0.01540132907876771</v>
+        <v>0.01556834902538903</v>
       </c>
       <c r="AJ5">
-        <v>0.03276878527397384</v>
+        <v>0.03312414686252985</v>
       </c>
       <c r="AK5">
-        <v>0.02349023500221596</v>
+        <v>0.02374497521172172</v>
       </c>
       <c r="AL5">
-        <v>0.01714787155161765</v>
+        <v>0.01733383190455685</v>
       </c>
       <c r="AM5">
-        <v>0.03648483308854818</v>
+        <v>0.03688049341395075</v>
       </c>
       <c r="AN5">
-        <v>0.01430050925977541</v>
+        <v>0.01806700126341356</v>
       </c>
       <c r="AO5">
-        <v>0.008654668204016079</v>
+        <v>0.01093414916461789</v>
       </c>
       <c r="AP5">
-        <v>0.01841418766811931</v>
+        <v>0.02326414715876146</v>
       </c>
       <c r="AQ5">
-        <v>0.01430050925977541</v>
+        <v>0.01806700126341356</v>
       </c>
       <c r="AR5">
-        <v>0.008654668204016079</v>
+        <v>0.01093414916461789</v>
       </c>
       <c r="AS5">
-        <v>0.01841418766811931</v>
+        <v>0.02326414715876146</v>
       </c>
       <c r="AT5">
-        <v>0.01910834873296241</v>
+        <v>0.01931556951040822</v>
       </c>
       <c r="AU5">
-        <v>0.01540132907876771</v>
+        <v>0.01556834902538903</v>
       </c>
       <c r="AV5">
-        <v>0.03276878527397384</v>
+        <v>0.03312414686252985</v>
       </c>
       <c r="AW5">
-        <v>0.01910834873296241</v>
+        <v>0.01931556951040822</v>
       </c>
       <c r="AX5">
-        <v>0.01540132907876771</v>
+        <v>0.01556834902538903</v>
       </c>
       <c r="AY5">
-        <v>0.03276878527397384</v>
+        <v>0.03312414686252985</v>
       </c>
     </row>
     <row r="6" spans="1:51">
       <c r="A6">
-        <v>0.0200649905390628</v>
+        <v>0.01697010025346673</v>
       </c>
       <c r="B6">
-        <v>0.01176611045210643</v>
+        <v>0.009951266788632892</v>
       </c>
       <c r="C6">
-        <v>0.02503427755767324</v>
+        <v>0.02117290806092104</v>
       </c>
       <c r="D6">
-        <v>0.0200649905390628</v>
+        <v>0.01697010025346673</v>
       </c>
       <c r="E6">
-        <v>0.01176611045210643</v>
+        <v>0.009951266788632892</v>
       </c>
       <c r="F6">
-        <v>0.02503427755767324</v>
+        <v>0.02117290806092104</v>
       </c>
       <c r="G6">
-        <v>0.01897465115387807</v>
+        <v>0.01915551567472249</v>
       </c>
       <c r="H6">
-        <v>0.01385149534233099</v>
+        <v>0.01398352644254742</v>
       </c>
       <c r="I6">
-        <v>0.02947126668581062</v>
+        <v>0.02975218392031365</v>
       </c>
       <c r="J6">
-        <v>0.003065715031786876</v>
+        <v>0.002592849039061308</v>
       </c>
       <c r="K6">
-        <v>0.002201183392822977</v>
+        <v>0.00186166561004602</v>
       </c>
       <c r="L6">
-        <v>0.004683368920899949</v>
+        <v>0.003960990659672381</v>
       </c>
       <c r="M6">
-        <v>0.01897465115387807</v>
+        <v>0.01915551567472249</v>
       </c>
       <c r="N6">
-        <v>0.01385149534233099</v>
+        <v>0.01398352644254742</v>
       </c>
       <c r="O6">
-        <v>0.02947126668581062</v>
+        <v>0.02975218392031365</v>
       </c>
       <c r="P6">
-        <v>0.01897465115387807</v>
+        <v>0.01915551567472249</v>
       </c>
       <c r="Q6">
-        <v>0.01385149534233099</v>
+        <v>0.01398352644254742</v>
       </c>
       <c r="R6">
-        <v>0.02947126668581062</v>
+        <v>0.02975218392031365</v>
       </c>
       <c r="S6">
-        <v>0.01897465115387807</v>
+        <v>0.01915551567472249</v>
       </c>
       <c r="T6">
-        <v>0.01385149534233099</v>
+        <v>0.01398352644254742</v>
       </c>
       <c r="U6">
-        <v>0.02947126668581062</v>
+        <v>0.02975218392031365</v>
       </c>
       <c r="V6">
-        <v>0.01714176930668186</v>
+        <v>0.01449776630045585</v>
       </c>
       <c r="W6">
-        <v>0.01069646404736948</v>
+        <v>0.009046606171484449</v>
       </c>
       <c r="X6">
-        <v>0.02275843414333931</v>
+        <v>0.01924809823720095</v>
       </c>
       <c r="Y6">
-        <v>0.01714176930668186</v>
+        <v>0.01449776630045585</v>
       </c>
       <c r="Z6">
-        <v>0.01069646404736948</v>
+        <v>0.009046606171484449</v>
       </c>
       <c r="AA6">
-        <v>0.02275843414333931</v>
+        <v>0.01924809823720095</v>
       </c>
       <c r="AB6">
-        <v>0.01714128814771631</v>
+        <v>0.0144973593570353</v>
       </c>
       <c r="AC6">
-        <v>0.01069616380417497</v>
+        <v>0.009046352238790025</v>
       </c>
       <c r="AD6">
-        <v>0.02275779532803186</v>
+        <v>0.01924755795487239</v>
       </c>
       <c r="AE6">
-        <v>0.01543510532356983</v>
+        <v>0.0155822312393978</v>
       </c>
       <c r="AF6">
-        <v>0.01244069489079728</v>
+        <v>0.01255927837895463</v>
       </c>
       <c r="AG6">
-        <v>0.02646956359744102</v>
+        <v>0.02672186889139282</v>
       </c>
       <c r="AH6">
-        <v>0.01543510532356983</v>
+        <v>0.0155822312393978</v>
       </c>
       <c r="AI6">
-        <v>0.01244069489079728</v>
+        <v>0.01255927837895463</v>
       </c>
       <c r="AJ6">
-        <v>0.02646956359744102</v>
+        <v>0.02672186889139282</v>
       </c>
       <c r="AK6">
-        <v>0.01897465115387807</v>
+        <v>0.01915551567472249</v>
       </c>
       <c r="AL6">
-        <v>0.01385149534233099</v>
+        <v>0.01398352644254742</v>
       </c>
       <c r="AM6">
-        <v>0.02947126668581062</v>
+        <v>0.02975218392031365</v>
       </c>
       <c r="AN6">
-        <v>0.01855797628839714</v>
+        <v>0.01569553284874202</v>
       </c>
       <c r="AO6">
-        <v>0.01123128724973795</v>
+        <v>0.009498936480058669</v>
       </c>
       <c r="AP6">
-        <v>0.02389635585050628</v>
+        <v>0.020210503149061</v>
       </c>
       <c r="AQ6">
-        <v>0.01855797628839714</v>
+        <v>0.01569553284874202</v>
       </c>
       <c r="AR6">
-        <v>0.01123128724973795</v>
+        <v>0.009498936480058669</v>
       </c>
       <c r="AS6">
-        <v>0.02389635585050628</v>
+        <v>0.020210503149061</v>
       </c>
       <c r="AT6">
-        <v>0.01543510532356983</v>
+        <v>0.0155822312393978</v>
       </c>
       <c r="AU6">
-        <v>0.01244069489079728</v>
+        <v>0.01255927837895463</v>
       </c>
       <c r="AV6">
-        <v>0.02646956359744102</v>
+        <v>0.02672186889139282</v>
       </c>
       <c r="AW6">
-        <v>0.01543510532356983</v>
+        <v>0.0155822312393978</v>
       </c>
       <c r="AX6">
-        <v>0.01244069489079728</v>
+        <v>0.01255927837895463</v>
       </c>
       <c r="AY6">
-        <v>0.02646956359744102</v>
+        <v>0.02672186889139282</v>
       </c>
     </row>
     <row r="7" spans="1:51">
       <c r="A7">
-        <v>0.01741008771037907</v>
+        <v>0.01765538706564372</v>
       </c>
       <c r="B7">
-        <v>0.01020927543336629</v>
+        <v>0.01035311897529348</v>
       </c>
       <c r="C7">
-        <v>0.02172186262418358</v>
+        <v>0.02202791271339038</v>
       </c>
       <c r="D7">
-        <v>0.01741008771037907</v>
+        <v>0.01765538706564372</v>
       </c>
       <c r="E7">
-        <v>0.01020927543336629</v>
+        <v>0.01035311897529348</v>
       </c>
       <c r="F7">
-        <v>0.02172186262418358</v>
+        <v>0.02202791271339038</v>
       </c>
       <c r="G7">
-        <v>0.0200711055068446</v>
+        <v>0.02040475168892487</v>
       </c>
       <c r="H7">
-        <v>0.01465190701999656</v>
+        <v>0.01489546873291515</v>
       </c>
       <c r="I7">
-        <v>0.03117427025531182</v>
+        <v>0.03169248666577692</v>
       </c>
       <c r="J7">
-        <v>0.002660074396473156</v>
+        <v>0.00269755350314198</v>
       </c>
       <c r="K7">
-        <v>0.001909933416667726</v>
+        <v>0.001936843415255942</v>
       </c>
       <c r="L7">
-        <v>0.004063688120569628</v>
+        <v>0.004120943436714769</v>
       </c>
       <c r="M7">
-        <v>0.0200711055068446</v>
+        <v>0.02040475168892487</v>
       </c>
       <c r="N7">
-        <v>0.01465190701999656</v>
+        <v>0.01489546873291515</v>
       </c>
       <c r="O7">
-        <v>0.03117427025531182</v>
+        <v>0.03169248666577692</v>
       </c>
       <c r="P7">
-        <v>0.0200711055068446</v>
+        <v>0.02040475168892487</v>
       </c>
       <c r="Q7">
-        <v>0.01465190701999656</v>
+        <v>0.01489546873291515</v>
       </c>
       <c r="R7">
-        <v>0.03117427025531182</v>
+        <v>0.03169248666577692</v>
       </c>
       <c r="S7">
-        <v>0.0200711055068446</v>
+        <v>0.02040475168892487</v>
       </c>
       <c r="T7">
-        <v>0.01465190701999656</v>
+        <v>0.01489546873291515</v>
       </c>
       <c r="U7">
-        <v>0.03117427025531182</v>
+        <v>0.03169248666577692</v>
       </c>
       <c r="V7">
-        <v>0.01487365302063853</v>
+        <v>0.01508321529034598</v>
       </c>
       <c r="W7">
-        <v>0.009281159484878442</v>
+        <v>0.009411926341175892</v>
       </c>
       <c r="X7">
-        <v>0.01974714784016689</v>
+        <v>0.02002537519399126</v>
       </c>
       <c r="Y7">
-        <v>0.01487365302063853</v>
+        <v>0.01508321529034598</v>
       </c>
       <c r="Z7">
-        <v>0.009281159484878442</v>
+        <v>0.009411926341175892</v>
       </c>
       <c r="AA7">
-        <v>0.01974714784016689</v>
+        <v>0.02002537519399126</v>
       </c>
       <c r="AB7">
-        <v>0.01487323552630796</v>
+        <v>0.01508279191373086</v>
       </c>
       <c r="AC7">
-        <v>0.009280898968416171</v>
+        <v>0.009411662154168055</v>
       </c>
       <c r="AD7">
-        <v>0.01974659354982164</v>
+        <v>0.02002481309397458</v>
       </c>
       <c r="AE7">
-        <v>0.01632702624919201</v>
+        <v>0.01659843381918907</v>
       </c>
       <c r="AF7">
-        <v>0.01315958315684876</v>
+        <v>0.01337833765826639</v>
       </c>
       <c r="AG7">
-        <v>0.02799911309967821</v>
+        <v>0.02846454820907742</v>
       </c>
       <c r="AH7">
-        <v>0.01632702624919201</v>
+        <v>0.01659843381918907</v>
       </c>
       <c r="AI7">
-        <v>0.01315958315684876</v>
+        <v>0.01337833765826639</v>
       </c>
       <c r="AJ7">
-        <v>0.02799911309967821</v>
+        <v>0.02846454820907742</v>
       </c>
       <c r="AK7">
-        <v>0.0200711055068446</v>
+        <v>0.02040475168892487</v>
       </c>
       <c r="AL7">
-        <v>0.01465190701999656</v>
+        <v>0.01489546873291515</v>
       </c>
       <c r="AM7">
-        <v>0.03117427025531182</v>
+        <v>0.03169248666577692</v>
       </c>
       <c r="AN7">
-        <v>0.01610247432108784</v>
+        <v>0.01632935006317694</v>
       </c>
       <c r="AO7">
-        <v>0.009745217459122364</v>
+        <v>0.009882522658234685</v>
       </c>
       <c r="AP7">
-        <v>0.02073450523217524</v>
+        <v>0.02102664395369082</v>
       </c>
       <c r="AQ7">
-        <v>0.01610247432108784</v>
+        <v>0.01632935006317694</v>
       </c>
       <c r="AR7">
-        <v>0.009745217459122364</v>
+        <v>0.009882522658234685</v>
       </c>
       <c r="AS7">
-        <v>0.02073450523217524</v>
+        <v>0.02102664395369082</v>
       </c>
       <c r="AT7">
-        <v>0.01632702624919201</v>
+        <v>0.01659843381918907</v>
       </c>
       <c r="AU7">
-        <v>0.01315958315684876</v>
+        <v>0.01337833765826639</v>
       </c>
       <c r="AV7">
-        <v>0.02799911309967821</v>
+        <v>0.02846454820907742</v>
       </c>
       <c r="AW7">
-        <v>0.01632702624919201</v>
+        <v>0.01659843381918907</v>
       </c>
       <c r="AX7">
-        <v>0.01315958315684876</v>
+        <v>0.01337833765826639</v>
       </c>
       <c r="AY7">
-        <v>0.02799911309967821</v>
+        <v>0.02846454820907742</v>
       </c>
     </row>
     <row r="8" spans="1:51">
       <c r="A8">
-        <v>0.01429456824873684</v>
+        <v>0.01457159641084726</v>
       </c>
       <c r="B8">
-        <v>0.008382334821059285</v>
+        <v>0.008544784135320834</v>
       </c>
       <c r="C8">
-        <v>0.01783475493842401</v>
+        <v>0.01818039177727837</v>
       </c>
       <c r="D8">
-        <v>0.01429456824873684</v>
+        <v>0.01457159641084726</v>
       </c>
       <c r="E8">
-        <v>0.008382334821059285</v>
+        <v>0.008544784135320834</v>
       </c>
       <c r="F8">
-        <v>0.01783475493842401</v>
+        <v>0.01818039177727837</v>
       </c>
       <c r="G8">
-        <v>0.01786861076156478</v>
+        <v>0.01809256628032066</v>
       </c>
       <c r="H8">
-        <v>0.01304408585594229</v>
+        <v>0.01320757338463408</v>
       </c>
       <c r="I8">
-        <v>0.02775337416157934</v>
+        <v>0.02810121996730656</v>
       </c>
       <c r="J8">
-        <v>0.002184056487230361</v>
+        <v>0.002226383414778959</v>
       </c>
       <c r="K8">
-        <v>0.0015681525578314</v>
+        <v>0.001598543291811292</v>
       </c>
       <c r="L8">
-        <v>0.003336494803896594</v>
+        <v>0.003401155940024026</v>
       </c>
       <c r="M8">
-        <v>0.01786861076156478</v>
+        <v>0.01809256628032066</v>
       </c>
       <c r="N8">
-        <v>0.01304408585594229</v>
+        <v>0.01320757338463408</v>
       </c>
       <c r="O8">
-        <v>0.02775337416157934</v>
+        <v>0.02810121996730656</v>
       </c>
       <c r="P8">
-        <v>0.01786861076156478</v>
+        <v>0.01809256628032066</v>
       </c>
       <c r="Q8">
-        <v>0.01304408585594229</v>
+        <v>0.01320757338463408</v>
       </c>
       <c r="R8">
-        <v>0.02775337416157934</v>
+        <v>0.02810121996730656</v>
       </c>
       <c r="S8">
-        <v>0.01786861076156478</v>
+        <v>0.01809256628032066</v>
       </c>
       <c r="T8">
-        <v>0.01304408585594229</v>
+        <v>0.01320757338463408</v>
       </c>
       <c r="U8">
-        <v>0.02775337416157934</v>
+        <v>0.02810121996730656</v>
       </c>
       <c r="V8">
-        <v>0.012212026254457</v>
+        <v>0.01244869483584038</v>
       </c>
       <c r="W8">
-        <v>0.007620304382781169</v>
+        <v>0.007767985577564395</v>
       </c>
       <c r="X8">
-        <v>0.01621341358038546</v>
+        <v>0.01652762888843488</v>
       </c>
       <c r="Y8">
-        <v>0.012212026254457</v>
+        <v>0.01244869483584038</v>
       </c>
       <c r="Z8">
-        <v>0.007620304382781169</v>
+        <v>0.007767985577564395</v>
       </c>
       <c r="AA8">
-        <v>0.01621341358038546</v>
+        <v>0.01652762888843488</v>
       </c>
       <c r="AB8">
-        <v>0.01221168347035959</v>
+        <v>0.01244834540860084</v>
       </c>
       <c r="AC8">
-        <v>0.007620090485504383</v>
+        <v>0.007767767534966922</v>
       </c>
       <c r="AD8">
-        <v>0.01621295847979656</v>
+        <v>0.01652716496801472</v>
       </c>
       <c r="AE8">
-        <v>0.01453538654565759</v>
+        <v>0.01471756523193533</v>
       </c>
       <c r="AF8">
-        <v>0.01171552155580002</v>
+        <v>0.01186235757693987</v>
       </c>
       <c r="AG8">
-        <v>0.02492664160808515</v>
+        <v>0.02523905867434015</v>
       </c>
       <c r="AH8">
-        <v>0.01453538654565759</v>
+        <v>0.01471756523193533</v>
       </c>
       <c r="AI8">
-        <v>0.01171552155580002</v>
+        <v>0.01186235757693987</v>
       </c>
       <c r="AJ8">
-        <v>0.02492664160808515</v>
+        <v>0.02523905867434015</v>
       </c>
       <c r="AK8">
-        <v>0.01786861076156478</v>
+        <v>0.01809256628032066</v>
       </c>
       <c r="AL8">
-        <v>0.01304408585594229</v>
+        <v>0.01320757338463408</v>
       </c>
       <c r="AM8">
-        <v>0.02775337416157934</v>
+        <v>0.02810121996730656</v>
       </c>
       <c r="AN8">
-        <v>0.01322095109372146</v>
+        <v>0.01347717259821979</v>
       </c>
       <c r="AO8">
-        <v>0.008001319601920227</v>
+        <v>0.008156384856442614</v>
       </c>
       <c r="AP8">
-        <v>0.01702408425940474</v>
+        <v>0.01735401033285662</v>
       </c>
       <c r="AQ8">
-        <v>0.01322095109372146</v>
+        <v>0.01347717259821979</v>
       </c>
       <c r="AR8">
-        <v>0.008001319601920227</v>
+        <v>0.008156384856442614</v>
       </c>
       <c r="AS8">
-        <v>0.01702408425940474</v>
+        <v>0.01735401033285662</v>
       </c>
       <c r="AT8">
-        <v>0.01453538654565759</v>
+        <v>0.01471756523193533</v>
       </c>
       <c r="AU8">
-        <v>0.01171552155580002</v>
+        <v>0.01186235757693987</v>
       </c>
       <c r="AV8">
-        <v>0.02492664160808515</v>
+        <v>0.02523905867434015</v>
       </c>
       <c r="AW8">
-        <v>0.01453538654565759</v>
+        <v>0.01471756523193533</v>
       </c>
       <c r="AX8">
-        <v>0.01171552155580002</v>
+        <v>0.01186235757693987</v>
       </c>
       <c r="AY8">
-        <v>0.02492664160808515</v>
+        <v>0.02523905867434015</v>
       </c>
     </row>
     <row r="9" spans="1:51">
       <c r="A9">
-        <v>0.0146407370778082</v>
+        <v>0.01491423981693576</v>
       </c>
       <c r="B9">
-        <v>0.00858532822242673</v>
+        <v>0.008745710228651128</v>
       </c>
       <c r="C9">
-        <v>0.01826665579239729</v>
+        <v>0.01860789410351303</v>
       </c>
       <c r="D9">
-        <v>0.0146407370778082</v>
+        <v>0.01491423981693576</v>
       </c>
       <c r="E9">
-        <v>0.00858532822242673</v>
+        <v>0.008745710228651128</v>
       </c>
       <c r="F9">
-        <v>0.01826665579239729</v>
+        <v>0.01860789410351303</v>
       </c>
       <c r="G9">
-        <v>0.01844896179112502</v>
+        <v>0.01867061263247171</v>
       </c>
       <c r="H9">
-        <v>0.01346774210752127</v>
+        <v>0.01362954722170435</v>
       </c>
       <c r="I9">
-        <v>0.0286547704415346</v>
+        <v>0.02899903664192415</v>
       </c>
       <c r="J9">
-        <v>0.002236947366035116</v>
+        <v>0.002278735646819294</v>
       </c>
       <c r="K9">
-        <v>0.001606128208813214</v>
+        <v>0.001636132194416253</v>
       </c>
       <c r="L9">
-        <v>0.003417294061304709</v>
+        <v>0.003481132328545219</v>
       </c>
       <c r="M9">
-        <v>0.01844896179112502</v>
+        <v>0.01867061263247171</v>
       </c>
       <c r="N9">
-        <v>0.01346774210752127</v>
+        <v>0.01362954722170435</v>
       </c>
       <c r="O9">
-        <v>0.0286547704415346</v>
+        <v>0.02899903664192415</v>
       </c>
       <c r="P9">
-        <v>0.01844896179112502</v>
+        <v>0.01867061263247171</v>
       </c>
       <c r="Q9">
-        <v>0.01346774210752127</v>
+        <v>0.01362954722170435</v>
       </c>
       <c r="R9">
-        <v>0.0286547704415346</v>
+        <v>0.02899903664192415</v>
       </c>
       <c r="S9">
-        <v>0.01844896179112502</v>
+        <v>0.01867061263247171</v>
       </c>
       <c r="T9">
-        <v>0.01346774210752127</v>
+        <v>0.01362954722170435</v>
       </c>
       <c r="U9">
-        <v>0.0286547704415346</v>
+        <v>0.02899903664192415</v>
       </c>
       <c r="V9">
-        <v>0.0125077625618105</v>
+        <v>0.01274141933078544</v>
       </c>
       <c r="W9">
-        <v>0.007804843838569755</v>
+        <v>0.007950645662410117</v>
       </c>
       <c r="X9">
-        <v>0.01660605072036118</v>
+        <v>0.01691626736683003</v>
       </c>
       <c r="Y9">
-        <v>0.0125077625618105</v>
+        <v>0.01274141933078544</v>
       </c>
       <c r="Z9">
-        <v>0.007804843838569755</v>
+        <v>0.007950645662410117</v>
       </c>
       <c r="AA9">
-        <v>0.01660605072036118</v>
+        <v>0.01691626736683003</v>
       </c>
       <c r="AB9">
-        <v>0.01250741147657607</v>
+        <v>0.01274106168694862</v>
       </c>
       <c r="AC9">
-        <v>0.00780462476138347</v>
+        <v>0.007950422492655937</v>
       </c>
       <c r="AD9">
-        <v>0.01660558459868823</v>
+        <v>0.01691579253756582</v>
       </c>
       <c r="AE9">
-        <v>0.01500747845360678</v>
+        <v>0.01518778237874876</v>
       </c>
       <c r="AF9">
-        <v>0.01209602763360706</v>
+        <v>0.0122413525972715</v>
       </c>
       <c r="AG9">
-        <v>0.0257362290076746</v>
+        <v>0.02604543105802447</v>
       </c>
       <c r="AH9">
-        <v>0.01500747845360678</v>
+        <v>0.01518778237874876</v>
       </c>
       <c r="AI9">
-        <v>0.01209602763360706</v>
+        <v>0.0122413525972715</v>
       </c>
       <c r="AJ9">
-        <v>0.0257362290076746</v>
+        <v>0.02604543105802447</v>
       </c>
       <c r="AK9">
-        <v>0.01844896179112502</v>
+        <v>0.01867061263247171</v>
       </c>
       <c r="AL9">
-        <v>0.01346774210752127</v>
+        <v>0.01362954722170435</v>
       </c>
       <c r="AM9">
-        <v>0.0286547704415346</v>
+        <v>0.02899903664192415</v>
       </c>
       <c r="AN9">
-        <v>0.01354112034120661</v>
+        <v>0.01379408120543725</v>
       </c>
       <c r="AO9">
-        <v>0.008195086030498242</v>
+        <v>0.008348177945530623</v>
       </c>
       <c r="AP9">
-        <v>0.01743635325637924</v>
+        <v>0.01776208073517153</v>
       </c>
       <c r="AQ9">
-        <v>0.01354112034120661</v>
+        <v>0.01379408120543725</v>
       </c>
       <c r="AR9">
-        <v>0.008195086030498242</v>
+        <v>0.008348177945530623</v>
       </c>
       <c r="AS9">
-        <v>0.01743635325637924</v>
+        <v>0.01776208073517153</v>
       </c>
       <c r="AT9">
-        <v>0.01500747845360678</v>
+        <v>0.01518778237874876</v>
       </c>
       <c r="AU9">
-        <v>0.01209602763360706</v>
+        <v>0.0122413525972715</v>
       </c>
       <c r="AV9">
-        <v>0.0257362290076746</v>
+        <v>0.02604543105802447</v>
       </c>
       <c r="AW9">
-        <v>0.01500747845360678</v>
+        <v>0.01518778237874876</v>
       </c>
       <c r="AX9">
-        <v>0.01209602763360706</v>
+        <v>0.0122413525972715</v>
       </c>
       <c r="AY9">
-        <v>0.0257362290076746</v>
+        <v>0.02604543105802447</v>
       </c>
     </row>
     <row r="10" spans="1:51">
       <c r="A10">
-        <v>0.1354320786390941</v>
+        <v>0.1312819359299788</v>
       </c>
       <c r="B10">
-        <v>0.07941737091396478</v>
+        <v>0.07698372722933958</v>
       </c>
       <c r="C10">
-        <v>0.1689731296041803</v>
+        <v>0.1637951643177437</v>
       </c>
       <c r="D10">
-        <v>0.1354320786390941</v>
+        <v>0.1312819359299788</v>
       </c>
       <c r="E10">
-        <v>0.07941737091396478</v>
+        <v>0.07698372722933958</v>
       </c>
       <c r="F10">
-        <v>0.1689731296041803</v>
+        <v>0.1637951643177437</v>
       </c>
       <c r="G10">
-        <v>0.06244974959713444</v>
+        <v>0.05931741052837072</v>
       </c>
       <c r="H10">
-        <v>0.04558831720590814</v>
+        <v>0.04330170968571063</v>
       </c>
       <c r="I10">
-        <v>0.09699641958703858</v>
+        <v>0.09213129720363962</v>
       </c>
       <c r="J10">
-        <v>0.02069256690959826</v>
+        <v>0.02005846968126287</v>
       </c>
       <c r="K10">
-        <v>0.01485726304109155</v>
+        <v>0.01440198123114674</v>
       </c>
       <c r="L10">
-        <v>0.03161119795976924</v>
+        <v>0.03064251325775902</v>
       </c>
       <c r="M10">
-        <v>0.06244974959713444</v>
+        <v>0.05931741052837072</v>
       </c>
       <c r="N10">
-        <v>0.04558831720590814</v>
+        <v>0.04330170968571063</v>
       </c>
       <c r="O10">
-        <v>0.09699641958703858</v>
+        <v>0.09213129720363962</v>
       </c>
       <c r="P10">
-        <v>0.06244974959713444</v>
+        <v>0.05931741052837072</v>
       </c>
       <c r="Q10">
-        <v>0.04558831720590814</v>
+        <v>0.04330170968571063</v>
       </c>
       <c r="R10">
-        <v>0.09699641958703858</v>
+        <v>0.09213129720363962</v>
       </c>
       <c r="S10">
-        <v>0.06244974959713444</v>
+        <v>0.05931741052837072</v>
       </c>
       <c r="T10">
-        <v>0.04558831720590814</v>
+        <v>0.04330170968571063</v>
       </c>
       <c r="U10">
-        <v>0.09699641958703858</v>
+        <v>0.09213129720363962</v>
       </c>
       <c r="V10">
-        <v>0.1157012979515804</v>
+        <v>0.1121557797630239</v>
       </c>
       <c r="W10">
-        <v>0.07219760992178617</v>
+        <v>0.0699852065721269</v>
       </c>
       <c r="X10">
-        <v>0.1536119360038003</v>
+        <v>0.1489046948343125</v>
       </c>
       <c r="Y10">
-        <v>0.1157012979515804</v>
+        <v>0.1121557797630239</v>
       </c>
       <c r="Z10">
-        <v>0.07219760992178617</v>
+        <v>0.0699852065721269</v>
       </c>
       <c r="AA10">
-        <v>0.1536119360038003</v>
+        <v>0.1489046948343125</v>
       </c>
       <c r="AB10">
-        <v>0.1156980502870109</v>
+        <v>0.1121526316189784</v>
       </c>
       <c r="AC10">
-        <v>0.07219558337909482</v>
+        <v>0.06998324213024253</v>
       </c>
       <c r="AD10">
-        <v>0.15360762421084</v>
+        <v>0.1489005151707287</v>
       </c>
       <c r="AE10">
-        <v>0.05080032590034337</v>
+        <v>0.04825229573929248</v>
       </c>
       <c r="AF10">
-        <v>0.04094506267567676</v>
+        <v>0.03889135036586974</v>
       </c>
       <c r="AG10">
-        <v>0.08711715462909948</v>
+        <v>0.08274755396993559</v>
       </c>
       <c r="AH10">
-        <v>0.05080032590034337</v>
+        <v>0.04825229573929248</v>
       </c>
       <c r="AI10">
-        <v>0.04094506267567676</v>
+        <v>0.03889135036586974</v>
       </c>
       <c r="AJ10">
-        <v>0.08711715462909948</v>
+        <v>0.08274755396993559</v>
       </c>
       <c r="AK10">
-        <v>0.06244974959713444</v>
+        <v>0.05931741052837072</v>
       </c>
       <c r="AL10">
-        <v>0.04558831720590814</v>
+        <v>0.04330170968571063</v>
       </c>
       <c r="AM10">
-        <v>0.09699641958703858</v>
+        <v>0.09213129720363962</v>
       </c>
       <c r="AN10">
-        <v>0.1252602287142688</v>
+        <v>0.1214217893270542</v>
       </c>
       <c r="AO10">
-        <v>0.07580749041787546</v>
+        <v>0.07348446690073324</v>
       </c>
       <c r="AP10">
-        <v>0.1612925328039903</v>
+        <v>0.1563499295760281</v>
       </c>
       <c r="AQ10">
-        <v>0.1252602287142688</v>
+        <v>0.1214217893270542</v>
       </c>
       <c r="AR10">
-        <v>0.07580749041787546</v>
+        <v>0.07348446690073324</v>
       </c>
       <c r="AS10">
-        <v>0.1612925328039903</v>
+        <v>0.1563499295760281</v>
       </c>
       <c r="AT10">
-        <v>0.05080032590034337</v>
+        <v>0.04825229573929248</v>
       </c>
       <c r="AU10">
-        <v>0.04094506267567676</v>
+        <v>0.03889135036586974</v>
       </c>
       <c r="AV10">
-        <v>0.08711715462909948</v>
+        <v>0.08274755396993559</v>
       </c>
       <c r="AW10">
-        <v>0.05080032590034337</v>
+        <v>0.04825229573929248</v>
       </c>
       <c r="AX10">
-        <v>0.04094506267567676</v>
+        <v>0.03889135036586974</v>
       </c>
       <c r="AY10">
-        <v>0.08711715462909948</v>
+        <v>0.08274755396993559</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improve fodder stubble calibration - no profit change (fodder still not selected)
</commit_message>
<xml_diff>
--- a/stubble sim.xlsx
+++ b/stubble sim.xlsx
@@ -351,7 +351,7 @@
         <v>0.05988132675614952</v>
       </c>
       <c r="B1">
-        <v>0.03511441000980608</v>
+        <v>0.2767500477278779</v>
       </c>
       <c r="C1">
         <v>0.07471151065916186</v>
@@ -360,7 +360,7 @@
         <v>0.05988132675614952</v>
       </c>
       <c r="E1">
-        <v>0.03511441000980608</v>
+        <v>0.2767500477278779</v>
       </c>
       <c r="F1">
         <v>0.07471151065916186</v>
@@ -369,7 +369,7 @@
         <v>0.0521744500435975</v>
       </c>
       <c r="H1">
-        <v>0.03808734853182617</v>
+        <v>0.2574457951240353</v>
       </c>
       <c r="I1">
         <v>0.08103691176984291</v>
@@ -378,7 +378,7 @@
         <v>0.00914922352952397</v>
       </c>
       <c r="K1">
-        <v>0.00656914249419821</v>
+        <v>0.0517739155603892</v>
       </c>
       <c r="L1">
         <v>0.01397689892382598</v>
@@ -387,7 +387,7 @@
         <v>0.0521744500435975</v>
       </c>
       <c r="N1">
-        <v>0.03808734853182617</v>
+        <v>0.2574457951240353</v>
       </c>
       <c r="O1">
         <v>0.08103691176984291</v>
@@ -396,7 +396,7 @@
         <v>0.0521744500435975</v>
       </c>
       <c r="Q1">
-        <v>0.03808734853182617</v>
+        <v>0.2574457951240353</v>
       </c>
       <c r="R1">
         <v>0.08103691176984291</v>
@@ -405,7 +405,7 @@
         <v>0.0521744500435975</v>
       </c>
       <c r="T1">
-        <v>0.03808734853182617</v>
+        <v>0.2574457951240353</v>
       </c>
       <c r="U1">
         <v>0.08103691176984291</v>
@@ -414,7 +414,7 @@
         <v>0.05115735724039348</v>
       </c>
       <c r="W1">
-        <v>0.03192219091800553</v>
+        <v>0.251590952479889</v>
       </c>
       <c r="X1">
         <v>0.06791955514469261</v>
@@ -423,7 +423,7 @@
         <v>0.05115735724039348</v>
       </c>
       <c r="Z1">
-        <v>0.03192219091800553</v>
+        <v>0.251590952479889</v>
       </c>
       <c r="AA1">
         <v>0.06791955514469261</v>
@@ -432,7 +432,7 @@
         <v>0.05115592128470829</v>
       </c>
       <c r="AC1">
-        <v>0.03192129488165797</v>
+        <v>0.2515838904759458</v>
       </c>
       <c r="AD1">
         <v>0.06791764868437865</v>
@@ -441,7 +441,7 @@
         <v>0.04244178852572304</v>
       </c>
       <c r="AF1">
-        <v>0.03420808155173277</v>
+        <v>0.2312244641391799</v>
       </c>
       <c r="AG1">
         <v>0.0727831522377293</v>
@@ -450,7 +450,7 @@
         <v>0.04244178852572304</v>
       </c>
       <c r="AI1">
-        <v>0.03420808155173277</v>
+        <v>0.2312244641391799</v>
       </c>
       <c r="AJ1">
         <v>0.0727831522377293</v>
@@ -459,7 +459,7 @@
         <v>0.0521744500435975</v>
       </c>
       <c r="AL1">
-        <v>0.03808734853182617</v>
+        <v>0.2574457951240353</v>
       </c>
       <c r="AM1">
         <v>0.08103691176984291</v>
@@ -468,7 +468,7 @@
         <v>0.05538384081940814</v>
       </c>
       <c r="AO1">
-        <v>0.0335183004639058</v>
+        <v>0.2641705001038834</v>
       </c>
       <c r="AP1">
         <v>0.07131553290192723</v>
@@ -477,7 +477,7 @@
         <v>0.05538384081940814</v>
       </c>
       <c r="AR1">
-        <v>0.0335183004639058</v>
+        <v>0.2641705001038834</v>
       </c>
       <c r="AS1">
         <v>0.07131553290192723</v>
@@ -486,7 +486,7 @@
         <v>0.04244178852572304</v>
       </c>
       <c r="AU1">
-        <v>0.03420808155173277</v>
+        <v>0.2312244641391799</v>
       </c>
       <c r="AV1">
         <v>0.0727831522377293</v>
@@ -495,7 +495,7 @@
         <v>0.04244178852572304</v>
       </c>
       <c r="AX1">
-        <v>0.03420808155173277</v>
+        <v>0.2312244641391799</v>
       </c>
       <c r="AY1">
         <v>0.0727831522377293</v>
@@ -506,7 +506,7 @@
         <v>0.0126434043002024</v>
       </c>
       <c r="B2">
-        <v>0.00741409228163869</v>
+        <v>0.0251590952479889</v>
       </c>
       <c r="C2">
         <v>0.01577466442901848</v>
@@ -515,7 +515,7 @@
         <v>0.0126434043002024</v>
       </c>
       <c r="E2">
-        <v>0.00741409228163869</v>
+        <v>0.0251590952479889</v>
       </c>
       <c r="F2">
         <v>0.01577466442901848</v>
@@ -524,7 +524,7 @@
         <v>0.01893955208721895</v>
       </c>
       <c r="H2">
-        <v>0.01382587302366983</v>
+        <v>0.02340416319309412</v>
       </c>
       <c r="I2">
         <v>0.02941675111419113</v>
@@ -533,7 +533,7 @@
         <v>0.001931776371418104</v>
       </c>
       <c r="K2">
-        <v>0.001387015434678199</v>
+        <v>0.004706719596399019</v>
       </c>
       <c r="L2">
         <v>0.002951096669528083</v>
@@ -542,7 +542,7 @@
         <v>0.01893955208721895</v>
       </c>
       <c r="N2">
-        <v>0.01382587302366983</v>
+        <v>0.02340416319309412</v>
       </c>
       <c r="O2">
         <v>0.02941675111419113</v>
@@ -551,7 +551,7 @@
         <v>0.01893955208721895</v>
       </c>
       <c r="Q2">
-        <v>0.01382587302366983</v>
+        <v>0.02340416319309412</v>
       </c>
       <c r="R2">
         <v>0.02941675111419113</v>
@@ -560,7 +560,7 @@
         <v>0.01893955208721895</v>
       </c>
       <c r="T2">
-        <v>0.01382587302366983</v>
+        <v>0.02340416319309412</v>
       </c>
       <c r="U2">
         <v>0.02941675111419113</v>
@@ -569,7 +569,7 @@
         <v>0.01080141649422886</v>
       </c>
       <c r="W2">
-        <v>0.006740083892398809</v>
+        <v>0.022871904770899</v>
       </c>
       <c r="X2">
         <v>0.01434060402638044</v>
@@ -578,7 +578,7 @@
         <v>0.01080141649422886</v>
       </c>
       <c r="Z2">
-        <v>0.006740083892398809</v>
+        <v>0.022871904770899</v>
       </c>
       <c r="AA2">
         <v>0.01434060402638044</v>
@@ -587,7 +587,7 @@
         <v>0.01080111330508345</v>
       </c>
       <c r="AC2">
-        <v>0.006739894702372076</v>
+        <v>0.02287126277054053</v>
       </c>
       <c r="AD2">
         <v>0.01434020149440867</v>
@@ -596,7 +596,7 @@
         <v>0.01540655366344975</v>
       </c>
       <c r="AF2">
-        <v>0.0124176822527405</v>
+        <v>0.02102040583083454</v>
       </c>
       <c r="AG2">
         <v>0.02642060053774574</v>
@@ -605,7 +605,7 @@
         <v>0.01540655366344975</v>
       </c>
       <c r="AI2">
-        <v>0.0124176822527405</v>
+        <v>0.02102040583083454</v>
       </c>
       <c r="AJ2">
         <v>0.02642060053774574</v>
@@ -614,7 +614,7 @@
         <v>0.01893955208721895</v>
       </c>
       <c r="AL2">
-        <v>0.01382587302366983</v>
+        <v>0.02340416319309412</v>
       </c>
       <c r="AM2">
         <v>0.02941675111419113</v>
@@ -623,7 +623,7 @@
         <v>0.01169380054034823</v>
       </c>
       <c r="AO2">
-        <v>0.007077088087018749</v>
+        <v>0.02401550000944395</v>
       </c>
       <c r="AP2">
         <v>0.01505763422769946</v>
@@ -632,7 +632,7 @@
         <v>0.01169380054034823</v>
       </c>
       <c r="AR2">
-        <v>0.007077088087018749</v>
+        <v>0.02401550000944395</v>
       </c>
       <c r="AS2">
         <v>0.01505763422769946</v>
@@ -641,7 +641,7 @@
         <v>0.01540655366344975</v>
       </c>
       <c r="AU2">
-        <v>0.0124176822527405</v>
+        <v>0.02102040583083454</v>
       </c>
       <c r="AV2">
         <v>0.02642060053774574</v>
@@ -650,7 +650,7 @@
         <v>0.01540655366344975</v>
       </c>
       <c r="AX2">
-        <v>0.0124176822527405</v>
+        <v>0.02102040583083454</v>
       </c>
       <c r="AY2">
         <v>0.02642060053774574</v>
@@ -661,7 +661,7 @@
         <v>0.02064126044938914</v>
       </c>
       <c r="B3">
-        <v>0.01210403512752179</v>
+        <v>0.03432010394244681</v>
       </c>
       <c r="C3">
         <v>0.02575326622876977</v>
@@ -670,7 +670,7 @@
         <v>0.02064126044938914</v>
       </c>
       <c r="E3">
-        <v>0.01210403512752179</v>
+        <v>0.03432010394244681</v>
       </c>
       <c r="F3">
         <v>0.02575326622876977</v>
@@ -679,7 +679,7 @@
         <v>0.02039971166164056</v>
       </c>
       <c r="H3">
-        <v>0.01489178951299761</v>
+        <v>0.03192616052189654</v>
       </c>
       <c r="I3">
         <v>0.03168465853829278</v>
@@ -688,7 +688,7 @@
         <v>0.003153762884239861</v>
       </c>
       <c r="K3">
-        <v>0.00226440175088422</v>
+        <v>0.006420545102442743</v>
       </c>
       <c r="L3">
         <v>0.004817876065711105</v>
@@ -697,7 +697,7 @@
         <v>0.02039971166164056</v>
       </c>
       <c r="N3">
-        <v>0.01489178951299761</v>
+        <v>0.03192616052189654</v>
       </c>
       <c r="O3">
         <v>0.03168465853829278</v>
@@ -706,7 +706,7 @@
         <v>0.02039971166164056</v>
       </c>
       <c r="Q3">
-        <v>0.01489178951299761</v>
+        <v>0.03192616052189654</v>
       </c>
       <c r="R3">
         <v>0.03168465853829278</v>
@@ -715,7 +715,7 @@
         <v>0.02039971166164056</v>
       </c>
       <c r="T3">
-        <v>0.01489178951299761</v>
+        <v>0.03192616052189654</v>
       </c>
       <c r="U3">
         <v>0.03168465853829278</v>
@@ -724,7 +724,7 @@
         <v>0.01763408381049212</v>
       </c>
       <c r="W3">
-        <v>0.01100366829774709</v>
+        <v>0.03120009449313346</v>
       </c>
       <c r="X3">
         <v>0.02341206020797252</v>
@@ -733,7 +733,7 @@
         <v>0.01763408381049212</v>
       </c>
       <c r="Z3">
-        <v>0.01100366829774709</v>
+        <v>0.03120009449313346</v>
       </c>
       <c r="AA3">
         <v>0.02341206020797252</v>
@@ -742,7 +742,7 @@
         <v>0.01763358883255998</v>
       </c>
       <c r="AC3">
-        <v>0.01100335943151743</v>
+        <v>0.03119921872559029</v>
       </c>
       <c r="AD3">
         <v>0.02341140304578176</v>
@@ -751,7 +751,7 @@
         <v>0.01659433396242037</v>
       </c>
       <c r="AF3">
-        <v>0.01337503317371082</v>
+        <v>0.0286744219502219</v>
       </c>
       <c r="AG3">
         <v>0.02845751739087408</v>
@@ -760,7 +760,7 @@
         <v>0.01659433396242037</v>
       </c>
       <c r="AI3">
-        <v>0.01337503317371082</v>
+        <v>0.0286744219502219</v>
       </c>
       <c r="AJ3">
         <v>0.02845751739087408</v>
@@ -769,7 +769,7 @@
         <v>0.02039971166164056</v>
       </c>
       <c r="AL3">
-        <v>0.01489178951299761</v>
+        <v>0.03192616052189654</v>
       </c>
       <c r="AM3">
         <v>0.03168465853829278</v>
@@ -778,7 +778,7 @@
         <v>0.01909096449543033</v>
       </c>
       <c r="AO3">
-        <v>0.01155385171263444</v>
+        <v>0.03276009921779013</v>
       </c>
       <c r="AP3">
         <v>0.02458266321837114</v>
@@ -787,7 +787,7 @@
         <v>0.01909096449543033</v>
       </c>
       <c r="AR3">
-        <v>0.01155385171263444</v>
+        <v>0.03276009921779013</v>
       </c>
       <c r="AS3">
         <v>0.02458266321837114</v>
@@ -796,7 +796,7 @@
         <v>0.01659433396242037</v>
       </c>
       <c r="AU3">
-        <v>0.01337503317371082</v>
+        <v>0.0286744219502219</v>
       </c>
       <c r="AV3">
         <v>0.02845751739087408</v>
@@ -805,7 +805,7 @@
         <v>0.01659433396242037</v>
       </c>
       <c r="AX3">
-        <v>0.01337503317371082</v>
+        <v>0.0286744219502219</v>
       </c>
       <c r="AY3">
         <v>0.02845751739087408</v>
@@ -816,7 +816,7 @@
         <v>0.01843537451228727</v>
       </c>
       <c r="B4">
-        <v>0.01081050361400525</v>
+        <v>0.03515292291467025</v>
       </c>
       <c r="C4">
         <v>0.02300107151916011</v>
@@ -825,7 +825,7 @@
         <v>0.01843537451228727</v>
       </c>
       <c r="E4">
-        <v>0.01081050361400525</v>
+        <v>0.03515292291467025</v>
       </c>
       <c r="F4">
         <v>0.02300107151916011</v>
@@ -834,7 +834,7 @@
         <v>0.02194479730016959</v>
       </c>
       <c r="H4">
-        <v>0.0160197020291238</v>
+        <v>0.03270088755178767</v>
       </c>
       <c r="I4">
         <v>0.03408447240239106</v>
@@ -843,7 +843,7 @@
         <v>0.002816727206968299</v>
       </c>
       <c r="K4">
-        <v>0.002022410134603239</v>
+        <v>0.00657634742117399</v>
       </c>
       <c r="L4">
         <v>0.00430300028638987</v>
@@ -852,7 +852,7 @@
         <v>0.02194479730016959</v>
       </c>
       <c r="N4">
-        <v>0.0160197020291238</v>
+        <v>0.03270088755178767</v>
       </c>
       <c r="O4">
         <v>0.03408447240239106</v>
@@ -861,7 +861,7 @@
         <v>0.02194479730016959</v>
       </c>
       <c r="Q4">
-        <v>0.0160197020291238</v>
+        <v>0.03270088755178767</v>
       </c>
       <c r="R4">
         <v>0.03408447240239106</v>
@@ -870,7 +870,7 @@
         <v>0.02194479730016959</v>
       </c>
       <c r="T4">
-        <v>0.0160197020291238</v>
+        <v>0.03270088755178767</v>
       </c>
       <c r="U4">
         <v>0.03408447240239106</v>
@@ -879,7 +879,7 @@
         <v>0.01574956820222211</v>
       </c>
       <c r="W4">
-        <v>0.009827730558186596</v>
+        <v>0.03195720264970024</v>
       </c>
       <c r="X4">
         <v>0.02091006501741828</v>
@@ -888,7 +888,7 @@
         <v>0.01574956820222211</v>
       </c>
       <c r="Z4">
-        <v>0.009827730558186596</v>
+        <v>0.03195720264970024</v>
       </c>
       <c r="AA4">
         <v>0.02091006501741828</v>
@@ -897,7 +897,7 @@
         <v>0.01574912612148887</v>
       </c>
       <c r="AC4">
-        <v>0.009827454699809056</v>
+        <v>0.03195630563059481</v>
       </c>
       <c r="AD4">
         <v>0.02090947808470011</v>
@@ -906,7 +906,7 @@
         <v>0.01785119815303061</v>
       </c>
       <c r="AF4">
-        <v>0.01438806571134268</v>
+        <v>0.02937024159743893</v>
       </c>
       <c r="AG4">
         <v>0.0306129057688142</v>
@@ -915,7 +915,7 @@
         <v>0.01785119815303061</v>
       </c>
       <c r="AI4">
-        <v>0.01438806571134268</v>
+        <v>0.02937024159743893</v>
       </c>
       <c r="AJ4">
         <v>0.0306129057688142</v>
@@ -924,7 +924,7 @@
         <v>0.02194479730016959</v>
       </c>
       <c r="AL4">
-        <v>0.0160197020291238</v>
+        <v>0.03270088755178767</v>
       </c>
       <c r="AM4">
         <v>0.03408447240239106</v>
@@ -933,7 +933,7 @@
         <v>0.01705075526453391</v>
       </c>
       <c r="AO4">
-        <v>0.01031911708609592</v>
+        <v>0.03355506278218524</v>
       </c>
       <c r="AP4">
         <v>0.0219555682682892</v>
@@ -942,7 +942,7 @@
         <v>0.01705075526453391</v>
       </c>
       <c r="AR4">
-        <v>0.01031911708609592</v>
+        <v>0.03355506278218524</v>
       </c>
       <c r="AS4">
         <v>0.0219555682682892</v>
@@ -951,7 +951,7 @@
         <v>0.01785119815303061</v>
       </c>
       <c r="AU4">
-        <v>0.01438806571134268</v>
+        <v>0.02937024159743893</v>
       </c>
       <c r="AV4">
         <v>0.0306129057688142</v>
@@ -960,7 +960,7 @@
         <v>0.01785119815303061</v>
       </c>
       <c r="AX4">
-        <v>0.01438806571134268</v>
+        <v>0.02937024159743893</v>
       </c>
       <c r="AY4">
         <v>0.0306129057688142</v>
@@ -971,7 +971,7 @@
         <v>0.01953414552244474</v>
       </c>
       <c r="B5">
-        <v>0.01145482293436159</v>
+        <v>0.03598574188689369</v>
       </c>
       <c r="C5">
         <v>0.02437196369013105</v>
@@ -980,7 +980,7 @@
         <v>0.01953414552244474</v>
       </c>
       <c r="E5">
-        <v>0.01145482293436159</v>
+        <v>0.03598574188689369</v>
       </c>
       <c r="F5">
         <v>0.02437196369013105</v>
@@ -989,7 +989,7 @@
         <v>0.02374497521172172</v>
       </c>
       <c r="H5">
-        <v>0.01733383190455685</v>
+        <v>0.0334756145816788</v>
       </c>
       <c r="I5">
         <v>0.03688049341395075</v>
@@ -998,7 +998,7 @@
         <v>0.002984607615173503</v>
       </c>
       <c r="K5">
-        <v>0.002142948267694575</v>
+        <v>0.006732149739905238</v>
       </c>
       <c r="L5">
         <v>0.00455946439935016</v>
@@ -1007,7 +1007,7 @@
         <v>0.02374497521172172</v>
       </c>
       <c r="N5">
-        <v>0.01733383190455685</v>
+        <v>0.0334756145816788</v>
       </c>
       <c r="O5">
         <v>0.03688049341395075</v>
@@ -1016,7 +1016,7 @@
         <v>0.02374497521172172</v>
       </c>
       <c r="Q5">
-        <v>0.01733383190455685</v>
+        <v>0.0334756145816788</v>
       </c>
       <c r="R5">
         <v>0.03688049341395075</v>
@@ -1025,7 +1025,7 @@
         <v>0.02374497521172172</v>
       </c>
       <c r="T5">
-        <v>0.01733383190455685</v>
+        <v>0.0334756145816788</v>
       </c>
       <c r="U5">
         <v>0.03688049341395075</v>
@@ -1034,7 +1034,7 @@
         <v>0.0166882618507599</v>
       </c>
       <c r="W5">
-        <v>0.01041347539487418</v>
+        <v>0.032714310806267</v>
       </c>
       <c r="X5">
         <v>0.02215633062739187</v>
@@ -1043,7 +1043,7 @@
         <v>0.0166882618507599</v>
       </c>
       <c r="Z5">
-        <v>0.01041347539487418</v>
+        <v>0.032714310806267</v>
       </c>
       <c r="AA5">
         <v>0.02215633062739187</v>
@@ -1052,7 +1052,7 @@
         <v>0.01668779342147088</v>
       </c>
       <c r="AC5">
-        <v>0.01041318309499783</v>
+        <v>0.03271339253559933</v>
       </c>
       <c r="AD5">
         <v>0.02215570871276133</v>
@@ -1061,7 +1061,7 @@
         <v>0.01931556951040822</v>
       </c>
       <c r="AF5">
-        <v>0.01556834902538903</v>
+        <v>0.03006606124465596</v>
       </c>
       <c r="AG5">
         <v>0.03312414686252985</v>
@@ -1070,7 +1070,7 @@
         <v>0.01931556951040822</v>
       </c>
       <c r="AI5">
-        <v>0.01556834902538903</v>
+        <v>0.03006606124465596</v>
       </c>
       <c r="AJ5">
         <v>0.03312414686252985</v>
@@ -1079,7 +1079,7 @@
         <v>0.02374497521172172</v>
       </c>
       <c r="AL5">
-        <v>0.01733383190455685</v>
+        <v>0.0334756145816788</v>
       </c>
       <c r="AM5">
         <v>0.03688049341395075</v>
@@ -1088,7 +1088,7 @@
         <v>0.01806700126341356</v>
       </c>
       <c r="AO5">
-        <v>0.01093414916461789</v>
+        <v>0.03435002634658035</v>
       </c>
       <c r="AP5">
         <v>0.02326414715876146</v>
@@ -1097,7 +1097,7 @@
         <v>0.01806700126341356</v>
       </c>
       <c r="AR5">
-        <v>0.01093414916461789</v>
+        <v>0.03435002634658035</v>
       </c>
       <c r="AS5">
         <v>0.02326414715876146</v>
@@ -1106,7 +1106,7 @@
         <v>0.01931556951040822</v>
       </c>
       <c r="AU5">
-        <v>0.01556834902538903</v>
+        <v>0.03006606124465596</v>
       </c>
       <c r="AV5">
         <v>0.03312414686252985</v>
@@ -1115,7 +1115,7 @@
         <v>0.01931556951040822</v>
       </c>
       <c r="AX5">
-        <v>0.01556834902538903</v>
+        <v>0.03006606124465596</v>
       </c>
       <c r="AY5">
         <v>0.03312414686252985</v>
@@ -1126,7 +1126,7 @@
         <v>0.01697010025346673</v>
       </c>
       <c r="B6">
-        <v>0.009951266788632892</v>
+        <v>0.0370674477993577</v>
       </c>
       <c r="C6">
         <v>0.02117290806092104</v>
@@ -1135,7 +1135,7 @@
         <v>0.01697010025346673</v>
       </c>
       <c r="E6">
-        <v>0.009951266788632892</v>
+        <v>0.0370674477993577</v>
       </c>
       <c r="F6">
         <v>0.02117290806092104</v>
@@ -1144,7 +1144,7 @@
         <v>0.01915551567472249</v>
       </c>
       <c r="H6">
-        <v>0.01398352644254742</v>
+        <v>0.03448186784526808</v>
       </c>
       <c r="I6">
         <v>0.02975218392031365</v>
@@ -1153,7 +1153,7 @@
         <v>0.002592849039061308</v>
       </c>
       <c r="K6">
-        <v>0.00186166561004602</v>
+        <v>0.006934513392713539</v>
       </c>
       <c r="L6">
         <v>0.003960990659672381</v>
@@ -1162,7 +1162,7 @@
         <v>0.01915551567472249</v>
       </c>
       <c r="N6">
-        <v>0.01398352644254742</v>
+        <v>0.03448186784526808</v>
       </c>
       <c r="O6">
         <v>0.02975218392031365</v>
@@ -1171,7 +1171,7 @@
         <v>0.01915551567472249</v>
       </c>
       <c r="Q6">
-        <v>0.01398352644254742</v>
+        <v>0.03448186784526808</v>
       </c>
       <c r="R6">
         <v>0.02975218392031365</v>
@@ -1180,7 +1180,7 @@
         <v>0.01915551567472249</v>
       </c>
       <c r="T6">
-        <v>0.01398352644254742</v>
+        <v>0.03448186784526808</v>
       </c>
       <c r="U6">
         <v>0.02975218392031365</v>
@@ -1189,7 +1189,7 @@
         <v>0.01449776630045585</v>
       </c>
       <c r="W6">
-        <v>0.009046606171484449</v>
+        <v>0.03369767981759791</v>
       </c>
       <c r="X6">
         <v>0.01924809823720095</v>
@@ -1198,7 +1198,7 @@
         <v>0.01449776630045585</v>
       </c>
       <c r="Z6">
-        <v>0.009046606171484449</v>
+        <v>0.03369767981759791</v>
       </c>
       <c r="AA6">
         <v>0.01924809823720095</v>
@@ -1207,7 +1207,7 @@
         <v>0.0144973593570353</v>
       </c>
       <c r="AC6">
-        <v>0.009046352238790025</v>
+        <v>0.03369673394436439</v>
       </c>
       <c r="AD6">
         <v>0.01924755795487239</v>
@@ -1216,7 +1216,7 @@
         <v>0.0155822312393978</v>
       </c>
       <c r="AF6">
-        <v>0.01255927837895463</v>
+        <v>0.0309698257499167</v>
       </c>
       <c r="AG6">
         <v>0.02672186889139282</v>
@@ -1225,7 +1225,7 @@
         <v>0.0155822312393978</v>
       </c>
       <c r="AI6">
-        <v>0.01255927837895463</v>
+        <v>0.0309698257499167</v>
       </c>
       <c r="AJ6">
         <v>0.02672186889139282</v>
@@ -1234,7 +1234,7 @@
         <v>0.01915551567472249</v>
       </c>
       <c r="AL6">
-        <v>0.01398352644254742</v>
+        <v>0.03448186784526808</v>
       </c>
       <c r="AM6">
         <v>0.02975218392031365</v>
@@ -1243,7 +1243,7 @@
         <v>0.01569553284874202</v>
       </c>
       <c r="AO6">
-        <v>0.009498936480058669</v>
+        <v>0.03538256380847781</v>
       </c>
       <c r="AP6">
         <v>0.020210503149061</v>
@@ -1252,7 +1252,7 @@
         <v>0.01569553284874202</v>
       </c>
       <c r="AR6">
-        <v>0.009498936480058669</v>
+        <v>0.03538256380847781</v>
       </c>
       <c r="AS6">
         <v>0.020210503149061</v>
@@ -1261,7 +1261,7 @@
         <v>0.0155822312393978</v>
       </c>
       <c r="AU6">
-        <v>0.01255927837895463</v>
+        <v>0.0309698257499167</v>
       </c>
       <c r="AV6">
         <v>0.02672186889139282</v>
@@ -1270,7 +1270,7 @@
         <v>0.0155822312393978</v>
       </c>
       <c r="AX6">
-        <v>0.01255927837895463</v>
+        <v>0.0309698257499167</v>
       </c>
       <c r="AY6">
         <v>0.02672186889139282</v>
@@ -1281,7 +1281,7 @@
         <v>0.01765538706564372</v>
       </c>
       <c r="B7">
-        <v>0.01035311897529348</v>
+        <v>0.03792289285705757</v>
       </c>
       <c r="C7">
         <v>0.02202791271339038</v>
@@ -1290,7 +1290,7 @@
         <v>0.01765538706564372</v>
       </c>
       <c r="E7">
-        <v>0.01035311897529348</v>
+        <v>0.03792289285705757</v>
       </c>
       <c r="F7">
         <v>0.02202791271339038</v>
@@ -1299,7 +1299,7 @@
         <v>0.02040475168892487</v>
       </c>
       <c r="H7">
-        <v>0.01489546873291515</v>
+        <v>0.03527764271458631</v>
       </c>
       <c r="I7">
         <v>0.03169248666577692</v>
@@ -1308,7 +1308,7 @@
         <v>0.00269755350314198</v>
       </c>
       <c r="K7">
-        <v>0.001936843415255942</v>
+        <v>0.007094548559997247</v>
       </c>
       <c r="L7">
         <v>0.004120943436714769</v>
@@ -1317,7 +1317,7 @@
         <v>0.02040475168892487</v>
       </c>
       <c r="N7">
-        <v>0.01489546873291515</v>
+        <v>0.03527764271458631</v>
       </c>
       <c r="O7">
         <v>0.03169248666577692</v>
@@ -1326,7 +1326,7 @@
         <v>0.02040475168892487</v>
       </c>
       <c r="Q7">
-        <v>0.01489546873291515</v>
+        <v>0.03527764271458631</v>
       </c>
       <c r="R7">
         <v>0.03169248666577692</v>
@@ -1335,7 +1335,7 @@
         <v>0.02040475168892487</v>
       </c>
       <c r="T7">
-        <v>0.01489546873291515</v>
+        <v>0.03527764271458631</v>
       </c>
       <c r="U7">
         <v>0.03169248666577692</v>
@@ -1344,7 +1344,7 @@
         <v>0.01508321529034598</v>
       </c>
       <c r="W7">
-        <v>0.009411926341175892</v>
+        <v>0.03447535714277961</v>
       </c>
       <c r="X7">
         <v>0.02002537519399126</v>
@@ -1353,7 +1353,7 @@
         <v>0.01508321529034598</v>
       </c>
       <c r="Z7">
-        <v>0.009411926341175892</v>
+        <v>0.03447535714277961</v>
       </c>
       <c r="AA7">
         <v>0.02002537519399126</v>
@@ -1362,7 +1362,7 @@
         <v>0.01508279191373086</v>
       </c>
       <c r="AC7">
-        <v>0.009411662154168055</v>
+        <v>0.03447438944061988</v>
       </c>
       <c r="AD7">
         <v>0.02002481309397458</v>
@@ -1371,7 +1371,7 @@
         <v>0.01659843381918907</v>
       </c>
       <c r="AF7">
-        <v>0.01337833765826639</v>
+        <v>0.03168454947513771</v>
       </c>
       <c r="AG7">
         <v>0.02846454820907742</v>
@@ -1380,7 +1380,7 @@
         <v>0.01659843381918907</v>
       </c>
       <c r="AI7">
-        <v>0.01337833765826639</v>
+        <v>0.03168454947513771</v>
       </c>
       <c r="AJ7">
         <v>0.02846454820907742</v>
@@ -1389,7 +1389,7 @@
         <v>0.02040475168892487</v>
       </c>
       <c r="AL7">
-        <v>0.01489546873291515</v>
+        <v>0.03527764271458631</v>
       </c>
       <c r="AM7">
         <v>0.03169248666577692</v>
@@ -1398,7 +1398,7 @@
         <v>0.01632935006317694</v>
       </c>
       <c r="AO7">
-        <v>0.009882522658234685</v>
+        <v>0.03619912499991858</v>
       </c>
       <c r="AP7">
         <v>0.02102664395369082</v>
@@ -1407,7 +1407,7 @@
         <v>0.01632935006317694</v>
       </c>
       <c r="AR7">
-        <v>0.009882522658234685</v>
+        <v>0.03619912499991858</v>
       </c>
       <c r="AS7">
         <v>0.02102664395369082</v>
@@ -1416,7 +1416,7 @@
         <v>0.01659843381918907</v>
       </c>
       <c r="AU7">
-        <v>0.01337833765826639</v>
+        <v>0.03168454947513771</v>
       </c>
       <c r="AV7">
         <v>0.02846454820907742</v>
@@ -1425,7 +1425,7 @@
         <v>0.01659843381918907</v>
       </c>
       <c r="AX7">
-        <v>0.01337833765826639</v>
+        <v>0.03168454947513771</v>
       </c>
       <c r="AY7">
         <v>0.02846454820907742</v>
@@ -1436,7 +1436,7 @@
         <v>0.01457159641084726</v>
       </c>
       <c r="B8">
-        <v>0.008544784135320834</v>
+        <v>0.02936844228005895</v>
       </c>
       <c r="C8">
         <v>0.01818039177727837</v>
@@ -1445,7 +1445,7 @@
         <v>0.01457159641084726</v>
       </c>
       <c r="E8">
-        <v>0.008544784135320834</v>
+        <v>0.02936844228005895</v>
       </c>
       <c r="F8">
         <v>0.01818039177727837</v>
@@ -1454,7 +1454,7 @@
         <v>0.01809256628032066</v>
       </c>
       <c r="H8">
-        <v>0.01320757338463408</v>
+        <v>0.02731989402140397</v>
       </c>
       <c r="I8">
         <v>0.02810121996730656</v>
@@ -1463,7 +1463,7 @@
         <v>0.002226383414778959</v>
       </c>
       <c r="K8">
-        <v>0.001598543291811292</v>
+        <v>0.005494196887160175</v>
       </c>
       <c r="L8">
         <v>0.003401155940024026</v>
@@ -1472,7 +1472,7 @@
         <v>0.01809256628032066</v>
       </c>
       <c r="N8">
-        <v>0.01320757338463408</v>
+        <v>0.02731989402140397</v>
       </c>
       <c r="O8">
         <v>0.02810121996730656</v>
@@ -1481,7 +1481,7 @@
         <v>0.01809256628032066</v>
       </c>
       <c r="Q8">
-        <v>0.01320757338463408</v>
+        <v>0.02731989402140397</v>
       </c>
       <c r="R8">
         <v>0.02810121996730656</v>
@@ -1490,7 +1490,7 @@
         <v>0.01809256628032066</v>
       </c>
       <c r="T8">
-        <v>0.01320757338463408</v>
+        <v>0.02731989402140397</v>
       </c>
       <c r="U8">
         <v>0.02810121996730656</v>
@@ -1499,7 +1499,7 @@
         <v>0.01244869483584038</v>
       </c>
       <c r="W8">
-        <v>0.007767985577564395</v>
+        <v>0.02669858389096269</v>
       </c>
       <c r="X8">
         <v>0.01652762888843488</v>
@@ -1508,7 +1508,7 @@
         <v>0.01244869483584038</v>
       </c>
       <c r="Z8">
-        <v>0.007767985577564395</v>
+        <v>0.02669858389096269</v>
       </c>
       <c r="AA8">
         <v>0.01652762888843488</v>
@@ -1517,7 +1517,7 @@
         <v>0.01244834540860084</v>
       </c>
       <c r="AC8">
-        <v>0.007767767534966922</v>
+        <v>0.02669783447806506</v>
       </c>
       <c r="AD8">
         <v>0.01652716496801472</v>
@@ -1526,7 +1526,7 @@
         <v>0.01471756523193533</v>
       </c>
       <c r="AF8">
-        <v>0.01186235757693987</v>
+        <v>0.02453731222292764</v>
       </c>
       <c r="AG8">
         <v>0.02523905867434015</v>
@@ -1535,7 +1535,7 @@
         <v>0.01471756523193533</v>
       </c>
       <c r="AI8">
-        <v>0.01186235757693987</v>
+        <v>0.02453731222292764</v>
       </c>
       <c r="AJ8">
         <v>0.02523905867434015</v>
@@ -1544,7 +1544,7 @@
         <v>0.01809256628032066</v>
       </c>
       <c r="AL8">
-        <v>0.01320757338463408</v>
+        <v>0.02731989402140397</v>
       </c>
       <c r="AM8">
         <v>0.02810121996730656</v>
@@ -1553,7 +1553,7 @@
         <v>0.01347717259821979</v>
       </c>
       <c r="AO8">
-        <v>0.008156384856442614</v>
+        <v>0.02803351308551082</v>
       </c>
       <c r="AP8">
         <v>0.01735401033285662</v>
@@ -1562,7 +1562,7 @@
         <v>0.01347717259821979</v>
       </c>
       <c r="AR8">
-        <v>0.008156384856442614</v>
+        <v>0.02803351308551082</v>
       </c>
       <c r="AS8">
         <v>0.01735401033285662</v>
@@ -1571,7 +1571,7 @@
         <v>0.01471756523193533</v>
       </c>
       <c r="AU8">
-        <v>0.01186235757693987</v>
+        <v>0.02453731222292764</v>
       </c>
       <c r="AV8">
         <v>0.02523905867434015</v>
@@ -1580,7 +1580,7 @@
         <v>0.01471756523193533</v>
       </c>
       <c r="AX8">
-        <v>0.01186235757693987</v>
+        <v>0.02453731222292764</v>
       </c>
       <c r="AY8">
         <v>0.02523905867434015</v>
@@ -1591,7 +1591,7 @@
         <v>0.01491423981693576</v>
       </c>
       <c r="B9">
-        <v>0.008745710228651128</v>
+        <v>0.03877833791475743</v>
       </c>
       <c r="C9">
         <v>0.01860789410351303</v>
@@ -1600,7 +1600,7 @@
         <v>0.01491423981693576</v>
       </c>
       <c r="E9">
-        <v>0.008745710228651128</v>
+        <v>0.03877833791475743</v>
       </c>
       <c r="F9">
         <v>0.01860789410351303</v>
@@ -1609,7 +1609,7 @@
         <v>0.01867061263247171</v>
       </c>
       <c r="H9">
-        <v>0.01362954722170435</v>
+        <v>0.03607341758390455</v>
       </c>
       <c r="I9">
         <v>0.02899903664192415</v>
@@ -1618,7 +1618,7 @@
         <v>0.002278735646819294</v>
       </c>
       <c r="K9">
-        <v>0.001636132194416253</v>
+        <v>0.007254583727280954</v>
       </c>
       <c r="L9">
         <v>0.003481132328545219</v>
@@ -1627,7 +1627,7 @@
         <v>0.01867061263247171</v>
       </c>
       <c r="N9">
-        <v>0.01362954722170435</v>
+        <v>0.03607341758390455</v>
       </c>
       <c r="O9">
         <v>0.02899903664192415</v>
@@ -1636,7 +1636,7 @@
         <v>0.01867061263247171</v>
       </c>
       <c r="Q9">
-        <v>0.01362954722170435</v>
+        <v>0.03607341758390455</v>
       </c>
       <c r="R9">
         <v>0.02899903664192415</v>
@@ -1645,7 +1645,7 @@
         <v>0.01867061263247171</v>
       </c>
       <c r="T9">
-        <v>0.01362954722170435</v>
+        <v>0.03607341758390455</v>
       </c>
       <c r="U9">
         <v>0.02899903664192415</v>
@@ -1654,7 +1654,7 @@
         <v>0.01274141933078544</v>
       </c>
       <c r="W9">
-        <v>0.007950645662410117</v>
+        <v>0.0352530344679613</v>
       </c>
       <c r="X9">
         <v>0.01691626736683003</v>
@@ -1663,7 +1663,7 @@
         <v>0.01274141933078544</v>
       </c>
       <c r="Z9">
-        <v>0.007950645662410117</v>
+        <v>0.0352530344679613</v>
       </c>
       <c r="AA9">
         <v>0.01691626736683003</v>
@@ -1672,7 +1672,7 @@
         <v>0.01274106168694862</v>
       </c>
       <c r="AC9">
-        <v>0.007950422492655937</v>
+        <v>0.03525204493687535</v>
       </c>
       <c r="AD9">
         <v>0.01691579253756582</v>
@@ -1681,7 +1681,7 @@
         <v>0.01518778237874876</v>
       </c>
       <c r="AF9">
-        <v>0.0122413525972715</v>
+        <v>0.03239927320035871</v>
       </c>
       <c r="AG9">
         <v>0.02604543105802447</v>
@@ -1690,7 +1690,7 @@
         <v>0.01518778237874876</v>
       </c>
       <c r="AI9">
-        <v>0.0122413525972715</v>
+        <v>0.03239927320035871</v>
       </c>
       <c r="AJ9">
         <v>0.02604543105802447</v>
@@ -1699,7 +1699,7 @@
         <v>0.01867061263247171</v>
       </c>
       <c r="AL9">
-        <v>0.01362954722170435</v>
+        <v>0.03607341758390455</v>
       </c>
       <c r="AM9">
         <v>0.02899903664192415</v>
@@ -1708,7 +1708,7 @@
         <v>0.01379408120543725</v>
       </c>
       <c r="AO9">
-        <v>0.008348177945530623</v>
+        <v>0.03701568619135936</v>
       </c>
       <c r="AP9">
         <v>0.01776208073517153</v>
@@ -1717,7 +1717,7 @@
         <v>0.01379408120543725</v>
       </c>
       <c r="AR9">
-        <v>0.008348177945530623</v>
+        <v>0.03701568619135936</v>
       </c>
       <c r="AS9">
         <v>0.01776208073517153</v>
@@ -1726,7 +1726,7 @@
         <v>0.01518778237874876</v>
       </c>
       <c r="AU9">
-        <v>0.0122413525972715</v>
+        <v>0.03239927320035871</v>
       </c>
       <c r="AV9">
         <v>0.02604543105802447</v>
@@ -1735,7 +1735,7 @@
         <v>0.01518778237874876</v>
       </c>
       <c r="AX9">
-        <v>0.0122413525972715</v>
+        <v>0.03239927320035871</v>
       </c>
       <c r="AY9">
         <v>0.02604543105802447</v>
@@ -1746,7 +1746,7 @@
         <v>0.1312819359299788</v>
       </c>
       <c r="B10">
-        <v>0.07698372722933958</v>
+        <v>0.2764956699217879</v>
       </c>
       <c r="C10">
         <v>0.1637951643177437</v>
@@ -1755,7 +1755,7 @@
         <v>0.1312819359299788</v>
       </c>
       <c r="E10">
-        <v>0.07698372722933958</v>
+        <v>0.2764956699217879</v>
       </c>
       <c r="F10">
         <v>0.1637951643177437</v>
@@ -1764,7 +1764,7 @@
         <v>0.05931741052837072</v>
       </c>
       <c r="H10">
-        <v>0.04330170968571063</v>
+        <v>0.2572091610309669</v>
       </c>
       <c r="I10">
         <v>0.09213129720363962</v>
@@ -1773,7 +1773,7 @@
         <v>0.02005846968126287</v>
       </c>
       <c r="K10">
-        <v>0.01440198123114674</v>
+        <v>0.05172632700471933</v>
       </c>
       <c r="L10">
         <v>0.03064251325775902</v>
@@ -1782,7 +1782,7 @@
         <v>0.05931741052837072</v>
       </c>
       <c r="N10">
-        <v>0.04330170968571063</v>
+        <v>0.2572091610309669</v>
       </c>
       <c r="O10">
         <v>0.09213129720363962</v>
@@ -1791,7 +1791,7 @@
         <v>0.05931741052837072</v>
       </c>
       <c r="Q10">
-        <v>0.04330170968571063</v>
+        <v>0.2572091610309669</v>
       </c>
       <c r="R10">
         <v>0.09213129720363962</v>
@@ -1800,7 +1800,7 @@
         <v>0.05931741052837072</v>
       </c>
       <c r="T10">
-        <v>0.04330170968571063</v>
+        <v>0.2572091610309669</v>
       </c>
       <c r="U10">
         <v>0.09213129720363962</v>
@@ -1809,7 +1809,7 @@
         <v>0.1121557797630239</v>
       </c>
       <c r="W10">
-        <v>0.0699852065721269</v>
+        <v>0.2513596999288981</v>
       </c>
       <c r="X10">
         <v>0.1489046948343125</v>
@@ -1818,7 +1818,7 @@
         <v>0.1121557797630239</v>
       </c>
       <c r="Z10">
-        <v>0.0699852065721269</v>
+        <v>0.2513596999288981</v>
       </c>
       <c r="AA10">
         <v>0.1489046948343125</v>
@@ -1827,7 +1827,7 @@
         <v>0.1121526316189784</v>
       </c>
       <c r="AC10">
-        <v>0.06998324213024253</v>
+        <v>0.2513526444160724</v>
       </c>
       <c r="AD10">
         <v>0.1489005151707287</v>
@@ -1836,7 +1836,7 @@
         <v>0.04825229573929248</v>
       </c>
       <c r="AF10">
-        <v>0.03889135036586974</v>
+        <v>0.2310119316667018</v>
       </c>
       <c r="AG10">
         <v>0.08274755396993559</v>
@@ -1845,7 +1845,7 @@
         <v>0.04825229573929248</v>
       </c>
       <c r="AI10">
-        <v>0.03889135036586974</v>
+        <v>0.2310119316667018</v>
       </c>
       <c r="AJ10">
         <v>0.08274755396993559</v>
@@ -1854,7 +1854,7 @@
         <v>0.05931741052837072</v>
       </c>
       <c r="AL10">
-        <v>0.04330170968571063</v>
+        <v>0.2572091610309669</v>
       </c>
       <c r="AM10">
         <v>0.09213129720363962</v>
@@ -1863,7 +1863,7 @@
         <v>0.1214217893270542</v>
       </c>
       <c r="AO10">
-        <v>0.07348446690073324</v>
+        <v>0.263927684925343</v>
       </c>
       <c r="AP10">
         <v>0.1563499295760281</v>
@@ -1872,7 +1872,7 @@
         <v>0.1214217893270542</v>
       </c>
       <c r="AR10">
-        <v>0.07348446690073324</v>
+        <v>0.263927684925343</v>
       </c>
       <c r="AS10">
         <v>0.1563499295760281</v>
@@ -1881,7 +1881,7 @@
         <v>0.04825229573929248</v>
       </c>
       <c r="AU10">
-        <v>0.03889135036586974</v>
+        <v>0.2310119316667018</v>
       </c>
       <c r="AV10">
         <v>0.08274755396993559</v>
@@ -1890,7 +1890,7 @@
         <v>0.04825229573929248</v>
       </c>
       <c r="AX10">
-        <v>0.03889135036586974</v>
+        <v>0.2310119316667018</v>
       </c>
       <c r="AY10">
         <v>0.08274755396993559</v>

</xml_diff>